<commit_message>
this code parse's through the excel spreadsheet and returns users by domain name
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,37 +1,228 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kizan-my.sharepoint.com/personal/julian_heidt_kizan_com/Documents/Documents/Code/Scott's shit/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_5E89CED68312A22637193B11595ED87656CF1448" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48FF9F9A-4A2A-454F-94AC-E08A4E986FC2}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Memberoutput" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Memberoutput" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+  <si>
+    <t>1SMCEMEA.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>smceu.com</t>
+  </si>
+  <si>
+    <t>smc.uk</t>
+  </si>
+  <si>
+    <t>smcitalia.it</t>
+  </si>
+  <si>
+    <t>smc.nu</t>
+  </si>
+  <si>
+    <t>smc.fi</t>
+  </si>
+  <si>
+    <t>smcdk.com</t>
+  </si>
+  <si>
+    <t>smcee.ee</t>
+  </si>
+  <si>
+    <t>marketing.smc.eu</t>
+  </si>
+  <si>
+    <t>smc.ch</t>
+  </si>
+  <si>
+    <t>smcpneumatics.ie</t>
+  </si>
+  <si>
+    <t>smcautomation.ie</t>
+  </si>
+  <si>
+    <t>smceit.com</t>
+  </si>
+  <si>
+    <t>smc-france.fr</t>
+  </si>
+  <si>
+    <t>smc.de</t>
+  </si>
+  <si>
+    <t>smc.ro</t>
+  </si>
+  <si>
+    <t>smc.cz</t>
+  </si>
+  <si>
+    <t>smc.at</t>
+  </si>
+  <si>
+    <t>smc.no</t>
+  </si>
+  <si>
+    <t>smc.pl</t>
+  </si>
+  <si>
+    <t>smc.bg</t>
+  </si>
+  <si>
+    <t>smc.sk</t>
+  </si>
+  <si>
+    <t>smc.si</t>
+  </si>
+  <si>
+    <t>smc.hr</t>
+  </si>
+  <si>
+    <t>smc.hu</t>
+  </si>
+  <si>
+    <t>smc.rs</t>
+  </si>
+  <si>
+    <t>smc.lv</t>
+  </si>
+  <si>
+    <t>1smcemea.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>smc.eu</t>
+  </si>
+  <si>
+    <t>smclt.lt</t>
+  </si>
+  <si>
+    <t>['SharePoint Backups', 'Emi Motegi (SMC-JP)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Michael D. Loggins', 'Luc Wambeke', 'Turgay Ucar', 'Kourychev Alexej', 'Bart Tuijnman', 'Ishiwata Masashi', 'Hugues Maes', 's.t.nauta', 'David Gallego', 'gberakoe', 'SharePoint Backups', 'Jon St. Arnaud', 'Marc D. Doades', 'Chris Cerny', 'Ryan K. Irwin', 'againes', 'SharePoint Backups', 'ftrocoletto', 'Claudio Peres', 'Alfredo Flores SMCMX', 'Sujino Iwao', 'pd-cpleader', 'Alper Guven', 'utku.cakir', 'Kenan Acar', 'Edwin Lenaerts', 'Tsuruta Tetsuya', 'Mark Williams', 'kurotaki.yuya', 'kyoneoka', 'Don Lachance', 'lgalhardo', 'mowen', 'Mariela.Robles', 'aandreassa', 'Gary G. Heinonen', 'Luis Jordan SMC MX', 'Dewayne A. Bruschi', 'pcastillo', 'ErnestoGesualdi', 'rmontser', 'Gustavo OrdoÃ±ana', 'Iker Lorenzo del Amo', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Tsuruta Tetsuya', 'naka.wataru', 'Aoyama Takeshi', 'morino.tatsuya', 'SharePoint Backups', 'SharePoint Backups', 'Asier Mansilla Cabrerizo', 'Mario Sanchez', 'Marina RodrÃ\xadguez', 'Jon Ugartondo Aramendia', 'Alberto GÃ³mez de Segura', 'Beatriz LÃ³pez Coca', 'Naiara Campo', 'Laura GarcÃ\xada Barriuso', 'Amaia MarÃ\xadn', 'Ander Bachiller Carrasco', 'bgutierr', 'Xabier Calvoecheaga Abarrategui', 'Eneko Sanz', 'Jurgi Berakoetxea', 'SharePoint Backups', 'Martin Kendall', 'Andy Shaw', 'SharePoint Backups', 'SharePoint Backups', 'Jurgen Peeters', 'Dennis Duin', 'MarÃ\xada Villaro FernÃ¡ndez', 'Gorka Landa', 'SharePoint Backups', 'Werner Meijers', 'Martin Kendall', 'Steve Tetley', 'Andy Shaw', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'PBO (Boerdijk, P)', 'Mr. Xiaolei Chen', 'carmie valderama', 'Amanda M. Wease', 'Matsumoto Daisuke', 'Akiyama Takeshi', 'Andy P. Thedjoprasetyono', 'gohsoolin', 'Shentley Tay', 'Yeo Xiang Lan', 'Ng Yi Shu', 'edwardchong', 'Tanto - SMC SG', 'Phuc Huynh', 'Eugene Tan', 'Mario Sanchez', 'Gaizka Urtaran Ibarzabal', 'Jon Ugartondo Aramendia', 'Alex Aguilar Miguel', 'Alejandro Molinero', 'Gorka Olano Perez del Palomar', 'jjubete', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Riaan Lof', 'Jeremy Bolt (Admin)', 'HROE (Roekens, H)', 'Luc Wambeke', 'Koyama Masato (SMC Japan GAO)', 'Denise Molloy', 'Kitamura Kentaro', 'Hidenori Ishigaki', 'Yamada Katsuhiro', 'Kanako Ishihara(SMC-JP)', 'Soga Kunihiko', 'Shimizu Toru(SMC-Japan IT)', 'Chris Forster', 'Sam Jones', 'Joao Ribeiro', 'Dale Roberts', 'James Wylie', 'David Walkingshaw', 'Alex Lloyd', 'Ng Heng Tee', 'Paul Harrington', 'Gaizka Urtaran Ibarzabal', 'Gorka Landa', 'Sandra Miguel Izquierdo', 'Oscar Torrecilla Portilla', 'Eda Alonso', 'Aitor LÃ³pez de Suso', 'Ismael Garmendia Urquiola', 'Patxi Andonegi', 'David Palomar', 'Josune SÃ¡nchez Goitia', 'Iker Arroyo', 'Werner Meijers', 'Riaan Lof', 'Peter Findlay', 'SharePoint Backups', 'Keith A Bodycomb', 'Hiroshige Nakano', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Eda Alonso', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Roger Peacock', 'Andy McLean', 'Bradley Reynolds-Price', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'Schuh, Michael', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Ben de Kimpe', 'Ivo Gels', 'Sushkov Alexej', 'Murat Ã–zsezer', 'Roberto MartÃ\xadnez de Lafuente', 'Ander Bachiller Carrasco', 'Ivan MartÃ\xadnez JimÃ©nez', 'Javier Aparicio Hidalgo', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'r.lehner07', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Jennifer.Kavanagh', 'adam.mccarthy', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Nick Tiloi (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'ZA Test Eli Marbach', 'Eli (Kafipause)', 'eleazar.marbach', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'Manuel Vieira', 'Wayne Bell', 'Warren Gates', 'Vic Bester', 'Ernest Snyders', 'Liezl Siebrits', 'Cornelius Kruger', 'Yattish Jugaroop', 'Wade Holland', 'Jbee Steyn', 'Terrance Buddingh', 'Alfie Branchina', 'Coen Pretorius', 'Shaun Collett', 'Shiven Singh', 'Ryan Janse van Rensburg', 'Andrea Banks', 'ZA-Mailbox Mitzie Maliepaard', 'ZA-Mailbox Derick Westerhuis', 'ZA-Mailbox Andile Fongqo', 'Cody Windram', 'Jacobus Smit', 'Armand Erasmus', 'SharePoint Backups', 'Amanda M. Wease', 'ESLO (Sloof, E)', 'JosÃ© Antonio EstÃ©vez', 'Alejandro Molinero', 'jjubete', 'Hielke Weda', 'Mixeev Andrej', 'SharePoint Backups', 'SharePoint Backups', 'Paula Currie (Admin)', 'Jen J. Glisson', 'michael.hadrian', 'SharePoint Backups', 'SharePoint Backups', 'Neumann, Jean Philippe', 'Bachmann, Benjamin', 'SharePoint Backups', 'Michael D. Loggins', 'Natalie C. Robinson', 'Manabe Mitsuhide(SMC Japan IT Dev.)', 'David Cartmel', 'Kitamura Kentaro', 'Robin Rodriguez', 'Chris Cerny', 'Kemas Ohale', 'Ben Kopel', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'HROE (Roekens, H)', 'Bob D. Stephan', 'Brian J. Katzfey', 'Steve J. Oechsle', 'Yutaro Hatagami', 'Jennifer L. Carey', 'Tom D. Smith', 'MarÃ\xada Villaro FernÃ¡ndez', 'Sandra Miguel Izquierdo', 'ipadilla', 'Oscar Torrecilla Portilla', 'Unai Roiz Escudero', 'Eda Alonso', 'Aitor LÃ³pez de Suso', 'Ismael Garmendia Urquiola', 'David Palomar', 'Werner Meijers', 'SharePoint Backups', 'SCHWEDER ANNE (SMC-JP)', 'Ino shunsuke', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Andy P. Thedjoprasetyono', 'Kobayashi Yukihiro', 'Tomobe Nozomi', 'Mario Sanchez', 'Gaizka Urtaran Ibarzabal', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'borja.arberas.smc', 'Borja Arberas Vigo', 'Beatriz LÃ³pez Coca', 'Sandra Miguel Izquierdo', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall (Admin)', 'Asier Mansilla Cabrerizo', 'Marina RodrÃ\xadguez', 'Alberto GÃ³mez de Segura', 'Naiara Campo', 'Ander Bachiller Carrasco', 'Lierni Rabanete', 'Ruben Marquinez', 'bgutierr', 'Eneko Sanz', 'Irakli Liparteliani', 'SharePoint Backups', 'Erdem Karaoglu', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall', 'Chris Santos', 'SharePoint Backups', 'Werner Meijers', 'Wayne Bell', 'Vic Bester', 'Cornelius Kruger', 'Alfie Branchina', 'Shaun Collett', 'ZA-Mailbox Mitzie Maliepaard', 'ZA-Mailbox Derick Westerhuis', 'Jacobus Smit', 'Armand Erasmus', 'SharePoint Backups', 'Werner Meijers', 'Riaan Lof', 'Michael Goulborn', 'Jbee Steyn', 'Brian Abbott', 'Ernst Smith', 'Peter Findlay', 'Theodore Philip', 'Joanne Zimmerman', 'Ingrid Horner', 'Newman Bvekerwa', 'Lerato Mnomiya', 'Nonzuzo Qwane', 'Phelokazi Mpondo', 'Vivian Bvekerwa', 'SharePoint Backups', 'Onder Ay', 'Nikolskiy Vsevolod', 'Bernard Piessevaux', 'Peton Hendriks', 'Jorge Salgado', 'Jone IbaÃ±ez', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'ESLO (Sloof, E)', 'Asier Mansilla Cabrerizo', 'Mario Sanchez', 'Marina RodrÃ\xadguez', 'Gaizka Urtaran Ibarzabal', 'Jon Ugartondo Aramendia', 'Naiara Campo', 'Laura GarcÃ\xada Barriuso', 'Ander Bachiller Carrasco', 'Lierni Rabanete', 'Ruben Marquinez', 'bgutierr', 'Xabier Calvoecheaga Abarrategui', 'Eneko Sanz', 'SharePoint Backups', 'MarÃ\xada Villaro FernÃ¡ndez', 'SharePoint Backups', 'SharePoint Backups', 'jmiradier', 'Gustavo Ozalla', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Unai Roiz Escudero', 'Ivan MartÃ\xadnez JimÃ©nez', 'SharePoint Backups', 'H. Klein Middelink', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Oscar Torrecilla Portilla', 'Aitor LÃ³pez de Suso', 'Ismael Garmendia Urquiola', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'Asier Mansilla Cabrerizo', 'Mario Sanchez', 'Gaizka Urtaran Ibarzabal', 'Maitxu Estrella', 'Beatriz LÃ³pez Coca', 'Joseba Urtaran', 'Ander Bachiller Carrasco', 'SharePoint Backups', 'Mario Sanchez', 'Gaizka Urtaran Ibarzabal', 'JosÃ© Antonio EstÃ©vez', 'Alex Aguilar Miguel', 'Gorka Olano Perez del Palomar', 'SharePoint Backups', 'SharePoint Backups', 'Alejandro Molinero', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'GKON (Konijn, G.H.)', 'Halil Ibrahim Karakelle', 'Lopatina Ekaterina', 'Kevin Janssens', 'Kevin Renette', 'Shakhmaev Vladislav', 'Gustavo Caicedo-SopeÃ±a', 'Eneko Sanz', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'Lou M. Moore', 'Martin Kendall', 'Steve Tetley', 'Kathy Y. Fridenmaker', 'David Cartmel', 'Chris Warner', 'MarÃ\xada Villaro FernÃ¡ndez', 'Werner Meijers', 'SharePoint Backups', 'Marina RodrÃ\xadguez', 'Sandra Miguel Izquierdo', 'Naiara Campo', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Denis Helfer (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'Mario Sanchez', 'Jon Ugartondo Aramendia', 'iibarzab', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall', 'Andy Shaw', 'SharePoint Backups', 'SharePoint Backups', 'borja.arberas.smc', 'Borja Arberas Vigo', 'Uxue Arostegui', 'Maitxu Estrella', 'Alberto GÃ³mez de Segura', 'Beatriz LÃ³pez Coca', 'Laura GarcÃ\xada Barriuso', 'Joseba Urtaran', 'Alex Aguilar Miguel', 'Ander Bachiller Carrasco', 'bgutierr', 'Gorka Olano Perez del Palomar', 'Eneko Sanz', 'usere03', 'Jurgi Berakoetxea', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'Riaan Lof', 'Michael Goulborn', 'Jbee Steyn', 'Peter Findlay', 'Theodore Philip', 'Nonzuzo Qwane', 'Phelokazi Mpondo', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'David Gallego', 'Sonia Pueyo Villaverde', 'SharePoint Backups', 'Werner Meijers', 'Brian Abbott', 'Ernst Smith', 'SharePoint Backups', "Stephen O'Neill (Admin)", 'SharePoint Backups', 'SharePoint Backups', 'Paula Currie (Admin)', 'Fred SMCAutomation1', 'Werner Meijers', 'Mavis SMCAutomation2', 'Liz SMCAutomation3', 'Anne SMCAutomation6', 'Simon SMCAutomation5', 'John SMCAutomation4', 'Martin Kendall', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Sonia Pueyo Villaverde', 'Gustavo Ozalla', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Brandon M. Waggoner', 'Robin Rodriguez', 'Kemas Ohale', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Dennis Bosman', 'JosÃ© Antonio EstÃ©vez', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Josephine Huschmann', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Peter Findlay', 'Michael D. Loggins', 'WDJ (Jong, de W)', 'Luc Wambeke', 'Koyama Masato (SMC Japan GAO)', 'Turgay Ucar', 'Kourychev Alexej', 'Bart Tuijnman', 'Kitamura Kentaro', 'David Gallego', 'gberakoe', 'Aitor LÃ³pez de Suso', 'Peter Findlay', 'SharePoint Backups', 'SharePoint Backups', 'Peter Findlay', 'Werner Meijers', 'HROE (Roekens, H)', 'Eliseev Igor', 'Jurgen Peeters', 'Dennis Duin', 'Luc Wambeke', 'Tyler W. Bradley', 'Jen J. Glisson', 'BGambrel', "Greg O'Neill", 'Mark Hodkinson', 'Muriel Caals', 'Yoichi', 'Haga Makiko', 'okumura.shinji', 'Risa Yokomura', 'Kimura Rie (SMC Japan IBD)', 'Amarendra Rakesh', 'Kim de Jong', 'MarÃ\xada Villaro FernÃ¡ndez', 'Unai Roiz Escudero', 'Patxi Andonegi', 'Werner Meijers', 'Peter Findlay', 'SharePoint Backups', 'Martin Kendall', 'Steve Tetley', 'Werner Meijers', 'SharePoint Backups', 'Jeremy Bolt (Admin)', 'SharePoint Backups', 'Manuel Vieira', 'Jbee Steyn', 'Johan Dorland', 'Dennis Bosman', 'Coen Lieshout', 'Jordy van der Mierden', 'm.vorrink', 'Jbee Steyn', 'Manuel Vieira', 'SharePoint Backups', 'Hirano Ken', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'Joanne Zimmerman', 'Ham Alexander', 'SharePoint Backups', 'Barbara J. Walters', 'John J. Bonca', 'Neil M. Reif', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'Martin Kendall', 'Steve Tetley', 'Michael E. Kobrowski', 'Kathy Y. Fridenmaker', 'Jennifer Ostrander', 'Werner Meijers', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall (Admin)', 'Riaan Lof', 'Michael Goulborn', 'Jbee Steyn', 'Peter Findlay', 'Werner Meijers', 'borja.arberas.smc', 'Borja Arberas Vigo', 'Gaizka Urtaran Ibarzabal', 'Pedro Acon', 'Werner Meijers', 'Jbee Steyn', 'Riaan Lof', 'Peter Findlay', 'Michael Goulborn', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall (Admin)', 'Fred SMCAutomation1', 'Martin Kendall', 'Steve Tetley', 'Jon St. Arnaud', 'Marc D. Doades', 'Chris Santos', 'Ryan K. Irwin', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Tyler Bradley (Admin)', 'Martin Kendall', 'Steve Tetley', 'Michael E. Kobrowski', 'Tyler W. Bradley', 'Jon St. Arnaud', 'Marc D. Doades', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Sandra Miguel Izquierdo', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'Jbee Steyn', 'Peter Findlay', 'Luc Wambeke', 'Turgay Ucar', 'Kourychev Alexej', 'Bart Tuijnman', 'Hugues Maes', 's.t.nauta', 'David Gallego', 'gberakoe', 'Jbee Steyn', 'Peter Findlay', 'SharePoint Backups', 'Jon St. Arnaud', 'Aitor LÃ³pez de Suso', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'WDJ (Jong, de W)', 'David Cartmel', 'Borja Arberas Vigo', 'Gorka Landa', 'Iker Arroyo', 'Lisa Waugh', 'Michael Daniells', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'Tyler W. Bradley', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'Ingrid Horner', 'Brandyn Le Roux', 'SharePoint Backups', 'Werner Meijers', 'Riaan Lof', 'Vincent Mashabane', 'Upeka Ranasinghe', 'SharePoint Backups', 'SharePoint Backups', 'Brian A. Johnson', 'GWBohannan', 'Stephen C. Nimmo', 'Jim W. Carnrike', 'yuyao', 'SharePoint Backups', 'Lou M. Moore', 'David Cartmel', 'Chris Warner', 'Andrew Howard', 'Rich J. Trimble', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'HROE (Roekens, H)', 'Ozgur Yuksel', 'WDJ (Jong, de W)', 'Natalie C. Robinson', 'Kitamura Kentaro', 'Raul Delpeche', 'Parshevnikov Ivan', 'MarÃ\xada Villaro FernÃ¡ndez', 'Werner Meijers', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'ESLO (Sloof, E)', 'Aad Jan Roos', 'Suzanne Lanfermeijer', 'Mario Sanchez', 'Ana Miguelez', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'HROE (Roekens, H)', 'Ozgur Yuksel', 'Johan Dorland', 'testmann', 'Luc Wambeke', 'Shelyapin Alexej', 'Sukhomlin Varvara', 'Kitamura Kentaro', 'Kanako Ishihara(SMC-JP)', 'Soga Kunihiko', 'Oscar Torrecilla Portilla', 'Aitor LÃ³pez de Suso', 'Patxi Andonegi', 'Arkaitz Moraga Amaro', 'Josune SÃ¡nchez Goitia', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Mario Sanchez', 'Gaizka Urtaran Ibarzabal', 'Alex Aguilar Miguel', 'Gorka Olano Perez del Palomar', 'SharePoint Backups', 'Martin Kendall (Admin)', 'Peter Stang (Admin)', 'Jeremy Bolt (Admin)', 'Bob D. Stephan', 'Jon St. Arnaud', 'Marc D. Doades', 'Chris Santos', 'Oscar Torrecilla Portilla', 'Eda Alonso', 'Aitor LÃ³pez de Suso', 'Ismael Garmendia Urquiola', 'David Palomar', 'SharePoint Backups', 'Patxi Andonegi', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'Warren Gates', 'Yattish Jugaroop', 'Terrance Buddingh', 'Shiven Singh', 'Ryan Janse van Rensburg', 'Andrea Banks', 'ZA-Mailbox Andile Fongqo', 'Cody Windram', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'è\x90¥ä¸šæœ¬éƒ¨ è¡Œä¸šå¼€å\x8f‘(ç”„å®ž)', 'è\x90¥ä¸šæœ¬éƒ¨ è¡Œä¸šå¼€å\x8f‘(æœ±è¶…)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Burak Orenel', 'Murat Ã–zsezer', 'UÄŸur Arslan', 'Kees van Kampen', 'Romanchenko Andrey', 'Eviatar Shem Tov', 'Roberto MartÃ\xadnez de Lafuente', 'Ander Bachiller Carrasco', 'Lander GarcÃ\xada Aguilera', 'lvillanu', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall (Admin)', 'Werner Meijers', 'Lou M. Moore', 'HROE (Roekens, H)', 'Brandon M. Waggoner', 'Eliseev Igor', 'Ozgur Yuksel', 'WDJ (Jong, de W)', 'Bob D. Stephan', 'Yutaro Hatagami', 'Kathy Y. Fridenmaker', 'Chandan Agarwal', 'Dmitry Solyanik', 'alexlau', 'Simon McDonald', 'Natalie C. Robinson', 'mdallacqua', 'Faitse', 'pyoungmoop', 'seongjinh', 'Omar IT_MX', 'Manabe Mitsuhide(SMC Japan IT Dev.)', 'l.r.wang', 'David Cartmel', 'Chris Warner', 'Jon St. Arnaud', 'Mark D. Baxter', 'Mona M.  Rich', 'Elizabeth K. Miller', 'Robin Rodriguez', 'IT Dept. [MengFanjia]', 'Leo Tang', 'Shawn Styfco', 'Chris Cerny', 'Winnie Chan', 'Mohammed A. Hassan', 'Jeff Johnfauno', 'Pramote T. [SMCTH]', 'Kemas Ohale', 'IT Dept. [QuanYongNan]', 'Volkan Ã–zsevgi', 'Fred Dijkstra', 'Raul Delpeche', 'Parshevnikov Ivan', 'TEJINDER PAL SINGH', 'MarÃ\xada Villaro FernÃ¡ndez', 'Aitor LÃ³pez de Suso', 'Werner Meijers', 'SharePoint Backups', 'Borja Arberas Vigo', 'Gaizka Urtaran Ibarzabal', 'Uxue Arostegui', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Ajima Yasutaka', 'Aketa Shigeo', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'Werner Meijers', 'SharePoint Backups', 'Martin Kendall (Admin)', 'Werner Meijers', 'Lou M. Moore', 'Michael D. Loggins', 'Martin Kendall', 'Steve Tetley', 'Johan Dorland', 'Andy Shaw', 'David Cartmel', 'Chris Warner', 'Kirk Becnel', 'Chris Santos', 'Hannah S. Morrison', 'MarÃ\xada Villaro FernÃ¡ndez', 'Borja Arberas Vigo', 'Uxue Arostegui', 'Oscar Torrecilla Portilla', 'Eda Alonso', 'Aitor LÃ³pez de Suso', 'Ismael Garmendia Urquiola', 'David Palomar', 'Werner Meijers', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'ESLO (Sloof, E)', 'Mario Sanchez', 'Gaizka Urtaran Ibarzabal', 'Javier Azcona Ochoa', 'SharePoint Backups', 'Nathan P. Eisel', 'Dave M. Phillips', 'GKON (Konijn, G.H.)', 'ftrocoletto', 'Jon A. Jensen', 'Scott M. Maurer', 'Mr. Xiaolei Chen', 'Halil Ibrahim Karakelle', 'Lopatina Ekaterina', 'jaidar', 'Hirata Kouji', 'Yoshitaka Yamada', 'Jos Persoon', 'Burak Orenel', 'Aytun Ersoy', 'Kevin Janssens', 'Kevin Renette', 'Gaizka Urtaran Ibarzabal', 'Gustavo Caicedo-SopeÃ±a', 'JosÃ© Antonio EstÃ©vez', 'Alex Aguilar Miguel', 'Alberto Moran', 'nizquierdo', 'Gorka Olano Perez del Palomar', 'Eneko Sanz', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Ino shunsuke', 'å¤–ç±\x8däººå‘˜ è\x90¥ä¸šæœ¬éƒ¨ä»˜(Sven Barner)', 'Gustavo OrdoÃ±ana', 'jmiradier', 'Iker Lorenzo del Amo', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Aitor LÃ³pez de Suso', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'MarÃ\xada Villaro FernÃ¡ndez', 'Gorka Landa', 'Unai Roiz Escudero', 'Ivan MartÃ\xadnez JimÃ©nez', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'ftrocoletto', 'bjsyholon5', 'liulaxi', 'sunzhibin', 'rturcatel', 'dweber', 'dpavesi', 'Richard Leenders', 'Sjors de Rooij', 'a.molenbroek', 'Bob J. Boggan', 'Jeff S. Vale', 'turban', 'Hiro Narita', 'fuzhonglin', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'ESLO (Sloof, E)', 'Mario Sanchez', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Mario Sanchez', 'SharePoint Backups', 'Asier Mansilla Cabrerizo', 'Borja Arberas Vigo', 'Marina RodrÃ\xadguez', 'Uxue Arostegui', 'Maitxu Estrella', 'Jon Ugartondo Aramendia', 'Alberto GÃ³mez de Segura', 'Beatriz LÃ³pez Coca', 'Sandra Miguel Izquierdo', 'Oscar Maruri', 'Naiara Campo', 'Laura GarcÃ\xada Barriuso', 'Joseba Urtaran', 'Alex Aguilar Miguel', 'Ander Bachiller Carrasco', 'Lierni Rabanete', 'Ruben Marquinez', 'bgutierr', 'ifernandez', 'Xabier Calvoecheaga Abarrategui', 'Gorka Olano Perez del Palomar', 'Eneko Sanz', 'Edurne Labrador', 'Jurgi Berakoetxea', 'SharePoint Backups', 'SharePoint Backups', 'WDJ (Jong, de W)', 'Koyama Masato (SMC Japan GAO)', 'Erkan GÃ¼rbÃ¼z', 'Gorka Landa', 'Ismael Garmendia Urquiola', 'Marta Soloeta', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Dyrkin Andrey', 'Johan Dorland', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Paula Currie (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Jon St. Arnaud', 'Aitor LÃ³pez de Suso', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Paula Currie (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Nonzuzo Qwane', 'Marlene Greeff', 'Jean-Marc Celliers', 'Denicha Rochelle Wie', 'Ryno Lombaard', 'Razeen van Rooyen', 'elainaa', 'Nonzuzo Qwane', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Ishiwata Masashi', 'David Gallego', 'gberakoe', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Paula Currie (Admin)', 'SharePoint Backups', 'Iker Lorenzo del Amo', 'SharePoint Backups', 'SharePoint Backups', 'Werner Meijers', 'Liezl Siebrits', 'Wade Holland', 'Coen Pretorius', 'SharePoint Backups', 'Martin Kendall (Admin)', 'Werner Meijers', 'Martin Kendall', 'Steve Tetley', 'Kathy Y. Fridenmaker', 'Jon St. Arnaud', 'Werner Meijers', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'MarÃ\xada Villaro FernÃ¡ndez', 'Unai Roiz Escudero', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'JosÃ© RamÃ³n BajÃ³n', 'SharePoint Backups', 'Dyrkin Andrey', 'Sukhomlin Varvara', 'Vasiliev Aleksey', 'Smotrakov Dmitry', 'Kozhinov Sergey', 'Oscar Torrecilla Portilla', 'Aitor LÃ³pez de Suso', 'Patxi Andonegi', 'scastro', 'David Palomar', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Jonny Dellhammar', 'SharePoint Backups', 'SharePoint Backups', 'Steven Greenhill (Admin)', 'Martin Kendall', 'Andreas Dietz', 'Sebastian Lenhard', 'Dr. Gerrit Seewald', 'Patrick Charbonnier', 'SharePoint Backups', 'SharePoint Backups', 'Eda Alonso', 'David Palomar', 'SharePoint Backups', 'SharePoint Backups', 'ESLO (Sloof, E)', 'Pedro Acon', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Andrew Hogg', 'Tracey Hayden', 'Craig Woodham', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Ben Groff', 'Martin Kendall', 'Andy Shaw', 'David Cartmel', 'Jacob W. Borden', 'Chris Santos', 'SharePoint Backups', 'SharePoint Backups', 'Martin Kendall (Admin)', 'Michael D. Loggins', 'Martin Kendall', 'Jason Legendre', 'Steve Tetley', 'Andy Shaw', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Alberto GÃ³mez de Segura', 'Beatriz LÃ³pez Coca', 'Jurgi Berakoetxea', 'SharePoint Backups', 'SharePoint Backups', 'Paula Currie (Admin)', 'SharePoint Backups', 'SharePoint Backups', 'Luc Wambeke', 'Patxi Andonegi', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'SharePoint Backups', 'Nonzuzo Qwane', 'Nonzuzo Qwane']</t>
+  </si>
+  <si>
+    <t>['Richard Driver', 'Chris Johnson', 'Colin Gibson', 'Miguel Hernandez', 'Stephen Farrow', 'Stephen MCSweeney', 'Shintaro Saito', 'Miguel Hernandez', 'Dany Tharakan', 'Girish Poojari', 'Miguel Pinto', 'Matthew Cockburn', 'Don Ward', 'Thomas West', 'Tom Crichton', 'Michael Hunter', 'Ian Brown', 'Paul S (ETC) Bennett', 'Vitaliy Burnashev', "Alex O'Connell", 'James Croucher', 'Ben Carter', 'Mark Jeacock', 'Martin Breen', 'Seamus Dunne', 'Daniel Ives', 'Owen R Jones', 'Diego Saiz', 'Mahesh Morjaria', 'Shintaro Saito', 'Evgeni Holodovsky', 'Sherwin Robinson', 'Seamus Dunne', 'Simon Barton', 'Matthew Cockburn', 'Alan Galbraith', 'Colin Gibson', 'Girish Poojari', 'Miguel Hernandez', 'Mahesh Morjaria', 'Stephen Farrow', 'Chris Johnson', 'Richard Driver', 'Simon Barton', 'Alan Galbraith', 'Martin Breen', 'Owen R Jones', 'Tom Crichton', 'Tom Hemingway', 'Ben Carter', 'Vignesh Patel', 'Sherwin Robinson', 'Paul Roberts', 'Colin Gibson', 'Vicky Wade', 'Jeanie Kennedy', 'Eugene Lobo', 'Chris Johnson', 'Agnieszka Green', 'Robert Mason', 'Akiko Iguchi', 'Dany Tharakan', 'Girish Poojari', 'Girish Poojari', 'Colin Gibson', 'Colin Gibson', 'Dany Tharakan', 'Girish Poojari', 'Chris Johnson', 'Colin Gibson', 'Julian Amarasena', 'Adrian Dica', 'Tom Bodsworth', 'Dany Tharakan', 'Girish Poojari', 'Miguel Pinto', 'Paul Roberts', 'Julian Amarasena', 'Adrian Dica', 'Matthew Ho', 'Tom Bodsworth', 'Dany Tharakan', 'Girish Poojari', 'Dany Tharakan', 'Girish Poojari', 'Miguel Pinto', 'Paul Roberts', 'Richard Driver', 'Chris Johnson', 'Nagore Blanco', 'Chris Johnson', 'Colin Gibson', 'Richard Driver', 'Nagore Blanco', 'Paul Roberts', 'Adrian Dica', 'Julian Amarasena', 'Matthew Ho', 'Thomas Litster', 'Sean Mackenzie', 'Tom Bodsworth', 'Abraam Asaad', 'Syed Ali', 'Yasmin Bahyan', 'Horacio Andres Acevedo', 'Dhimesh Parmar', 'Dany Tharakan', 'Girish Poojari', 'Paul Roberts', 'Adrian Dica', 'Thomas Litster', 'Dany Tharakan', 'Dany Tharakan', 'Miguel Pinto']</t>
+  </si>
+  <si>
+    <t>['Dave Robinson', "Kevin O'Carroll", 'Paula Currie', 'Simon Healy', 'Steve Arnold', 'Richard Phillips', 'Sonya Scott', 'Millie Ciciura', 'John Turner', 'Sean Edney', 'Hidetaka Shimuta', 'Justin Ellis', 'Dave Fordham', 'Karl Davies', 'Douglas Stewart', 'Andy Linscott', 'Andrew Massey', 'Julie Hannan', 'Simon Healy', 'Paul Jackson', 'Peter Norris', 'Julie Hannan', 'Paul Dillon', 'Paula Currie', 'Simon Healy', 'Pete Humphreys', 'David Gibbs', "Kevin O'Carroll", 'Mark Coppins', 'Paul Hands', 'Helen Brooks', 'Peter Norris', 'Chris Ball', 'Peter Austin', 'Simon Healy', 'Paul Barnes', 'James Owers', 'Jamie Moss', 'Jonathan Lennox', 'Tom Dudgeon', 'Stuart Robb', 'Scott Bell', 'Sean Edney', 'Darren Barnes', 'Julie Hannan', 'Nick Pittwood', 'Peter Rogers', 'Mark Jeffries', 'Nick Pittwood', 'Tracey Richardson', 'Pete Humphreys', 'Paul Barnes', 'James Owers', 'John Turner', 'Adam Clark', 'Lewis Williams', 'Richard Phillips', 'Fiona James', 'Sonya Scott', 'Millie Ciciura', 'Eleazar Marbach Test UK', 'Jeremy Wicks', 'Andy Still', 'David Gibbs', 'Mark Coppins', 'Peter Rogers', 'Steve Arnold', 'Andy Still', 'Peter Norris', 'Mike Brown', 'Richard Stirling', 'Ian Hay', 'Gedi Sleckus', 'Richard Weir', 'Julie Hannan', 'Dave Westbury', 'Helen Brooks', 'Chris Ball', "Damien O'Carroll", 'Kirsty Hensher', 'Simon Vaughan West', 'Mike Smee', 'Jeremy Wicks', 'David Gibbs', 'Kenny Choong', 'Joanne Gardiner', 'Hayley Walker', 'Scott Murrin', 'Peter Norris', 'Clive Norris', 'John Turner', 'Michael Spence', 'Dave Robinson', 'Pete Humphreys', 'Ranga Nasho', 'Julie Hannan', 'Stuart Knox', 'Dave Westbury', 'Rajdeep Datta', 'Marcus Costello', 'Martyn Sharp', 'Paul Boff', 'Sam Culley', 'Dave Manning', 'Richard Stirling', 'Barrie Wolfe', 'James Jones', 'Clive Norris', 'Andy Still', 'Mike Brown', 'Gary Brown', 'Paul Dillon', 'Paul Treadwell', 'David Quincey', 'Rick Voutt', 'Julie Hannan', 'Lewis Williams', 'Nick Pittwood', 'Dave Westbury', "Kevin O'Carroll", 'Hayley Walker', "Kevin O'Carroll", 'Julie Hannan', 'Nick Pittwood', 'Peter Rogers', 'Mark Jeffries', 'Dave Robinson', 'Mark Brinsley', 'Martin Eadon', 'Nicholas Bryant', 'Mark Welch', 'Hmad Naatit', 'Gavin Howell', 'Giorgos Markitanis', 'Dean Chidley', 'David Dunne', 'Janine Mellor', 'Adam Carter', 'Kenny Choong', 'Pete Humphreys', 'Jeremy Wicks', 'James Owers', 'Michael Spence', 'Phil Ward', 'Paul Dillon', 'Andy Hutchings', 'Keith Williams', 'Niall Murray', 'Glenn Moffat', 'Julie Hannan', 'Jason Nixon', 'Nick Pittwood', 'Tracey Richardson', 'Pete Humphreys', 'Scott Pritchard', 'Mark Jeffries', 'Paul Dillon', 'Clive Norris', 'Paul Barnes', 'James Owers', 'John Turner', 'Dave Fordham', 'Peter Noble', 'Lauren Gibson', 'Stuart John', 'Mark Jeffries', 'Sean Edney', 'Robert Wadsworth', 'Ben Malone', 'Dave Westbury', 'Helen Brooks', 'Darren Long', 'Lynn Whitehead', 'Sharon Stimpson', 'Adrian Murphy', 'Ross Threlfall', 'Julie Hannan', 'Jason Nixon', 'Simon Healy', 'Keith Nichols', 'Peter Norris', 'Paul Dillon', 'Nick Pittwood', "Kevin O'Carroll", 'Paula Currie', 'Julie Hannan', 'Jason Nixon', 'Julie Hannan', 'Tim Dicks', 'Dave Westbury', "Kevin O'Carroll", 'Dave Westbury', 'Peter Norris', 'Chris Ball', 'Julie Hannan', 'Jason Nixon', 'Paula Currie', 'Paul Jackson', 'Keith Nichols', 'Lewis Brock', 'Lewis Williams', 'Richard Phillips', "Kevin O'Carroll", 'Paula Currie', 'Julie Hannan', 'Jason Nixon', 'Simon Healy', 'Dave Westbury', "Kevin O'Carroll", 'Paul Barnes', 'Chris Ball', 'Kirsty Hensher', 'Ian Hay', 'Dave Westbury', 'Steve Kinns', 'Stephen Martin', 'Martin Bazeley', 'Owen Jones', 'Tim Dicks', 'Philip James', 'Martin Bjeletic', 'Alan Pacey', 'Andrei Imbrovschi', 'Dave Matthews', 'Roy Hutton', 'Stuart Bunby', 'Dwane Barker', 'Alex Goli', 'Paula Currie', 'Simon Healy', 'Mark Jeffries', 'Paula Currie', 'Paul Barnes', 'Andy Moffat', 'Nick Tyson', 'Sean Edney', 'Julie Hannan', 'Lewis Williams', 'Peter Noble', 'Norman Seaward', 'Hayley Walker', 'Mark Jeffries', 'Peter Norris', 'Chris Ball', 'Ranga Nasho', 'Richard Phillips', 'Stuart John', 'Fiona James', 'Stephanie Muigai', 'Mark Jeffries', 'Richard Broughton', 'Ralph Craven', 'Jonathan Lennox', 'Graeme Ewart', 'Peter Mann', 'Gary Haynes', 'Stuart Cheyne', 'Mark Jeffries', 'Clive Norris', 'Andrew Butlin', 'Martin Costin', 'Nick Tyson', 'Sean Edney', 'Sam Curson', 'Adrian Hickson', "Kevin O'Carroll", 'Lewis Williams', 'Nick Pittwood', 'Dave Westbury', "Kevin O'Carroll", 'Mark Coppins', 'Lewis Williams', 'Peter Norris', 'Julie Hannan', 'Lewis Williams', 'Dave Westbury', 'Norman Seaward', 'Hayley Walker', 'Lauren Gibson', 'Helen Brooks', 'Richard Phillips', 'Gary Haynes', 'Scott Pritchard', 'Roni DaSilva', 'Julie Hannan', 'Chris Ball', 'Nick Beaumont', 'Kirsty Hensher', 'Charlotte Lowe', 'Alex McKears', 'Simon Vaughan West', 'Ranga Nasho', 'Clive Norris', 'Andrew Quainton', 'Mark Nicol', 'Peter Bell', 'Craig Hibbert', 'Tim Makin', 'Sam Curson', 'Dave Westbury', "Kevin O'Carroll", 'Mark Coppins', 'Peter Norris', 'Paul Beaumont', 'Pete Humphreys', 'Paula Currie', 'Peter Norris', 'Simon Healy', 'Dave Westbury', 'Dave Fordham', 'Nick Pittwood', 'Tracey Richardson', 'Scott Pritchard', 'Clive Norris', 'Gareth Thomas', 'Mark Brinsley', 'Dean Chidley', 'Adam Carter', 'Julie Hannan', 'Ranga Nasho', 'Mark Jeffries', 'Tom Dudgeon', 'Scott Bell', 'Darrin Laing', 'Julie Hannan', 'Jason Nixon', 'Peter Rogers', 'Paul Jackson', 'Keith Nichols', 'Lewis Brock', 'Peter Rogers', 'Paula Currie', 'Julie Hannan', 'Jason Nixon', 'Simon Healy', 'Paul Jackson', 'Keith Nichols', 'Lewis Brock', 'Dave Fordham', 'Andrew Butlin', 'Nick Tyson', 'Adrian Hickson', 'Radley Plotegher', 'Mark Jeffries', 'Bill Turner', 'Simon Young', 'Gary Boucher', 'Jason Lee', 'Pete Humphreys', 'Ranga Nasho', 'Dave Robinson', 'Glenn Moffat', 'Dave Fordham', 'Richard Liddy', 'Toby Elliot', 'Struan Clark', 'Peter Norris', 'Paul Barnes', 'James Owers', 'Bill Turner', 'Andrew Duffy', 'Nick Tyson', 'Peter Mann', 'Adrian Hickson', 'Al Ahmed', 'Dave Westbury', 'Mark Coppins', 'Peter Norris', 'Paul Barnes', 'James Owers', 'Andy Moffat', 'Darren Devenish', 'Tony Sponsillo', 'Andrew Streeting', 'Tim Wenman', 'Christian Lyth', 'Steve Arnold', 'Paul Treadwell', 'Pete Humphreys', 'Dave Westbury', 'Paul Beaumont', 'Jason Reynolds', "Damien O'Carroll", 'Victoria May', 'Jackie Morris', 'Lindsey Purser', 'Hidetaka Shimuta', 'Imola Ilyes', 'Pete Humphreys', 'Lewis Williams', 'Peter Noble', 'Nick Pittwood', 'Tracey Richardson', 'Mark Jeffries', 'Paul Dillon', 'Dave Fordham', 'Julie Hannan', 'Lauren Gibson', 'Lewis Brock', 'Dave Westbury', 'Peter Noble', 'Dave Robinson', 'Steve Kinns', 'Norman Seaward', 'Mark Coppins', 'Paul Hands', 'Peter Rogers', 'Hayley Walker', 'Helen Brooks', 'Lewis Williams', 'Peter Norris', 'Chris Ball', 'Peter Austin', 'Paul Beaumont', 'Stuart Knox', 'Richard Stirling', 'Stuart John', 'Scott Murrin', 'Peter Noble', 'Dave Fordham', 'Graeme Chesworth', 'Scott Tully', 'Phil Ward', 'Gedi Sleckus', 'Louise West', 'Norman Seaward', 'Callum Barrell', 'Lee MacGuinness', 'Dave Westbury', 'Scott Murrin', 'Anna James', 'Lewis Williams', 'Richard Phillips', 'Fiona James', 'Sonya Scott', 'Millie Ciciura', 'Paul Dillon', 'James Owers', 'Nik Watson', 'Glenn Moffat', 'Martin Costin', 'Adam Clark', 'David Gibbs', 'Justin Ellis', 'Sarah King', "Kevin O'Carroll", 'Paul Barnes', 'Dave Pritchard', 'Malcolm Smith', 'Paula Currie', 'Julie Hannan', 'Jason Nixon', 'Simon Healy', 'Nick Pittwood', 'Peter Rogers', 'Peter Norris', 'Julie Hannan', 'Jason Nixon', 'Keith Nichols', 'Dave Westbury', 'Chris Ball', 'Peter Rogers', 'Nick Beaumont', 'Rebecca Talbot', 'Kirsty Hensher', 'Charlotte Lowe', 'Alex McKears', 'Thomas Heneghan', 'Safira Ahmed', 'Andrew Nolan', 'Simon Vaughan West', 'Caroline Jeffery', 'Dillon Corby-North', 'Hayley Wyatt', 'Chris Elliott', 'Laura Horwood', 'Eva Szczurek', 'Luisa Whatling', 'Julie Hannan', 'Peter Norris', 'Mark Coppins', 'Peter Rogers', 'Gavin Howell', 'Dave Westbury', 'Helen Brooks', 'Peter Austin', 'Stuart Knox', 'Stuart John', 'Mark Jeffries', 'Jonathan Lennox', 'Graeme Ewart', 'Peter Mann', 'Paul Barnes', 'James Owers', 'Jonathan Lennox', 'Peter Mann', 'Paul Barnes', 'Lewis Williams', 'Richard Phillips', 'Fiona James', 'Sonya Scott', 'Millie Ciciura', "Kevin O'Carroll", 'Julie Hannan', 'Paula Currie', 'Simon Healy', "Kevin O'Carroll", 'Mark Coppins', 'Lewis Williams', 'Richard Phillips', 'Fiona James', 'Sonya Scott', 'Millie Ciciura']</t>
+  </si>
+  <si>
+    <t>['Toti Maria', 'Saltarelli, Stefano', 'Moriggi Lucio', 'Perlini, Fabio', 'Severgnini, Walter', 'Gaetti Massimo', 'Giuliani Giacomo', 'Bartoli, Riccardo', 'Nicoli, Nicola', 'Scagliarini Andrea', 'Tebano, Raffaele', 'Bianchino Fabio', 'DirectionSMC-IT', 'Moriggi Lucio', 'Sala, Reginella', 'Rossi, Stefano', 'Riva, Mauro', 'Teruzzi Alessandro', 'Severgnini, Walter', 'Zeneli Betis', 'Colombo, Marino', 'Rubiliani, Roberto', 'Parigi Dafne', 'Londero, Luca', 'Borghi Francesco', 'Radaelli, Sonia', 'Trecca, Vincenzo', 'Roberta Mariani', 'Gnocchi Walter', 'Mancina, Giovanni', 'Occhionero, Andrea', 'Ferraresi, Francesca', 'Toccotelli, Gianmaria', 'Nubile, Rocco', 'Marinoni Paolo', 'Cataudella Natalino', 'Severgnini, Walter', 'Zeneli Betis', 'Colombo, Marino', 'Rubiliani, Roberto', 'Parigi Dafne', 'Trifone, Andrea', 'Borghi Francesco', 'Radaelli, Sonia', 'Trecca, Vincenzo', 'Mancina, Giovanni', 'Occhionero, Andrea', 'Nubile, Rocco', 'Di Paolo Leopoldo', 'Franceschi, Alberto', 'Arcari Matteo', 'Salacone Dario', 'Contini, Alessandro', 'Beretta, Viviana', 'Pollastri, Elisabetta', 'Mapelli Chiara', 'Colombo, Marino', 'Trifone, Andrea', 'Moriggi Lucio', 'Gazzaniga Massimo', 'Zeneli Betis', 'Severgnini, Walter', 'Ferrandi, Patrizio', 'Rossi, Stefano', 'Belloni, Laura', 'Borghi Francesco', 'Berto, Alessandro', 'Trecca, Vincenzo', 'Gnocchi Walter', 'Mancina, Giovanni', 'Catti Fabio', 'Di Paolo Leopoldo', 'Franceschi, Alberto', 'Bianchi Alberto', 'Severgnini, Walter', 'Colombo, Marino', 'Trifone, Andrea', 'Roberta Mariani', 'SciannamÃ¨ Maurizio', 'Cannamela Daniele', 'Radaelli, Sonia', 'SciannamÃ¨ Maurizio', 'Ferrandi, Patrizio', 'Severgnini, Walter', 'Zeneli Betis', 'Colombo, Marino', 'Rubiliani, Roberto', 'Parigi Dafne', 'Gnocchi Walter', 'Rubiliani, Roberto', 'Gamarino, Paolo', 'Castagnetti, Andrea', 'Severgnini, Walter', 'Zeneli Betis', 'Colombo, Marino', 'Trifone, Andrea', 'Colombo, Marino', 'Toti Maria', 'Gnocchi Walter', 'Roberta Mariani', 'Bevini Roberto', 'Moriggi Lucio', 'Perlini, Fabio', 'Severgnini, Walter', 'Gaetti Massimo', 'Giuliani Giacomo', 'Giovagnoni Marco', 'Lombardo, Eugenio', 'Pozzi Jonathan', 'Battistini Andrea', 'Trevisan Diego', 'Moriggi Lucio', 'Perlini, Fabio', 'Marinoni Paolo', 'Cataudella Natalino', 'Gnocchi Walter', 'Ferraresi, Francesca', 'Toccotelli, Gianmaria', 'Mustacchio Giorgio', 'Belletti, Gianni', 'Perlini, Fabio', 'La Spina Giuseppe', 'Coppola Giuseppe', 'Moriggi Lucio', 'Perlini, Fabio', 'Severgnini, Walter', 'Vassura Raffaele', 'Gaetti Massimo', 'Guerra, Luca', 'Battistini Andrea', 'Cazzaniga, Giancarlo', 'Veneziani, Luca', 'Vitiello Alessandro', 'Catti Fabio', 'Moriggi Lucio', 'Cavagna, Rosanna', 'Gnocchi Walter', 'Franceschi, Alberto', 'Borghi Francesco', 'Radaelli, Sonia', 'Brambilla, Max', 'Trecca, Vincenzo', 'Franceschi, Alberto', 'Moriggi Lucio', 'Gnocchi Walter', 'Rossi, Stefano', 'Villa, Massimiliano', 'Ravanelli, Diego', 'Casadio, Alberto', 'Bernazzani, Massimo', 'Muschi Andrea', 'Crippa Simone', 'Vendramini, Matteo', 'Colombo Andrea', 'Carro Alessandro', 'Tonati Fabio', 'Cazzaniga Simone', 'Ornaghi Filippo', 'Occhionero, Andrea', 'Nubile, Rocco', 'Gnocchi Walter', 'Bevini Roberto', 'Perlini, Fabio', 'Berto, Alessandro', 'Zeneli Betis', 'Cataudella Natalino', 'Manni, Mauro', 'Lanotte Davide', 'Milani Cristian', 'Vassura Raffaele', 'Gaetti Massimo', 'Zagatti, Marco', 'Saltarelli, Stefano', 'Coppola Giuseppe', 'Manco Giuseppe', 'Bolzoni Massimiliano', 'Marchesini, Andrea', 'Ditta Fabrizio', 'Guerra, Luca', 'Bertolin Filippo', 'Lombardo, Eugenio', 'Di Gaetano Mattia', 'Bartoli, Riccardo', 'Nicoli, Nicola', 'Calandra Buonaura Paolo', 'Morlini Nicola', 'Maione Egidio', 'Forte, Giovanni', 'Pifferi Simone', 'Galli Ruggero', 'Vecchi Michele', 'DiCarlo Matteo', 'Vitiello Alessandro', 'Bacchelli Mattia', 'Bianchino Fabio', 'Grippi Alex', 'Casolari Marco', 'Bartucca Giuseppe', 'Milani Cristian', 'Ravagli Gabriele', 'Moriggi Lucio', 'Perlini, Fabio', 'Severgnini, Walter', 'La Spina Giuseppe', 'Compare, Giuseppe', 'Coniglio Federico', 'Luporini Massimiliano', 'Forte, Giovanni', 'Occhionero, Andrea', 'Moriggi Lucio', 'Sala, Reginella', 'Rossi, Stefano', 'Meuti Tilde', 'Gnocchi Walter', 'Sala, Paola', 'Luppino Giulia', 'Roberta Mariani', 'Trecca, Vincenzo', 'Giuliani Francesca', 'Franceschi, Alberto', 'Severgnini, Walter', 'Zeneli Betis', 'Roberta Mariani', 'Mancina, Giovanni', 'Occhionero, Andrea', 'Nubile, Rocco', 'Franceschi, Alberto', 'Pilotti, Mauro', 'Ornaghi Filippo', 'Lanotte Davide', 'Panista Chiara', 'Gnocchi Walter', 'Parigi Dafne', 'Borghi Francesco', 'Radaelli, Sonia', 'Moriggi Lucio', 'Perlini, Fabio', 'Brambilla, Max', 'Colombo, Federica', 'Rossi, Paolo', 'De Fusco, Giuseppe', 'Severgnini, Walter', 'Roberta Mariani', 'SciannamÃ¨ Maurizio', 'Trecca, Vincenzo', 'Cavagna, Rosanna', 'Gnocchi Walter', 'Mancina, Giovanni', 'Occhionero, Andrea', 'Trifone, Andrea', 'Ferraresi, Francesca', 'Toccotelli, Gianmaria', 'Nubile, Rocco', 'Mandelli, Enrico', 'Ferrandi, Patrizio', 'Contini, Alessandro', 'Ciccu, Marcello', 'Marinoni Paolo', 'Cataudella Natalino', 'Perego, Stefano', 'Arcari Matteo', 'Patricelli, Alessandro', 'Franceschi, Alberto', 'Tornaghi, Fabio', 'Toffanin Massimo', 'Riva, Mauro', 'Gaetti Massimo', 'Mustacchio Giorgio', 'Milani Cristian', 'Colombo, Marino', 'Toti Maria', 'Roberta Mariani', 'Bernazzani, Massimo', 'Moriggi Lucio', 'Perlini, Fabio', 'Severgnini, Walter', 'Riva, Mauro', 'Piana Marco', 'Busato, Livio', 'Muschi Andrea', 'Borsani, Michele', 'Colombo Andrea', 'Bartoli, Riccardo', 'Tomo Matteo', 'Trotta Andrea', 'Trevisan Diego', 'Tebano, Raffaele', 'Verzeroli, Claudio', 'Hiroshi.Ueda', 'Roberta Mariani', 'Severgnini, Walter', 'Gnocchi Walter', 'Radaelli, Sonia', 'Moriggi Lucio', 'Perlini, Fabio', 'Sala, Reginella', 'Severgnini, Walter', 'SciannamÃ¨ Maurizio', 'Longo, Antonio', 'Cavagna, Rosanna', 'Sala, Paola', 'Zeneli Betis', 'Trifone, Andrea', 'Catti Fabio', 'Ferrandi, Patrizio', 'Contini, Alessandro', 'Scalabrini Elena', 'Colloi, Sara', 'Bevini Roberto', 'Milani Cristian', 'Franceschi, Alberto', 'Bianchi Alberto', 'Fruci Giuseppe', 'Savino Lodovico', 'Severgnini, Walter', 'Longo, Antonio', 'Cavagna, Rosanna', 'Barlassina Chiara', 'Cimmino, Pasquale', 'Patricelli, Alessandro', 'Marchesini, Andrea', 'Bevini Roberto', 'DiCarlo Matteo', 'Vitiello Alessandro', 'Bacchelli Mattia', 'Bianchino Fabio', 'Moriggi Lucio', 'Gnocchi Walter', 'Roberta Mariani', 'SciannamÃ¨ Maurizio', 'Colombo, Marino', 'Belpasso Marco', 'Trecca, Vincenzo', 'Centofanti Massimiliano', 'Cimmino, Pasquale', 'Di Paolo Leopoldo', 'Mancina, Giovanni', 'Rossi, Stefano', 'Milani Cristian', 'Gaetti Massimo', 'Coppola Giuseppe', 'Milani Cristian', 'Moriggi Lucio', 'Perlini, Fabio', 'Severgnini, Walter', 'Gaetti Massimo', 'Coppola Giuseppe', 'Guerra, Luca', 'Marega, Stefano', 'Forte, Giovanni', 'Semenzato Marco', 'Borghi Francesco', 'Belletti, Gianni', 'Moriggi Lucio', 'Perlini, Fabio', 'Severgnini, Walter', 'La Spina Giuseppe', 'Giuliani Giacomo', 'Bernardi, Davide', 'Laurenti, Raffaele', 'Battistini Andrea', 'Veneziani, Luca', 'Tosolini, Gianni', 'Franceschi, Alberto', 'Moriggi Lucio']</t>
+  </si>
+  <si>
+    <t>['Aniene Cading', 'Jimmy Nilsson', 'TorbjÃ¶rn Lundberg', 'Marcus Mazetti', 'Fredrik Lundberg', 'Aisha Loma Roman', 'Jimmy Nilsson', 'Nicklas LÃ¶vebrant', 'Jimmy Nilsson', 'Edvard Larsheden', 'Martin Hanson', 'Joakim Kalcidis', 'Joakim Floberg', 'Magnus KarlstrÃ¶m', 'Nicklas LÃ¶vebrant', 'Klas Axelson', 'Jimmy Nilsson', 'Mikael Andersson', 'Peter Ã„lgekrans', 'Robert Schill', 'Jimmy Nilsson', 'Magnus KarlstrÃ¶m', 'Aniene Cading', 'Mattias Sundberg', 'Martin Jarlegren', 'Klas Axelson', 'Jimmy Nilsson', 'Mikael Andersson', 'Magnus Innala', 'Martin Hanson', 'Henrik Lyckekrantz', 'Mattias LidÃ©n', 'Markus ThÃ¤rning', 'Theresa Hultgren', 'Jimmy Nilsson', 'Magnus KarlstrÃ¶m', 'Aniene Cading', 'Mattias Sundberg', 'Martin Jarlegren', 'Klas Axelson', 'Jonas Lyngemark', 'Mikael Andersson', 'Jerker Ã…strand', 'Mattias LidÃ©n', 'Nicklas LÃ¶vebrant', 'Mikael Andersson', 'TorbjÃ¶rn Lundberg', 'Joakim Floberg', 'Melker Holmgren', 'Bianca Ã–hman', 'Cecilia Charo', 'Bianca Ã–hman', 'PÃ¥l HallstrÃ¶m', 'HÃ¥kan Vestergren', 'Anders BjÃ¶rkstrÃ¶m', 'Maria SÃ¶dergren', 'Mikael Andersson', 'Mattias Sundberg', 'Mattias LidÃ©n', 'Nicklas LÃ¶vebrant', 'Nicklas LÃ¶vebrant', 'Nicklas LÃ¶vebrant', 'Nicklas LÃ¶vebrant', 'TorbjÃ¶rn Lundberg', 'Joakim Floberg', 'Nicklas LÃ¶vebrant', 'Jimmy Nilsson', 'Edvard Larsheden', 'Aniene Cading', 'Bianca Ã–hman', 'Peter Larsson', 'Jimmy Nilsson', 'Nicklas LÃ¶vebrant', 'Mattias Sundberg', 'Nicklas LÃ¶vebrant', 'Jimmy Nilsson', 'Mikael Andersson', 'TorbjÃ¶rn Lundberg', 'Theresa Hultgren', 'Nicklas LÃ¶vebrant', 'Bianca Ã–hman', 'Nicklas LÃ¶vebrant', 'Bianca Ã–hman', 'Jimmy Nilsson', 'Mikael Andersson', 'TorbjÃ¶rn Lundberg', 'Joakim Floberg', 'Maria SÃ¶dergren', 'Peter Larsson', 'Cecilia Charo', 'Jimmy Nilsson', 'Joakim Kalcidis', 'Jonas Lyngemark', 'Jimmy Nilsson', 'Bianca Ã–hman', 'Joakim Floberg', 'Peter Larsson', 'Martin Jonsson', 'Jimmy Nilsson', 'Jimmy Nilsson', 'Edvard Larsheden', 'Joakim Kalcidis', 'Michael Milanius', 'Magnus KarlstrÃ¶m', 'Aniene Cading', 'Mattias Sundberg', 'Martin Jarlegren', 'Klas Axelson', 'Bianca Ã–hman', 'Peter Larsson', 'Joakim Floberg', 'Nicklas LÃ¶vebrant', 'Carola Fredriksson', 'Ulrica HÃ¶rnstrÃ¶m', 'PÃ¥l HallstrÃ¶m', 'Oskar Holm', 'Fredrik Digertz', 'Mats Ruberg', 'Maria KÃ¥vestam', 'Melker Holmgren', 'Jan Jingbro', 'Daniel Sterner', 'Tomas Ekholm', 'Bianca Ã–hman', 'Per-Olof MÃ¥nsson', 'Jimmy Nilsson', 'Mikael Andersson', 'TorbjÃ¶rn Lundberg', 'Joakim Floberg', 'HÃ¥kan Vestergren', 'Joakim Jensen', 'Stefan Svensson', 'Tommy Lindqvist', 'Marko Baarman', 'Lager AllmÃ¤n', 'Fredrik Lundberg', 'Edvard Larsheden', 'Michael Milanius', 'Magnus Innala', 'Martin Hanson', 'Peter Ã„lgekrans', 'LÃ¶n Admin', 'Anders BjÃ¶rkstrÃ¶m', 'Robert Schill', 'Bertil Wernius', 'Jamaal Humud', 'Tomas Ericson', 'Bengt Eriksson', 'Joachim Lind', 'Tomas LandstrÃ¶m', 'Magnus KarlstrÃ¶m', 'Aniene Cading', 'Edvin Tjernlund', 'Henrik Lyckekrantz', 'JÃ¶rgen Samuelsson', 'Maria SÃ¶dergren', 'Mattias Sundberg', 'Jerker Ã…strand', 'Niklas Lindberg', 'Bonny Johansson', 'Linda Salo', 'Marcus Andersson', 'Martin Jarlegren', 'Richard Godenhielm', 'Peter Larsson', 'Martin Jonsson', 'JÃ¶rgen Petersson', 'Kenny Svanberg', 'Hans Frick', 'Tobias Viberg', 'Mattias LidÃ©n', 'Aisha Loma Roman', 'Christian Larsson', 'Markus ThÃ¤rning', 'Cecilia Charo', 'Stefan Johannisson', 'Ulf Petersen', 'Alexander Zurka', 'Kenneth Karlsson', 'Lars Hjalmarsson', 'Klas Axelson', 'Anders Wineteg', 'Gailen Moondone', 'Johan Folkesson', 'Thomas Wisting', 'Jonas Lyngemark', 'Daniel Koneski', 'Jimmy SunnegÃ¥rdh', 'Joakim Kalcidis', 'Theresa Hultgren', 'Filip Ristic', 'Helena Wallner', 'Peter KohlstrÃ¶m', 'Marcus Mazetti', 'Martin Fredriksson-Pehrson', 'Joakim Quist', 'Emil Wahlberg', 'Bianca Ã–hman', 'Bianca Ã–hman', 'HÃ¥kan Vestergren', 'PÃ¥l HallstrÃ¶m', 'Anders BjÃ¶rkstrÃ¶m', 'Maria SÃ¶dergren', 'Marcus Mazetti', 'Bianca Ã–hman', 'HÃ¥kan Vestergren', 'Anders BjÃ¶rkstrÃ¶m', 'Bianca Ã–hman', 'Cecilia Charo', 'Nicklas LÃ¶vebrant', 'Cecilia Charo', 'Melker Holmgren', 'Bianca Ã–hman', 'Filip Ristic', 'Bianca Ã–hman']</t>
+  </si>
+  <si>
+    <t>['Krista Koskinen', 'Petri Keski-Honkola', 'Johan GrÃ¤sbeck', 'Jan Carlsson', 'Harri Lehtola', 'Petri Keski-Honkola', 'Pauli Korkolainen', 'Harri Lehtola', 'Ari Salminen', 'Petri Keski-Honkola', 'Pauli Korkolainen', 'Toni SkogstrÃ¶m', 'Harri Lehtola', 'Johan GrÃ¤sbeck', 'Ossi Ojainmaa', 'Tuomas Hakanen', 'Krista Koskinen', 'Pauli Korkolainen', 'Taina SillanpÃ¤Ã¤', 'Jan Carlsson', 'Toni SkogstrÃ¶m', 'Petri Keski-Honkola', 'Eeva Toivanen', 'Sampsa Paasisalo', 'Harri LeppÃ¤nen', 'Kai Palotie', 'Joanna SirÃ©n', 'Sanni Kokkonen', 'Juuso Reinikka', 'Samuli Suokas', 'Marko Lipponen', 'Jukka Muhonen', 'BÃ¶rje Kuusisto', 'Risto Honkanen', 'Jarmo Koivulahti', 'Harri Lehtola', 'Johan GrÃ¤sbeck', 'Juha-Pekka Tikkanen', 'Timo Peurala', 'Jani StengÃ¥rd', 'Juha Kemppi', 'Ossi Ojainmaa', 'Jorma HyvÃ¶nen', 'Ari Salminen', 'Jari Lehtonen', 'Tuomas Hakanen', 'Markku PerÃ¤lampi', 'Esa KivistÃ¶', 'Jarno Kaikkonen', 'Simo Lyytinen', 'Jarno TantarimÃ¤ki', 'Erja Valkonen', 'Eeva Toivanen', 'Samuli Suokas', 'Kai Palotie', 'Joanna SirÃ©n', 'Sanni Kokkonen', 'Juuso Reinikka', 'Johan GrÃ¤sbeck', 'Taina SillanpÃ¤Ã¤', 'Harri Lehtola', 'Johan GrÃ¤sbeck', 'Toni SkogstrÃ¶m', 'Petri Keski-Honkola', 'Harri Lehtola', 'Johan GrÃ¤sbeck', 'Ossi Ojainmaa', 'Johan GrÃ¤sbeck', 'Pauli Korkolainen', 'Krista Koskinen', 'Krista Koskinen', 'Harri Lehtola', 'Toni SkogstrÃ¶m', 'Taina SillanpÃ¤Ã¤']</t>
+  </si>
+  <si>
+    <t>['SMC - Ole JÃ¸rgensen', 'SMC - Mia B. F. JÃ¸rgensen', 'SMC - Steen Herbild', 'SMC - Mia B. F. JÃ¸rgensen', 'SMC - Benjamin Mackenhauer', 'SMC - Lasse Hindsig', 'SMC - Jakob BjÃ¸rner Kirkegaard', 'SMC - Anja Kruse Kristensen', 'SMC - Benjamin Mackenhauer', 'SMC - Claus Rathje', 'SMC - Tina Mortensen', 'SMC - Glennie T. SÃ¸rensen', 'SMC - Ole Mathiesen', 'SMC - Joan Nowak HÃ¸gh', 'SMC - Benjamin Mackenhauer', 'SMC - Martin BÃ¼ttner', 'SMC - Mia B. F. JÃ¸rgensen', 'SMC - Benjamin Mackenhauer', 'SMC - Benjamin Mackenhauer', 'SMC - Anja Kruse Kristensen', 'SMC - Martin Minddal Jakobsen', 'SMC - Henrik Bonde Jespersen', 'SMC - Ole JÃ¸rgensen', 'SMC - Mia B. F. JÃ¸rgensen', 'SMC - Kenneth Dam Nielsen', 'SMC - Daniel KÃ¸pke', 'SMC - Steen Herbild', 'SMC - Dorthe Holm', 'SMC - Tommy Testmann', 'SMC - Mick SÃ¸rensen', 'SMC - Ole JÃ¸rgensen', 'SMC - Jakob BjÃ¸rner Kirkegaard', 'SMC - Ivar Christensen', 'SMC - Anja Kruse Kristensen', 'SMC - Nicoline Svit Thomasen', 'SMC - Rikke Friis Bonde', 'SMC - Joan Nowak HÃ¸gh', 'SMC - Glennie T. SÃ¸rensen', 'SMC - Gerda Bigum Nielsen', 'SMC - Henrik Bonde Jespersen', 'SMC - Martin Minddal Jakobsen', 'SMC - Lasse Hindsig', 'SMC - Phillip Lund Rasmussen', 'SMC - Susanne Jakobsen', 'SMC - Martin Skovsgaard Jensen', 'SMC - Martin BÃ¼ttner', 'SMC - Claus Rathje', 'SMC - Ole Mathiesen', 'SMC - Michelle Lindgren Nielsen', 'SMC - Tina Mortensen', 'SMC - Mia B. F. JÃ¸rgensen', 'SMC - Marianne Rasmussen', 'SMC - Marianne Juul Larsen', 'SMC - Benjamin Mackenhauer', 'SMC - Iben Skov Eslund', 'SMC - Jonny Hilgenfeld', 'SMC - Kenneth Dam Nielsen', 'SMC - Steen Herbild', 'SMC - Joan Nowak HÃ¸gh', 'SMC - Kenneth Dam Nielsen', 'SMC - Tommy Testmann', 'SMC - Glennie T. SÃ¸rensen', 'SMC - Nicoline Svit Thomasen', 'SMC - Tina Mortensen', 'SMC - Steen Herbild', 'SMC - Kenneth Dam Nielsen', 'SMC - Glennie T. SÃ¸rensen', 'SMC - Kenneth Dam Nielsen', 'SMC - Tommy Testmann', 'SMC - Henrik Bonde Jespersen', 'SMC - Tina Mortensen', 'SMC - Claus Rathje', 'SMC - Kenneth Dam Nielsen', 'SMC - Tina Mortensen', 'SMC - Steen Herbild', 'SMC - Joan Nowak HÃ¸gh', 'SMC - Kenneth Dam Nielsen', 'SMC - Steen Herbild', 'SMC - Tina Mortensen', 'SMC - Anja Kruse Kristensen', 'SMC - Joan Nowak HÃ¸gh', 'SMC - Mia B. F. JÃ¸rgensen', 'SMC - Tina Mortensen', 'SMC - Ole Mathiesen', 'SMC - Tommy Testmann', 'SMC - Kenneth Dam Nielsen', 'SMC - Tina Mortensen', 'SMC - Glennie T. SÃ¸rensen']</t>
+  </si>
+  <si>
+    <t>['Ellen Parik', 'Eduard Sauks', 'Valeria Serebrjanski', 'Ellen Parik', 'Helgi Arjut', 'Sulev Lindlaan', 'Veiko VainkÃ¼la', 'Marika Seen', 'Martin Paigelkaln', 'Nikita Berlinberg', 'Marko PÃµldoja', 'Ellen Parik', 'Nikita Berlinberg', 'Aleksandr Trummal', 'Ellen Parik', 'Eduard Sauks', 'Ellen Parik', 'Nikita Berlinberg', 'Aleksandr Trummal', 'Valeria Serebrjanski', 'Eduard Sauks', 'Ellen Parik', 'Eduard Sauks']</t>
+  </si>
+  <si>
+    <t>['Javier Azcona', 'David Perez', 'Agustin Gomez', 'Nerea Izquierdo', 'Laura Herran', 'Inigo Ibarzabal', 'Agustin Gomez', 'Laura Herran', 'Inigo Ibarzabal', 'Laura Herran', 'Inigo Ibarzabal', 'Javier Azcona', 'Inigo Ibarzabal', 'Borja Arberas', 'David Perez', 'Laura Herran', 'Javier Azcona', 'Agustin Gomez', 'Nerea Izquierdo', 'Agustin Gomez', 'Javier Azcona', 'Inigo Ibarzabal', 'Nerea Izquierdo', 'Laura Herran', 'Javier Azcona', 'Agustin Gomez', 'Veronica Perez', 'Inigo Ibarzabal', 'Javier Azcona', 'Agustin Gomez', 'Inigo Ibarzabal', 'Laura Herran', 'Javier Azcona', 'Inigo Ibarzabal', 'Agustin Gomez', 'David Perez', 'Nerea Izquierdo', 'Veronica Perez', 'Laura Herran', 'Agustin Gomez', 'Nerea Izquierdo', 'Javier Azcona', 'Inigo Ibarzabal', 'Agustin Gomez', 'Nerea Izquierdo', 'Laura Herran', 'Inigo Ibarzabal', 'Javier Azcona', 'Javier Azcona', 'David Perez', 'Inigo Ibarzabal', 'Agustin Gomez', 'Borja Arberas', 'Nerea Izquierdo', 'Veronica Perez', 'Laura Herran', 'Javier Azcona', 'Javier Azcona', 'David Perez', 'Javier Azcona', 'Borja Arberas', 'Veronica Perez', 'Javier Azcona', 'Inigo Ibarzabal', 'Javier Azcona', 'Agustin Gomez', 'Laura Herran', 'Agustin Gomez', 'David Perez', 'David Perez', 'Javier Azcona', 'David Perez', 'Veronica Perez', 'Inigo Ibarzabal', 'Javier Azcona', 'Agustin Gomez', 'Nerea Izquierdo', 'Javier Azcona', 'Javier Azcona', 'Inigo Ibarzabal', 'Laura Herran', 'Javier Azcona', 'Inigo Ibarzabal', 'Agustin Gomez', 'David Perez', 'Nerea Izquierdo', 'Veronica Perez', 'Laura Herran', 'Inigo Ibarzabal', 'Javier Azcona', 'Agustin Gomez', 'David Perez', 'Nerea Izquierdo', 'Veronica Perez', 'Laura Herran']</t>
+  </si>
+  <si>
+    <t>['Daniel Langmeier', 'Eleazar Marbach', 'Patrick Caviezel', 'Gilbert Schmid', 'Andreas GÃ¼ttinger', 'Jeremy Bolt', 'Doris Roth', 'Robin Hassler', 'Peter Niederhauser', 'Francoise Gledhill-Taylor', 'Jean-Pierre Eugler', 'JÃ¼rgen Kern', 'Michael Conde', 'Pius Furrer', 'Pierre-AndrÃ© Borne', 'Andreas GÃ¼ttinger', 'Fabrice Buser', 'Robert Camenzind', 'Diego SchlÃ¼ssel', 'Elsbeth Kaegi', 'Eveline Meili', 'Dilara Dumanoglu', 'Tea Tubanovic', 'Manuel HÃ¤nni', 'Michael Vonarburg', 'Patrizia Eberhart', 'Jeremy Bolt', 'Eleazar Marbach', 'Gilbert Schmid', 'Patrick Caviezel', 'Eleazar Marbach', 'Daniel Rellstab', 'Jeremy Bolt', 'Eleazar Marbach', 'Kurt Wyss', 'Helmut Spiegelhalter', 'Edy Brueschweiler', 'Jessica Spuehler', 'Daniel Langmeier', 'Helmut Spiegelhalter', 'JÃ¼rgen Kern', 'Gabriela Notz', 'Michael Trachsler', 'Martin Henseler', 'Kezban Karatas-Koca', 'Peter Niederhauser', 'Jessica Spuehler', 'Parwaneh Rajabi', 'Jeremy Bolt', 'Alessandro Grizzetti', 'Denise Aregger', 'Christopher Closuit', 'Christine Giacobetti', 'StÃ©phane Wampfler', 'Gregor RÃ¼egg', 'Jeremy Bolt', 'Eleazar Marbach', 'Francoise Gledhill-Taylor', 'Christof Brux', 'Stefan RÃ¼egg', 'Daniel Rellstab', 'Edy Brueschweiler', 'Daniel Langmeier', 'Michael Vonarburg', 'Samuel Marti', 'Kurt Wyss', 'Edith Rickenbacher', 'Peter Niederhauser', 'Karin Martin', 'Robert Camenzind', 'Cornelis De Vos', 'Ronny Balmer', 'Roland Bruggmann', 'Kurt Meili', 'Alessandro Grizzetti', 'Christine Giacobetti', 'Helmut Spiegelhalter', 'Marco Aeschimann', 'Christoph Peter', 'Francesco Paradiso', 'Pascal Bass', 'Andreas Irminger', 'Nadja Pfister', 'Manuel HÃ¤nni', 'Parwaneh Rajabi', 'Monica Stoop', 'Christopher Closuit', 'Patrick Wydler', 'Patrizia Eberhart', 'Jean-Pierre Eugler', 'JÃ¼rgen Kern', 'Marcel Volkart', 'Rolf Gutknecht', 'Mike Vogel', 'Artan Kabashi', 'Walter Tschanen', 'Leandro Schwengeler', 'David De Silva', 'Ufuk SÃ¶nmez', 'Rahel Glanzmann', 'Raphael Steiner', 'Kilian GrÃ¤nicher', 'Andreas Mebold', 'Atilla Bagci', 'Roland Stamm', 'Gabriela Notz', 'Fritz Diebold', 'Diego SchlÃ¼ssel', 'Roman Meier', 'Luca Nuzzo', 'Georges Gassmann', 'Marc Schultheiss', 'Simon Ganz', 'Reto BÃ¼chel', 'Michael Trachsler', 'Elsbeth Kaegi', 'Eveline Meili', 'Patrick Suchet', 'Pierre Anker', 'Martin Specker', 'Peter Klein', 'Roman FÃ¤ssler', 'Michael Conde', 'Reto Gassmann', 'Nuno Mesquita', 'Martin Henseler', 'Franz Koch', 'Marco Biasi', 'Pius Furrer', 'Remo Wettach', 'Roberto Bufano', 'Denise Aregger', 'Marco RÃ¼egg', 'Claude Brunner', 'Pierre-AndrÃ© Borne', 'Joel Faivre', 'Andreas GÃ¼ttinger', 'Marco Bertozzi', 'Aris Helfenstein', 'Patrick Zeller', 'Oliver Trummer', 'Simon Gremaud', 'Fabrice Buser', 'Daniel Balmer', 'Atdhe Kadrijaj', 'Fabio Andretto', 'Michel Schmid', 'Doris Roth', 'Dominik HÃ¼ttig', 'Roger MÃ¼ller', 'Steven Matzinger', 'Dominik Gubler', 'Sorija Sun', 'Brian Molteni', 'Fatmir Shoshi', 'StÃ©phane Wampfler', 'Gregor RÃ¼egg', 'Martin Traxler', 'Dilara Dumanoglu', 'Gabriele Pellegrino', 'Sptim Zulali', 'Edvard Volmer', 'Kezban Karatas-Koca', 'Sacha Croset', 'Sylvain Chabert', 'Sergio Nuzzo', 'Tea Tubanovic', 'Mirza Alimanovic', 'Marc Bucher', 'Pascal Knechtenhofer', 'Pascal Rehnelt', 'Elif Kokolar', 'Roger Haefeli', 'Francesco Racinelli', 'Brigitte Kronenberg', 'Robin Hassler', "Maweshi N'kabuthusa", 'Dilek Koca', 'Gilbert Schmid', 'Patrick Caviezel', 'Manuel Bonjour', 'Jerome Chindamo', 'Patrik Scherrer', 'Michelle Odermatt', 'ChengChung Wu', 'Jerry Berchtold', 'Roger Marti', 'Vilson Qeta', 'Eleazar Marbach', 'Eleazar Marbach Test CH 1', 'Eleazar Marbach Test CH 2', 'Jeremy Bolt', 'Helmut Spiegelhalter', 'Patrizia Eberhart', 'Gabriela Notz', 'Robin Hassler', "Maweshi N'kabuthusa", 'Patrick Caviezel', 'Patrizia Eberhart', 'ChengChung Wu', 'Marco Aeschimann', 'Roman Meier', 'Luca Nuzzo', 'Dilara Dumanoglu', 'Dilek Koca', 'Edith Rickenbacher', 'Helmut Spiegelhalter', 'Jessica Spuehler', 'Robin Hassler', 'Jeremy Bolt', 'Michael Conde', 'Pius Furrer', 'Roberto Bufano', 'Doris Roth', 'Sylvain Chabert', 'Sergio Nuzzo', 'Eleazar Marbach', 'Patrick Caviezel', 'Pius Furrer', 'Kurt Meili', 'Manuel HÃ¤nni', 'Michael Trachsler', 'Jeremy Bolt', 'Stefan RÃ¼egg', 'Michael Vonarburg', 'Edith Rickenbacher', 'Roland Bruggmann', 'Helmut Spiegelhalter', 'Parwaneh Rajabi', 'Patrizia Eberhart', 'Jessica Spuehler', 'Michael Trachsler', 'Denise Aregger', 'Robin Hassler', 'Robin Hassler', 'Manuel HÃ¤nni', 'Jessica Spuehler', 'Atilla Bagci', 'Denise Aregger', 'Atilla Bagci', 'Jeremy Bolt', 'Eleazar Marbach', 'Jeremy Bolt', 'Jessica Spuehler', 'Roland Stamm', 'Robin Hassler', 'Fritz Diebold', 'Patrick Suchet', 'Reto Gassmann', 'Remo Wettach', 'Roberto Bufano', 'Michael Trachsler', 'Martin Specker', 'Peter Klein', 'Roman FÃ¤ssler', 'Pascal Rehnelt', 'Brigitte Kronenberg', 'Jeremy Bolt', 'Jeremy Bolt', 'Jessica Spuehler', 'Robin Hassler', 'Andreas Mebold', 'Pius Furrer', 'Marco Bertozzi', 'Aris Helfenstein', 'Dominik HÃ¼ttig', 'Dominik Gubler', 'Roger Haefeli', 'Michael Trachsler', 'Christopher Closuit', 'Marc Schultheiss', 'Karin Martin', 'Robert Camenzind', 'Jessica Spuehler', 'Diego SchlÃ¼ssel', 'Dilara Dumanoglu', 'Tea Tubanovic', 'Jeremy Bolt', 'Jessica Spuehler', 'Robin Hassler', 'Jean-Pierre Eugler', 'Nuno Mesquita', 'Pius Furrer', 'Atdhe Kadrijaj', 'Fabio Andretto', 'Brian Molteni', 'Eleazar Marbach', 'Jessica Spuehler', 'Ronny Balmer', 'Christoph Peter', 'Andreas Irminger', 'Marco Biasi', 'Marco RÃ¼egg', 'Jeremy Bolt', 'Jessica Spuehler', 'Denise Aregger', 'Stefan RÃ¼egg', 'Michael Vonarburg', 'Alessandro Grizzetti', 'Francoise Gledhill-Taylor', 'Jeremy Bolt', 'Jessica Spuehler', 'Kurt Wyss', 'Rolf Gutknecht', 'Mike Vogel', 'Walter Tschanen', 'Leandro Schwengeler', 'David De Silva', 'Ufuk SÃ¶nmez', 'Rahel Glanzmann', 'Martin Traxler', 'Gabriele Pellegrino', 'Sptim Zulali', 'Edvard Volmer', 'Michael Trachsler', 'Jessica Spuehler', 'Michael Trachsler', 'Michael Vonarburg', 'Kurt Meili', 'Manuel HÃ¤nni', 'Edy Brueschweiler', 'Daniel Langmeier', 'Cornelis De Vos', 'JÃ¼rgen Kern', 'Patrizia Eberhart', 'Michael Vonarburg', 'Andreas Irminger', 'Kezban Karatas-Koca', 'Pius Furrer', 'Jeremy Bolt', 'Samuel Marti', 'Andreas Mebold', 'Oliver Trummer', 'Brian Molteni', 'Daniel Langmeier', 'Jessica Spuehler', 'Gabriela Notz', 'Edy Brueschweiler', 'Kurt Wyss', 'Kurt Meili', 'Alessandro Grizzetti', 'Helmut Spiegelhalter', 'Marco Aeschimann', 'Andreas Irminger', 'Francoise Gledhill-Taylor', 'JÃ¼rgen Kern', 'Michael Trachsler', 'Pierre Anker', 'Martin Henseler', 'Pius Furrer', 'Fabrice Buser', 'Kezban Karatas-Koca', 'Peter Niederhauser', 'Jessica Spuehler', 'Eleazar Marbach', 'Jeremy Bolt', 'Patrick Caviezel', 'Samuel Marti', 'Kilian GrÃ¤nicher', 'Robin Hassler', 'Franz Koch', 'Daniel Balmer', 'Mirza Alimanovic', 'Roger Marti', 'Andreas Mebold', 'Remo Wettach', 'Dominik HÃ¼ttig', 'Dominik Gubler', 'Roger Haefeli', 'Eleazar Marbach', 'Gilbert Schmid', 'Patrick Caviezel', 'Jeremy Bolt', 'Jessica Spuehler', 'Christine Giacobetti', 'Christopher Closuit', 'Patrick Wydler', 'Patrick Suchet', 'Pierre Anker', 'Claude Brunner', 'Pierre-AndrÃ© Borne', 'Joel Faivre', 'Patrick Zeller', 'Simon Gremaud', 'Fabrice Buser', 'Sorija Sun', 'StÃ©phane Wampfler', 'Gregor RÃ¼egg', 'Sacha Croset', 'Sylvain Chabert', 'Eleazar Marbach', 'Jeremy Bolt', 'Roland Bruggmann', 'Ronny Balmer', 'Marc Schultheiss', 'Reto BÃ¼chel', 'Andreas GÃ¼ttinger', 'Steven Matzinger', 'Jeremy Bolt', 'Eleazar Marbach', 'Jessica Spuehler', 'Christof Brux', 'Edy Brueschweiler', 'Robin Hassler', 'Gilbert Schmid', 'Patrick Caviezel', 'Daniel Langmeier', 'JÃ¼rgen Kern', 'Eleazar Marbach', 'Jeremy Bolt', 'Patrizia Eberhart', 'Eleazar Marbach', 'Francoise Gledhill-Taylor', 'Jessica Spuehler', 'Jeremy Bolt', 'Edy Brueschweiler', 'Karin Martin', 'Robert Camenzind', 'Cornelis De Vos', 'Marcel Volkart', 'Elsbeth Kaegi', 'Eveline Meili', 'Cornelis De Vos', 'Patrizia Eberhart', 'ChengChung Wu', 'Pius Furrer', 'Jessica Spuehler', 'Pierre Anker', 'Simon Gremaud', 'Sorija Sun', 'Jeremy Bolt', 'Eleazar Marbach', 'Jessica Spuehler', 'Christof Brux', 'Manuel HÃ¤nni', 'Patrik Scherrer', 'Helmut Spiegelhalter', 'Marco Aeschimann', 'Eleazar Marbach', 'Jeremy Bolt', 'Patrizia Eberhart', 'Gilbert Schmid', 'Patrick Caviezel', 'Patrizia Eberhart', 'Peter Niederhauser', 'Jessica Spuehler', 'Atilla Bagci', 'Steven Matzinger', 'Eleazar Marbach', 'Jeremy Bolt', 'Patrizia Eberhart', 'Andreas Irminger', 'Jessica Spuehler', 'Kezban Karatas-Koca', 'Ronny Balmer', 'Christoph Peter', 'Francesco Paradiso', 'Pascal Bass', 'Nadja Pfister', 'Monica Stoop', 'Marco Biasi', 'Marco RÃ¼egg', 'StÃ©phane Wampfler', 'Gregor RÃ¼egg', 'Elif Kokolar', 'Robin Hassler', 'Pierre Anker', 'Claude Brunner', 'Jeremy Bolt', 'Robin Hassler', 'Jean-Pierre Eugler', 'JÃ¼rgen Kern', 'Roland Stamm', 'Pierre Anker', 'Martin Henseler', 'Pius Furrer', 'Doris Roth', 'Jessica Spuehler', 'Doris Roth', 'Eleazar Marbach', 'Jeremy Bolt', 'Edy Brueschweiler', 'Helmut Spiegelhalter', 'Marco Aeschimann', 'Andreas Irminger', 'Patrizia Eberhart', 'Jessica Spuehler', 'Michael Trachsler', 'Kezban Karatas-Koca', 'Robin Hassler', 'Gilbert Schmid', 'Patrick Caviezel', 'Christof Brux', 'Manuel HÃ¤nni', 'Parwaneh Rajabi', 'Patrik Scherrer', 'Atilla Bagci', 'JÃ¼rgen Kern', 'Jessica Spuehler', 'Daniel Rellstab', 'Edy Brueschweiler', 'Daniel Langmeier', 'Kurt Meili', 'Helmut Spiegelhalter', 'Manuel HÃ¤nni', 'Gabriela Notz', 'Simon Ganz', 'Michael Trachsler', 'Elsbeth Kaegi', 'Martin Henseler', 'Kezban Karatas-Koca', 'Jeremy Bolt', 'Jessica Spuehler', 'Gabriela Notz', 'Elsbeth Kaegi', 'Jeremy Bolt', 'Pius Furrer', 'Robin Hassler', 'Oliver Trummer', 'Fatmir Shoshi', 'Pascal Knechtenhofer', 'Francesco Racinelli', 'Jessica Spuehler', 'Alessandro Grizzetti', 'Atilla Bagci', 'Fritz Diebold', 'Patrik Scherrer', 'Alessandro Grizzetti', 'Patrik Scherrer', 'Edy Brueschweiler', 'Cornelis De Vos', 'Marco Aeschimann', 'Michael Trachsler', 'Daniel Rellstab', 'Roland Bruggmann', 'Kurt Meili', 'Christoph Peter', 'Marc Schultheiss', 'Jeremy Bolt', 'Eleazar Marbach', 'Cornelis De Vos', 'Eleazar Marbach', 'Jeremy Bolt', 'Gilbert Schmid', 'Patrick Caviezel', 'Jessica Spuehler', 'Steven Matzinger', 'Atilla Bagci', 'Daniel Langmeier', 'Jessica Spuehler', 'Gabriela Notz', 'Kurt Wyss', 'Robert Camenzind', 'Helmut Spiegelhalter', 'Andreas Irminger', 'Francoise Gledhill-Taylor', 'JÃ¼rgen Kern', 'Michael Trachsler', 'Martin Henseler', 'Kezban Karatas-Koca', 'Jeremy Bolt', 'Kurt Wyss', 'Eleazar Marbach', 'Jeremy Bolt', 'Jessica Spuehler', 'Robin Hassler', 'Pierre Anker', 'Patrick Zeller', 'Simon Gremaud', 'Sacha Croset', 'Sylvain Chabert', 'Jeremy Bolt', 'Jeremy Bolt', 'Robin Hassler', 'Helmut Spiegelhalter', 'CH-RPA-Account', 'Eleazar Marbach', 'Edy Brueschweiler', 'Jessica Spuehler', 'Karin Martin', 'Robert Camenzind', 'Cornelis De Vos', 'Diego SchlÃ¼ssel', 'Elsbeth Kaegi', 'Eveline Meili', 'Patrizia Eberhart', 'ChengChung Wu', 'Michael Vonarburg', 'Jessica Spuehler', 'Kurt Meili', 'Michael Trachsler', 'Jeremy Bolt', 'Peter Niederhauser', 'Robin Hassler', 'Pius Furrer', 'Marco Bertozzi', 'Sergio Nuzzo', 'Jeremy Bolt', 'Jessica Spuehler', 'Robin Hassler', 'Patrick Wydler', 'Pierre Anker', 'Joel Faivre', 'Patrick Zeller', 'Sorija Sun', 'Sylvain Chabert', 'Jerome Chindamo']</t>
+  </si>
+  <si>
+    <t>['Shaun Buchanan', 'Martin Summerville', 'John Irwin', 'Shaun Buchanan', 'Shaun Buchanan', 'Rory Geoghegan', 'Martin Summerville', 'Stephen Finneran', 'Martin Noonan', 'John Irwin', 'Damien Pender', 'Martin Summerville', 'Shaun Buchanan', 'Rory Geoghegan', 'Martin Summerville', 'Martin Noonan', 'Martin Summerville', 'Shaun Buchanan', 'Shaun Buchanan', 'Orla Rowse', 'Orla Rowse', 'Martin Summerville', 'Orla Rowse', 'Orla Rowse', 'Shaun Buchanan', 'Shaun Buchanan', 'Damien Pender', 'Shaun Buchanan', 'Shaun Buchanan', 'Martin Summerville', 'John Irwin', 'Rory Geoghegan', 'Shaun Buchanan', 'Rory Geoghegan', 'Orla Rowse', 'Martin Summerville', 'Stephen Finneran', 'Martin Noonan', 'John Irwin', 'Damien Pender', 'Shaun Buchanan', 'Martin Summerville', 'Orla Rowse', 'Shaun Buchanan', 'Martin Summerville', 'Damien Pender', 'Shaun Buchanan', 'Shaun Buchanan', 'IE-Mailbox Warehouse']</t>
+  </si>
+  <si>
+    <t>['Mark Eivers', 'Mark Eivers', "Stephen O'Neill", 'Martin Gilligan', 'John Donohoe', 'Barry McDermott', "Stephen O'Neill", 'Martin Gilligan', 'John Donohoe', 'Barry McDermott', 'Martin Walsh', 'William Joyce', "PJ O'Neill", 'Pablo Fernandez', 'Paul Murphy', "Stephen O'Neill", 'Martin Gilligan', 'John Donohoe', 'Barry McDermott', 'William Joyce', 'Mark Eivers', 'Martin Gilligan', "Stephen O'Neill", 'John Donohoe', "Stephen O'Neill", 'Barry McDermott', 'John Donohoe', 'Pablo Fernandez', 'Mark Eivers', 'Paul Murphy', 'Mark Eivers', 'Fintan Byrne', 'Martin Gilligan', 'Mark Eivers', "Stephen O'Neill", 'Mark Eivers', "Stephen O'Neill", 'John Donohoe', "Stephen O'Neill", "Stephen O'Neill", 'Mark Eivers', "Stephen O'Neill", "Stephen O'Neill", 'Martin Gilligan', 'William Joyce', "Stephen O'Neill", 'John Donohoe', 'Mark Eivers', 'John Donohoe', "Stephen O'Neill", 'Barry McDermott', 'Martin Gilligan', 'John Donohoe', 'Paul Murphy', "Stephen O'Neill", "Stephen O'Neill", 'John Donohoe', 'Barry McDermott', 'Mark Eivers', 'Keith Brennan', 'Martin Gilligan', 'Shauna Buchanan', 'Anthony Walsh', 'Joseph Browne', 'Martin Walsh', 'William Joyce', "PJ O'Neill", 'Fintan Byrne', 'Pablo Fernandez', 'Paul Murphy', 'Dylan Maher', 'Christian Byrne', "Stephen O'Neill", "Stephen O'Neill", 'John Donohoe', 'Keith Brennan', 'Shauna Buchanan', 'Anthony Walsh', 'Joseph Browne', "Stephen O'Neill", 'John Donohoe', "Stephen O'Neill", 'Martin Gilligan', 'John Donohoe', "Stephen O'Neill", 'Mark Eivers', "Stephen O'Neill", 'Martin Gilligan', 'John Donohoe', 'Paul Murphy', "Stephen O'Neill", 'Keith Brennan', 'Shauna Buchanan', 'Anthony Walsh', 'Joseph Browne', "Stephen O'Neill", 'John Donohoe', 'Dylan Maher', 'Christian Byrne', "Stephen O'Neill"]</t>
+  </si>
+  <si>
+    <t>['Goran Oberg', 'Goran Oberg', 'Chris Santos', 'Goran Oberg', 'Michael Loggins', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Michael Loggins', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Jon St.Arnaud', 'Marc Doades', 'Goran Oberg', 'Goran Oberg', 'Michael Loggins', 'Goran Oberg', 'Goran Oberg', 'Michael Loggins', 'Jon St.Arnaud', 'Marc Doades', 'Chris Santos', 'Michael Loggins', 'Goran Oberg', 'Goran Oberg', 'Michael Loggins', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Goran Oberg', 'Marc Doades', 'Goran Oberg', 'Goran Oberg']</t>
+  </si>
+  <si>
+    <t>['Chevalier Olivier', 'Pinto Philippe', 'Beringue Nicolas', 'Baumert Robert', 'Legeard Arnaud', 'Beringue Nicolas', 'ClÃ©rin RÃ©mi', 'Imamura Shogo', 'Orny Marc Olivier', 'Delsaux Axel', 'Caron Julien', 'Strohl Mathieu', 'Le Provost Philippe', 'Georget SÃ©bastien', 'Helfer Denis', 'Belkacem Karim', 'Rita Massimo', 'Chevalier Olivier', 'Royal Vincent', 'Berthelot Laure', 'Bauer Alexandre', 'Aumard Lucie', 'Belkacem Karim', 'Delauge Francois', 'Beringue Nicolas', 'Orny Marc Olivier', 'Stahn Richard', 'Laine MickaÃ«l', 'Hauptmann Michael', 'Lemacon Max', 'Ploton Laurent', 'Forest GaÃ«tan', 'Rastel Nicolas', 'Sonvico Jacques', 'Tomasi CÃ©dric', 'Lemoine CÃ©dric', 'Montaclair Luc', 'Ledermann Jonathan', 'Bellet Nicolas', 'Francois VÃ©ronique', 'Rita Massimo', 'Haouzi Ashley', 'Pinto Philippe', 'Beringue Nicolas', 'Chanteloup Willy', 'ClÃ©rin RÃ©mi', 'Stoykoff Jean Denis', 'Baumert Robert', 'Perraud Vincent', 'Kadmi Zouhair', 'Le Cam Brice', 'Legeard Arnaud', 'Subtil Bruno', 'Lohisse Marc', 'Beringue Nicolas', 'Chanteloup Willy', 'ClÃ©rin RÃ©mi', 'Stoykoff Jean Denis', 'Baumert Robert', 'Duvernet Jean Denis', 'Le Cam Brice', 'Legeard Arnaud', 'Dazin Patrice', 'Nollet Anthony', 'Michard StÃ©phane', 'Gree SÃ©bastien', 'Usquelis Arnaud', 'Maraval BenoÃ®t', 'Bertrand Julie', 'Redon JÃ©rÃ©my', 'Michard StÃ©phane', 'Vanderriele Laetitia', 'Roumejon Loic', 'Goutherot GrÃ©gory', 'Mansau Philippe', 'Braley StÃ©phane', 'Hienne Eric', 'Rault Claude', 'Raymond Denis', 'Courtois Karine', 'Bauer Alexandre', 'Delsaux Axel', 'Delauge Francois', 'Anousone Sukhaseum', 'Belkacem Karim', 'Helfer Denis', 'Haouzi Ashley', 'Lalorcey GÃ©rald', 'Bauer Alexandre', 'Duroure Francis', 'Veret Nicolas', 'Delsaux Axel', 'Pellizzari Alexandre', 'Lemoine CÃ©dric', 'Laniel Christophe', 'Lafay Martial', 'Bucchi StÃ©phane', 'Richet Fabienne', 'Ledermann Jonathan', 'Buron Nicolas', 'Orny Marc Olivier', 'Corbiere Antoine', 'Perraud Vincent', 'Dubard CÃ©cile', 'Orjollet Claude', 'Brugerolle Guillaume', 'Andres Corentin', 'Ferrieres Pascal', 'Joly Christophe', 'Bento Susana', 'Pinto Philippe', 'Lemacon Max', 'Bozzini Florie', 'Orny Marc Olivier', 'Helfer Denis', 'Bauer Alexandre', 'Duroure Francis', 'Lang FrÃ©dÃ©ric', 'Pajot FrÃ©dÃ©ric', 'Germain Bruno', 'Audiot Julien', 'Salami Bruno', 'Lohisse Marc', 'Perraud Vincent', 'Pouplier Patrice', 'Wiss SÃ©bastien', 'Boireau Sylvain', 'Berthelot Laure', 'Potard Yannick', 'Letellier Steevy', 'Edeline Franck', 'Bauer Alexandre', 'Pinto Philippe', 'Hauptmann Michael', 'Ploton Laurent', 'Ladant Sophie', 'Stahn Richard', 'Beaucourt Nicolas', 'Briatte Bruno', 'Lemoine CÃ©dric', 'Compte Patrice', 'Taouri Youness', 'Jouret Gilles', 'Faleix Julien', 'Neto Georges', 'Mazzola Serge', 'Pierrel Patrick', 'Basuyau Pauline', 'Marchal Jean-Philippe', 'Haouzi Ashley', 'Beringue Nicolas', 'Chanteloup Willy', 'ClÃ©rin RÃ©mi', 'Stoykoff Jean Denis', 'Baumert Robert', 'Thebault William', 'Gaudron Alexis', 'Aze SÃ©bastien', 'Douay Alexis', 'Legeard Arnaud', 'Loget Emmanuelle', 'Orny Marc Olivier', 'Bauer Alexandre', 'Salami Bruno', 'Berthelot Laure', 'Bozzini Florie', 'Loget Emmanuelle', 'Bauer Alexandre', 'Chevalier Olivier', 'Perraud Vincent', 'Royal Vincent', 'Belkacem Karim', 'Delauge Francois', 'Legeard Arnaud', 'Hauptmann Michael', 'Amable Franck', 'Gouin Sophie', 'Orny Monique', 'Briatte Bruno', 'Duroure Francis', 'Gubiani Marco', 'Gregorio Patrice', 'Gruat FrÃ©dÃ©ric', 'Thebault William', 'Lang FrÃ©dÃ©ric', 'Nemoz-Billet Fabien', 'Landrault Thierry', 'Gaudron Alexis', 'Ploton Laurent', 'Veret Nicolas', 'Dias StÃ©phane', 'Forest GaÃ«tan', 'Mansau Philippe', 'Pajot FrÃ©dÃ©ric', 'Briantais Laurent', 'Aumard Lucie', 'Goutherot GrÃ©gory', 'Braley StÃ©phane', 'Douay Alexis', 'Delavier Alexis', 'Salami Bruno', 'Beringue Nicolas', 'Potard Yannick', 'Orny Marc Olivier', 'Delsaux Axel', 'Brugerolle Guillaume', 'Caron Julien', 'Beck Vanessa', 'Lebert Claudine', 'Strohl Mathieu', 'Jamet Pascal', 'Charette Olivier', 'Ocal Aydovan', 'Leclercq Pierre', 'Grelot Christelle', 'Duvernet Jean Denis', 'Dubard CÃ©cile', 'Ferrieres Pascal', 'Pellizzari Alexandre', 'Le Provost Philippe', 'Ladant Sophie', 'Puccinelli Ludovic', 'Georget SÃ©bastien', 'Bicheray StÃ©phane', 'Rault Claude', 'Moal Thierry', 'Lemoine CÃ©dric', 'Griotier Cyril', 'Edeline Franck', 'Joly Christophe', 'ClÃ©rin RÃ©mi', 'Laniel Christophe', 'Le Cam Brice', 'Courtois Karine', 'Lenoir CÃ©dric', 'Damien Eddy', 'Lafay Martial', 'Montaclair Luc', 'Jacquinot Vincent', 'Bucchi StÃ©phane', 'Maraval BenoÃ®t', 'Richet Fabienne', 'Mezange Dominique', 'Peeters Christophe', 'Ledermann Jonathan', 'Mazzola Serge', 'Michard StÃ©phane', 'Helfer Denis', 'Reux Adrien', 'Bellet Nicolas', 'Blayo Sylvie', 'Elise Christopher', 'Buron Nicolas', 'Subtil Bruno', 'Chambon Laura', 'Ducreux StÃ©phane', 'Guttin SÃ©bastien', 'Bordas Julia', 'Ait Boufousse Mariama', 'Sirier AmÃ©lie', 'Tolle Sofia', 'Orny Marc Olivier', 'Delsaux Axel', 'Helfer Denis', 'Delauge Francois', 'Loget Emmanuelle', 'Legeard Arnaud', 'Michard StÃ©phane', 'Bauer Alexandre', 'Berthelot Laure', 'Anousone Sukhaseum', 'Loget Emmanuelle', 'Laine MickaÃ«l', 'Hauptmann Michael', 'Orny Monique', 'Lemacon Max', 'Dazin Patrice', 'Briatte Bruno', 'Duroure Francis', 'Gubiani Marco', 'Gregorio Patrice', 'Compte Patrice', 'Gruat FrÃ©dÃ©ric', 'Thebault William', 'Drancourt FrÃ©dÃ©ric', 'Garcia William', 'Veyreveze Karine', 'Lang FrÃ©dÃ©ric', 'Nemoz-Billet Fabien', 'Egea Jordy', 'Muller Emmanuel', 'Letellier Steevy', 'Landrault Thierry', 'Gaudron Alexis', 'Ploton Laurent', 'Veret Nicolas', 'BrulÃ© Damien', 'Dias StÃ©phane', 'Forest GaÃ«tan', 'Aze SÃ©bastien', 'Mansau Philippe', 'Pajot FrÃ©dÃ©ric', 'Germain Bruno', 'Allard RÃ©gis', 'Briantais Laurent', 'David GaÃ«tan', 'Audiot Julien', 'Mainot SÃ©bastien', 'Aumard Lucie', 'Goutherot GrÃ©gory', 'Braley StÃ©phane', 'Taouri Youness', 'Douay Alexis', 'Delavier Alexis', 'Bertrand Julie', 'Salami Bruno', 'Beringue Nicolas', 'Chevalier Olivier', 'Jourdain Emmanuel', 'Potard Yannick', 'Orny Marc Olivier', 'Delsaux Axel', 'Ribeiro Olinda', 'Fouquet ValÃ©rie', 'Caron Julien', 'Lametairie Patricia', 'Arenillas SÃ©bastien', 'Seiller BÃ©atrice', 'Beck Vanessa', 'Calmels Christophe', 'Zana Sue Ellen', 'Deronne Marion', 'Lebert Claudine', 'Tonnelier Sophie', 'Bezard ValÃ©rie', 'Strohl Mathieu', 'Jouret Gilles', 'Charette Olivier', 'Coudan Jean Christophe', 'Ocal Aydovan', 'Lohisse Marc', 'Delobel Christophe', 'Leclercq Pierre', 'Nollet Anthony', 'Chanteloup Willy', 'Duvernet Jean Denis', 'Pereira Cristina', 'Rastel Nicolas', 'Rollet Didier', 'Pereira MÃ©lissa', 'Perraud Vincent', 'Pouplier Patrice', 'Royal Vincent', 'Dumas Pauline', 'Belkacem Karim', 'Pellizzari Alexandre', 'Sonvico Jacques', 'Lima Christophe', 'Le Provost Philippe', 'Lefrere Emmanuel', 'Ladant Sophie', 'Vrancic Isabelle', 'Georget SÃ©bastien', 'Bicheray StÃ©phane', 'Kadmi Zouhair', 'Tomasi CÃ©dric', 'Faleix Julien', 'Godard Pierrick', 'Moal Thierry', 'Lemoine CÃ©dric', 'Griotier Cyril', 'Edeline Franck', 'Maczenko CÃ©dric', 'ClÃ©rin RÃ©mi', 'Laniel Christophe', 'Le Cam Brice', 'Moura Patrick', 'Duez Thomas', 'Lenoir CÃ©dric', 'Friocourt Anthony', 'Delauge Francois', 'Noel Jean FranÃ§ois', 'Lafay Martial', 'Pagni Sophie', 'Montaclair Luc', 'Jacquinot Vincent', 'Bucchi StÃ©phane', 'Maraval BenoÃ®t', 'Neto Georges', 'Garcia Ballester Nicolas', 'Legeard Arnaud', 'Redon JÃ©rÃ©my', 'Richet Fabienne', 'Mezange Dominique', 'Zabka Patrick', 'Peeters Christophe', 'Levy HervÃ©', 'Ledermann Jonathan', 'Mazzola Serge', 'Michard StÃ©phane', 'Tiercelin Olivier', 'Rita Massimo', 'Imbert Caroline', 'Russo Florian', 'Stahn Richard', 'Helfer Denis', 'Pierrel Patrick', 'Reux Adrien', 'Bellet Nicolas', 'Abdi Nacer', 'Elise Christopher', 'Marcucci Anthony', 'Buron Nicolas', 'Subtil Bruno', 'Nollet Guillaume', 'Ducreux StÃ©phane', 'Scrofani Laura', 'Klein Thibault', 'Guttin SÃ©bastien', 'Karoui Emir', 'Basuyau Pauline', 'Beaucourt Nicolas', 'Hatterer Nicolas', 'Gree SÃ©bastien', 'Bordas Julia', 'Amphoux Lionel', 'Lalorcey GÃ©rald', 'Marchal Jean-Philippe', 'Wiss SÃ©bastien', 'Boireau Sylvain', 'Vanderriele Laetitia', 'Stoykoff Jean Denis', 'Bernard AurÃ©lie', 'Braud SÃ©bastien', 'Crey Rodolphe', 'Florentine Manuella', 'Moscone Franco', 'Baumert Robert', 'Jeannin Christophe', 'Baudry Nathalie', 'Harivel David', 'Usquelis Arnaud', 'Ghabri Marouane', 'Jolivet Bruno', 'Bouzid Firas', 'Imamura Shogo', 'Dell Flavien', 'Denis Jean-Charles', 'Guillot Claire', 'Le Mab Mathieu', 'Roumejon Loic', 'Ledermann Jonathan', 'Dias StÃ©phane', 'Mainot SÃ©bastien', 'Veret Nicolas', 'Lenoir CÃ©dric', 'Laine MickaÃ«l', 'Duez Thomas', 'Neto Georges', 'Mazzola Serge', 'Basuyau Pauline', 'Chevalier Olivier', 'Delauge Francois', 'Egea Jordy', 'Allard RÃ©gis', 'Faleix Julien', 'Moura Patrick', 'Russo Florian', 'Guillot Claire', 'Garcia Ballester Nicolas', 'Ducreux StÃ©phane', 'Berthelot Laure', 'Chevalier Olivier', 'Loget Emmanuelle', 'Bauer Alexandre', 'Perraud Vincent', 'Belkacem Karim', 'Delauge Francois', 'Legeard Arnaud', 'Rita Massimo', 'Moal Thierry', 'Nemoz-Billet Fabien', 'Egea Jordy', 'Calmels Christophe', 'Jouret Gilles', 'Coudan Jean Christophe', 'Delobel Christophe', 'Russo Florian', 'Forest GaÃ«tan', 'Garcia William', 'Letellier Steevy', 'Landrault Thierry', 'Germain Bruno', 'David GaÃ«tan', 'Potard Yannick', 'Jouret Gilles', 'Rastel Nicolas', 'Pouplier Patrice', 'Bicheray StÃ©phane', 'Godard Pierrick', 'Edeline Franck', 'Friocourt Anthony', 'Boireau Sylvain', 'Le Mab Mathieu', 'Michard StÃ©phane', 'Dazin Patrice', 'Garcia William', 'Letellier Steevy', 'Landrault Thierry', 'BrulÃ© Damien', 'Forest GaÃ«tan', 'Briantais Laurent', 'David GaÃ«tan', 'Delavier Alexis', 'Bertrand Julie', 'Potard Yannick', 'Nollet Anthony', 'Rastel Nicolas', 'Bicheray StÃ©phane', 'Godard Pierrick', 'Edeline Franck', 'Friocourt Anthony', 'Maraval BenoÃ®t', 'Redon JÃ©rÃ©my', 'Elise Christopher', 'Buron Nicolas', 'Gree SÃ©bastien', 'Bordas Julia', 'Vanderriele Laetitia', 'Usquelis Arnaud', 'Perraud Vincent', 'Chevalier Olivier', 'Ledermann Jonathan', 'Ploton Laurent', 'Veret Nicolas', 'Forest GaÃ«tan', 'Delauge Francois', 'Peeters Christophe', 'Michard StÃ©phane', 'Belkacem Karim', 'Rita Massimo', 'Lemoine CÃ©dric', 'Bauer Alexandre', 'Chevalier Olivier', 'Helfer Denis', 'Dias StÃ©phane', 'Imbert Caroline', 'Moscone Franco', 'Veret Nicolas', 'Duez Thomas', 'Lenoir CÃ©dric', 'Crey Rodolphe', 'Noel Jean FranÃ§ois', 'Loget Emmanuelle', 'David GaÃ«tan', 'Pagni Sophie', 'Ledermann Jonathan', 'Helfer Denis', 'Francois VÃ©ronique', 'Bauer Alexandre', 'Loget Emmanuelle', 'Lefrere Emmanuel', 'Mezange Dominique', 'Beringue Nicolas', 'Stoykoff Jean Denis', 'Lima Christophe', 'ClÃ©rin RÃ©mi', 'Le Cam Brice', 'Maraval BenoÃ®t', 'Legeard Arnaud', 'Subtil Bruno', 'Baumert Robert', 'Imamura Shogo', 'Francois VÃ©ronique', 'Ploton Laurent', 'Hauptmann Michael', 'Lafay Martial', 'Garcia Ballester Nicolas', 'Chevalier Olivier', 'Pinto Philippe', 'Mainot SÃ©bastien', 'Drancourt FrÃ©dÃ©ric', 'Ploton Laurent', 'Forest GaÃ«tan', 'Calmels Christophe', 'Leclercq Pierre', 'Ladant Sophie', 'Godard Pierrick', 'Garcia Ballester Nicolas', 'Ledermann Jonathan', 'Mazzola Serge', 'Marcucci Anthony', 'Ducreux StÃ©phane', 'Gree SÃ©bastien', 'Bordas Julia', 'Harivel David', 'Ploton Laurent', 'Ledermann Jonathan', 'Forest GaÃ«tan', 'Caron Julien', 'Strohl Mathieu', 'Perraud Vincent', 'Gregorio Patrice', 'Jacquinot Vincent', 'Reux Adrien', 'Abdi Nacer', 'Klein Thibault', 'Karoui Emir', 'Jeannin Christophe', 'Bauer Alexandre', 'Chevalier Olivier', 'Laniel Christophe', 'Ledermann Jonathan', 'Briatte Bruno', 'Rollet Didier', 'Pellizzari Alexandre', 'Bauer Alexandre', 'Laniel Christophe', 'Ledermann Jonathan', 'Berthelot Laure', 'Dias StÃ©phane', 'Forest GaÃ«tan', 'Orny Marc Olivier', 'Delsaux Axel', 'Bicheray StÃ©phane', 'Damien Eddy', 'Ducreux StÃ©phane', 'Pinto Philippe', 'Forest GaÃ«tan', 'David GaÃ«tan', 'Rastel Nicolas', 'Bicheray StÃ©phane', 'Helfer Denis', 'Bozzini Florie', 'Haouzi Ashley', 'Belkacem Karim', 'Legeard Arnaud', 'Lemacon Max', 'Beringue Nicolas', 'Lemoine CÃ©dric', 'ClÃ©rin RÃ©mi', 'Stoykoff Jean Denis', 'Bauer Alexandre', 'Orny Marc Olivier', 'Francois VÃ©ronique', 'Haouzi Ashley', 'Belkacem Karim', 'Orny Marc Olivier', 'Lemacon Max', 'Duroure Francis', 'Beringue Nicolas', 'Caron Julien', 'Perraud Vincent', 'Dubard CÃ©cile', 'Le Provost Philippe', 'Kadmi Zouhair', 'Lemoine CÃ©dric', 'Arenillas SÃ©bastien', 'Abdelbaki Malik', 'Ledermann Jonathan', 'Drancourt FrÃ©dÃ©ric', 'Dias StÃ©phane', 'Mainot SÃ©bastien', 'Imbert Caroline', 'Nollet Guillaume', 'Moscone Franco', 'Harivel David', 'Lemacon Max', 'Arenillas SÃ©bastien', 'Legeard Arnaud', 'Landrault Thierry', 'Laniel Christophe', 'Taouri Youness', 'Monseux GrÃ©gory', 'Royal Vincent', 'Griotier Cyril', 'Zabka Patrick', 'Hama Alaa', 'Ghabri Marouane', 'Bouzid Firas', 'Berthelot Laure', 'Helfer Denis', 'Loget Emmanuelle', 'Helfer Denis', 'Comparot Christophe', 'Berthelot Laure', 'Anousone Sukhaseum', 'Shaik Madarsa Mouhamad', 'Torti Thomas', 'Garcia Ballester Nicolas', 'Taouri Youness', 'Comparot Christophe', 'Francois VÃ©ronique', 'Helfer Denis', 'Haouzi Ashley', 'Duroure Francis', 'Gaudron Alexis', 'Charette Olivier', 'Le Provost Philippe', 'Lemoine CÃ©dric', 'Bento Susana', 'Loget Emmanuelle', 'Orny Marc Olivier', 'Caron Julien', 'Loget Emmanuelle', 'Bucchi StÃ©phane', 'Bauer Alexandre', 'Gubiani Marco', 'Gruat FrÃ©dÃ©ric', 'Egea Jordy', 'Briantais Laurent', 'Calmels Christophe', 'Ocal Aydovan', 'Duez Thomas', 'Amphoux Lionel', 'Vanderriele Laetitia', 'Mainot SÃ©bastien', 'Drancourt FrÃ©dÃ©ric', 'Nollet Guillaume', 'Harivel David', 'Jourdain Emmanuel', 'Belkacem Karim', 'Haouzi Ashley', 'Loget Emmanuelle', 'Orny Marc Olivier', 'Beringue Nicolas', 'Chanteloup Willy', 'ClÃ©rin RÃ©mi', 'Stoykoff Jean Denis', 'Baumert Robert', 'Thebault William', 'Gaudron Alexis', 'Legeard Arnaud', 'Comparot Christophe', 'Berthelot Laure', 'Helfer Denis', 'Anousone Sukhaseum', 'Shaik Madarsa Mouhamad', 'Orny Marc Olivier', 'Berthelot Laure', 'Orny Monique', 'Chevalier Olivier', 'Laniel Christophe', 'Ledermann Jonathan', 'Berthelot Laure', 'Bauer Alexandre', 'Duroure Francis', 'Lang FrÃ©dÃ©ric', 'Orny Marc Olivier', 'Rollet Didier', 'Moal Thierry', 'Jacquinot Vincent', 'Bucchi StÃ©phane', 'Berthelot Laure', 'Sirier AmÃ©lie', 'Jourdain Emmanuel', 'Puccinelli Ludovic', 'Lafay Martial', 'Tomasi CÃ©dric', 'Levy HervÃ©', 'Bellet Nicolas', 'Marcucci Anthony', 'Goutherot GrÃ©gory', 'Hienne Eric', 'Audiot Julien', 'Lefrere Emmanuel', 'Raymond Denis', 'Damien Eddy', 'Mezange Dominique', 'Boireau Sylvain', 'Buron Nicolas', 'BrulÃ© Damien', 'Delavier Alexis', 'Elise Christopher', 'Bordas Julia', 'Lemacon Max', 'Arenillas SÃ©bastien', 'Abdelbaki Malik', 'Seiler Sidney', "D'Angelo Thierry", 'Chevalier Olivier', 'Lemacon Max', 'Muller Emmanuel', 'Arenillas SÃ©bastien', 'Rollet Didier', 'Maczenko CÃ©dric', 'Bauer Alexandre', 'Helfer Denis', 'Ledermann Jonathan', 'Belkacem Karim', 'Lemacon Max', 'Maczenko CÃ©dric', 'Legeard Arnaud', 'Pinto Philippe', 'Loget Emmanuelle', 'Deronne Marion', 'Belkacem Karim', 'Rita Massimo', 'Haouzi Ashley', 'Veret Nicolas', 'Crey Rodolphe', 'Compte Patrice', 'Duez Thomas', 'Tiercelin Olivier', 'Landrault Thierry', 'Garcia William', 'Letellier Steevy', 'Ploton Laurent', 'Forest GaÃ«tan', 'Potard Yannick', 'Leclercq Pierre', 'Sonvico Jacques', 'Ladant Sophie', 'Bicheray StÃ©phane', 'Godard Pierrick', 'Lemoine CÃ©dric', 'Levy HervÃ©', 'Ledermann Jonathan', 'Imbert Caroline', 'Stahn Richard', 'Bellet Nicolas', 'Marcucci Anthony', 'Hatterer Nicolas', 'Harivel David', 'Puccinelli Ludovic', 'Peyrouse Laurent', 'Ouriemmi salim', 'Robardelle Sylvain', 'Amable Franck', 'Mdiouani Abdelaziz', 'Fornage FrÃ©dÃ©ric', 'Rault Claude', 'Georget SÃ©bastien', 'Richet Fabienne', 'Rodrigues Pina Tony', 'Laine MickaÃ«l', 'Amable Franck', 'Braley StÃ©phane', 'Potard Yannick', 'Delsaux Axel', 'Fouquet ValÃ©rie', 'Ocal Aydovan', 'Griotier Cyril', 'Raymond Denis', 'Joly Christophe', 'ClÃ©rin RÃ©mi', 'Jacquinot Vincent', 'Ronchi Paolo', 'Imbert Caroline', 'Peeters Christophe', 'Hauptmann Michael', 'Allard RÃ©gis', 'Ladant Sophie', 'Moura Patrick', 'Noel Jean FranÃ§ois', 'Stahn Richard', 'Pierrel Patrick', 'Beaucourt Nicolas', 'Amphoux Lionel', 'Marchal Jean-Philippe', 'Wiss SÃ©bastien', 'Chanteloup Willy', 'Laine MickaÃ«l', 'Compte Patrice', 'Nemoz-Billet Fabien', 'BrulÃ© Damien', 'Briantais Laurent', 'Delavier Alexis', 'Beringue Nicolas', 'Calmels Christophe', 'Tiercelin Olivier', 'Elise Christopher', 'Buron Nicolas', 'Bordas Julia', 'Usquelis Arnaud', 'Beringue Nicolas', 'Chanteloup Willy', 'ClÃ©rin RÃ©mi', 'Stoykoff Jean Denis', 'Baumert Robert', 'Thebault William', 'Gaudron Alexis', 'Aze SÃ©bastien', 'Douay Alexis', 'Duvernet Jean Denis', 'Lima Christophe', 'Le Cam Brice', 'Legeard Arnaud', 'Subtil Bruno', 'Imamura Shogo', 'Belkacem Karim', 'Puccinelli Ludovic', 'Peyrouse Laurent', 'Amable Franck', 'Lemacon Max', 'Jourdain Emmanuel', 'Orjollet Claude', 'Corbiere Antoine', 'Perraud Vincent', 'Mdiouani Abdelaziz', 'Dubard CÃ©cile', 'Belkacem Karim', 'Ferrieres Pascal', 'Fornage FrÃ©dÃ©ric', 'Uruthirakumaran Ananthu', 'Sirier AmÃ©lie']</t>
+  </si>
+  <si>
+    <t>['Ralf Laber', 'Fabian Strodl', 'Ralph Kabitzke', 'Ralf Laber', 'Heiko Hestermann', 'Norbert Hertel', 'Viola Jost', 'Stephanie Tschunt', 'Stephanie Kirchner', 'Oliver Keil', 'Matthias Kern', 'Torsten Lamparter', 'Rainer Schroeder', 'Stephan Johann', 'Dominik Heck', 'Christian Haastert', 'Harald Kuehne', 'Tobias Hartherz', 'Klaus Brinkmann', 'Michael Becker', 'Olaf Hagelstein', 'Michael Losert', 'Kim Holy', 'Gen Uchimido', 'Ulrich Lampen', 'Kristina Schatz', 'Irina Hermann', 'Lisa Meerheim', 'Olaf Hagelstein', 'Bulut Karabulut', 'Stephan Huebner', 'Klaus Koop', 'Steffen Tewes', 'Timo Eberle', 'Nils Boy', 'Ulrich Lampen', 'Irina Hermann', 'Martina Hinkel', 'Roland Kraemer', 'Helge Bunk', 'Michael Below', 'David Blasek', 'Peter Schaefer', 'Peter Stang', 'Ute Schroeder', 'Daniel Dittmann', 'Stephan Johann', 'Yoko Igarashi', 'Christoph Gote', 'Christian von der Hoya', 'Emanuel Stuebner', 'Pascal Dupuy', 'Tim Trellenberg', 'Eva-Maria Perez-Gonzalez', 'Torsten Lamparter', 'Marcel Geisen', 'Martin Knoess', 'Bjoern Mittenzwei', 'Jonas Hohmann', 'Hung Nguyen-Thanh', 'Jan Mennerich', 'Peter Stang', 'Angelika Frittmann', 'Matthias Menge', 'Nicolas-Eric Lamm', 'Sylvia Borchers', 'Kadira Merdzic', 'Pascal Borusiak', 'Axel Teichgraeber', 'Bernd Lede', 'Nico Bernhardt', 'Rolf-Eric Matthies', 'Juan Bueno', 'Christoph Gote', 'Markus Prokopp', 'Emanuel Stuebner', 'Pascal Dupuy', 'Thorsten Rasch', 'Tim Trellenberg', 'Alexander Ochs', 'Christian Bauer', 'Felix Rossmann', 'Andreas Egelseder', 'Viktor Wulfert', 'Arno Neumann', 'Azubi Customer Services', 'Joerg Honka', 'Vincenzo Addison', 'Thomas Walther', 'Marius Bueger', 'Bernd Walter', 'Samuel Groh', 'Michael Kretzschmar', 'Anna Graf', 'Monika Metz', 'Marco Gruber', 'Marius Diem', 'Claudia Wenchel', 'Markus Witte', 'Sabrina Kranz', 'Jan Hanse', 'Mirko Ganz', 'Nikolaj Krez', 'Irina Kistner', 'Marcel Ploesser', 'Jens Heppert', 'Thorsten Winter', 'Sylvia Borchers', 'Lukasz Krol', 'Kadira Merdzic', 'Peter Schaefer', 'Pascal Borusiak', 'Gabriele Sonntag', 'Christian von der Hoya', 'Diana Zdanowicz', 'Juergen Puscher', 'Emanuel Stuebner', 'Sven Schelian', 'Verena Hellfritsch', 'Katja Seifert', 'Marcel Voigt', 'Christian-Alexander Krebs', 'Bettina Fink', 'Anja Pistner', 'Juergen Puscher', 'Martin Wickler', 'Eric Straib', 'Rainer Schroeder', 'Martin Herisch', 'Stefan Jaenicke', 'Helge Bunk', 'Andreas Greiner', 'Frank Launspach', 'Michael Below', 'Peter Stang', 'Angelika Frittmann', 'Ulrike Kolbinger', 'Andreas Willberger', 'Bjoern Stoll', 'Steven Greenhill', 'Juergen Puscher', 'Harald Haenssgen', 'Michael-Gerhard Czapp', 'Helge Bunk', 'Peter Stang', 'Katinka Hohmann', 'Markus Pachert', 'Sabrina Luft', 'Danny Kostorz', 'Kim Pau', 'Olaya Leon-Romero', 'Oliver Keil', 'Antje Abel', 'Karl-Heinz Riehl', 'Karolin Eysenbach', 'Matthias Kern', 'Sebastian Knippel', 'Astrid Stanzl', 'Andre Kellmann', 'Vanessa Keil', 'Karin Kroll', 'Sebastian Goldbach', 'Desiree Altintas', 'Eric Kretschmann', 'Steven Greenhill', 'Juergen Puscher', 'Lukasz Krol', 'Rainer Schroeder', 'Stefan Jaenicke', 'Helge Bunk', 'Andreas Greiner', 'Martin Herisch', 'Frank Launspach', 'Michael Below', 'Peter Stang', 'Angelika Frittmann', 'Ulrike Kolbinger', 'Andreas Willberger', 'Jonas Baumann', 'Bjoern Stoll', 'Florian Auth', 'Paulo Mesquita', 'Kai Schneider', 'Nicolas-Eric Lamm', 'Daniel Farani', 'Manuel Hoffmann', 'Manuel Schinzel', 'Chiara Bellomo', 'Berfu-Merve Aydinyer', 'Christopher Doerr', 'Olaf Hagelstein', 'Michael Losert', 'Denis Salesski', 'Mohammed El Hadrati', 'Dmitry Wied', 'Andreas Sever', 'Klaus Koop', 'Kim Holy', 'Ralf Ginter', 'Frank Lieberwirth', 'Peter Ellersiek', 'Christian Vollmer', 'Ingrid Kellermann', 'Andre Ohmen', 'Christian Schafmeister', 'Stefan Atz', 'Volker Stock', 'Mario Krapp', 'Christoph Theissing', 'Tobias Fritsche', 'Johan Mitev', 'Christian Rotter', 'Rainer Schaefenacker', 'Herbert Linhardt', 'Marco Taufer', 'Ulrich Lampen', 'Irina Hermann', 'Ute Schroeder', 'Simone Baumann', 'Katrin Thor', 'Jonas Baumann', 'Emanuel Stuebner', 'Bettina Greifzu-Eberhardt', 'Ina Kulessa', 'Tim Trellenberg', 'Monika Schmuck', 'Azubi Pricing2', 'Azubi Pricing', 'Juan Bueno', 'Youness Ajouaou', 'Stephan Johann', 'Yoko Igarashi', 'Dominik Heck', 'Khalid Boulkhair', 'Cornelius Moeglich', 'Steffen Schmidt', 'Christian Haastert', 'Klaus Brinkmann', 'Oliver Jost', 'Andreas Sever', 'Steffen Kron', 'Kim Holy', 'Viola Jost', 'Thorsten Rasch', 'Stephanie Tschunt', 'Christian-Alexander Krebs', 'Ulrich Lampen', 'Kristina Schatz', 'Stephanie Kirchner', 'Karl-Heinz Fuchs', 'Katrin Thor', 'Bettina Greifzu-Eberhardt', 'Annika-Frederike Helmer', 'Christian Ziegler', 'Christian-Alexander Krebs', 'Bjoern Stoll', 'Steven Greenhill', 'Juergen Puscher', 'Kai Schneider', 'Frank Launspach', 'Felice Scarpa', 'Martin Knoess', 'Verena Hellfritsch', 'Andre Baldauf', 'Anja Pistner', 'Gerd Gaydoul', 'Christopher Steitz', 'Andreas Kopp', 'Markus Reents', 'Joerg Kohlbacher', 'Mario Heitmann', 'Thorsten Hergenroether', 'Stefan Jaenicke', 'Martin Herisch', 'Christoph Gote', 'Martin Knoess', 'Markus Prokopp', 'Pascal Dupuy', 'Michael Drogi', 'Frank Gehron', 'Claudio Alfarano', 'Steffen Schmidt', 'Walter Mohr', 'Daniel Dittmann', 'Alexander Arent', 'Christoph Gote', 'Debora Knobloch', 'Angelika Sztycharz', 'Sandra Jansen', 'Danijel Romanik', 'Thomas Brandeis', 'Pascal Dupuy', 'Klaus Mank', 'Alexander Ochs', 'Amir Salihefendic', 'Reiner Fuellhardt', 'Marcus Gote', 'Marcel Geisen', 'Viktor Wulfert', 'Florian Kindler', 'Daniel Dittmann', 'Rebecca Ruehl', 'Stephan Johann', 'Susanne Filius', 'Jonas Baumann', 'Joerg Dahlhoff', 'Frank Lieberwirth', 'Thomas Jochum', 'Andreas Brandt', 'Daniella Wichary', 'Konrad Hufmann', 'Diego Mirabelli', 'Roland Sieg', 'Oliver Meyer', 'Pierre Dalbritz', 'Emanuel Stuebner', 'Thomas Schwan', 'Jasmin Perez', 'Christoph Lang', 'Friedrich Wander', 'Pascal Dupuy', 'Christian Tome', 'Frank Gehron', 'Holger Scholl', 'Bjoern Mittenzwei', 'Rene Henning', 'Jonas Hohmann', 'Uwe Zimmermann', 'Marcus Leiste', 'Sebastian Birzer', 'Tim Trellenberg', 'Matthias Kern', 'Paul Stahmer', 'Christian Bauer', 'Christos Kyriakou', 'Andreas Reder', 'Andre Baldauf', 'Andreas Koch', 'Dominik Dehm', 'Eric Kretschmann', 'Harald Muenster', 'Frank Wesemann', 'Uwe Fritsch', 'Torsten Lamparter', 'Simon Schlenker', 'Stefan Dreilich', 'Marius-Florin Magher', 'Misel Balic', 'Sylvia Borchers', 'Anne Schweder', 'Markus Prokopp', 'Achim Goelter', 'Emanuel Stuebner', 'Tadashi Takeuchi', 'Nico Rohm', 'Harald Kuehne', 'Martina Hinkel', 'Monika Schwebel', 'Christoph Gote', 'Peter Pfaffenberger', 'Vincenzo Addison', 'Daniela Schoeneberger', 'Harald Diel', 'Barbara Trippel', 'Emanuel Stuebner', 'Danijel Romanik', 'Holger Scholl', 'Mario Krapp', 'Lukas Soukup', 'Reinhard Schade', 'Nils Boy', 'Marco Taufer', 'Michael Losert', 'Mario Heitmann', 'Sven Haindl', 'Ronald Ehrlich', 'Gen Uchimido', 'Tobias Bachmeier', 'Mitsunobu Shinohara', 'Christopher Steitz', 'Andreas Kopp', 'Markus Prokopp', 'Markus Reents', 'Frank Gehron', 'Christian Bauer', 'Joerg Kohlbacher', 'Yoko Igarashi', 'Cornelius Moeglich', 'Anna-Maria Scarpa', 'Christian Haastert', 'Helge Bunk', 'Thomas Lindhammer', 'Alexander Pawera', 'Steven Greenhill', 'Harald Kuehne', 'Tobias Hartherz', 'Klaus Brinkmann', 'Michael Becker', 'Olaf Hagelstein', 'Michael Losert', 'Kim Holy', 'Christine Seidel', 'Ulrich Lampen', 'Irina Hermann', 'Lisa Meerheim', 'Juergen Puscher', 'Marc-Oliver Schroeder', 'Emanuel Stuebner', 'Matthias Ronacher', 'Ina Kulessa', 'Tim Trellenberg', 'Alexander Banzhaf', 'Patricia Jonientz', 'Michael-Gerhard Czapp', 'Christian Haastert', 'Andreas Egelseder', 'Eric Straib', 'Kadira Merdzic', 'Pascal Borusiak', 'Marcel Geisen', 'Juan Bueno', 'Daniel Dittmann', 'Stephan Johann', 'Marc Spriestersbach', 'Yoko Igarashi', 'Alexander Arent', 'Frank Friedmann', 'Ana Karach', 'Christoph Gote', 'Dominik Heck', 'Dragan Dankic', 'Debora Knobloch', 'Maximilian Stork', 'Martin Knoess', 'Markus Prokopp', 'Angelika Sztycharz', 'Sandra Jansen', 'Danijel Romanik', 'Cornelius Moeglich', 'Thomas Brandeis', 'Pascal Dupuy', 'Michael Drogi', 'Dierck Kerber', 'Frank Gehron', 'Klaus Mank', 'Sven Schelian', 'Angelo Adduci', 'Juergen Schoernig', 'Bjoern Mittenzwei', 'Marius Diem', 'Jonas Hohmann', 'Waldemar Sawatzky', 'Alexander Ochs', 'Amir Salihefendic', 'Christian Bauer', 'Claudio Alfarano', 'Alexander Kistner', 'Tobias Seifert', 'Andreas Reder', 'Hung Nguyen-Thanh', 'Robert Homm', 'Reiner Fuellhardt', 'Dominik Dehm', 'Steffen Schmidt', 'Walter Mohr', 'Anja Pistner', 'Christian Haastert', 'Jan Mennerich', 'Jens Prockl', 'Diana Zdanowicz', 'Marc-Oliver Schroeder', 'Stefan Jaenicke', 'Diego Mirabelli', 'Christian Ziegler', 'Oliver Prang', 'Christian-Alexander Krebs', 'Richard Spengler', 'Ralph Herbrich', 'Verena Hellfritsch', 'Kerstin Nordquist', 'Jennifer Moreno-Barrientos', 'Karin Keller', 'Anja Pistner', 'Lisa Zierock', 'Julia Schwab', 'Claudio Sicorello', 'Tamoor Hussain', 'Steven Greenhill', 'Martin Herisch', 'Christian Ziegler', 'Pascal Borusiak', 'Angelika Frittmann', 'Ulrike Kolbinger', 'Andreas Willberger', 'Verena Hellfritsch', 'Christian-Alexander Krebs', 'Bettina Fink', 'Jennifer Moreno-Barrientos', 'Anja Pistner', 'Lena-Alejandra Lauer-Toro', 'Bjoern Stoll', 'Melis Bora', 'Juergen Puscher', 'Florian Auth', 'Paulo Mesquita', 'Christian Ziegler', 'Tobias Hartherz', 'Klaus Brinkmann', 'Olaf Hagelstein', 'Christian Vollmer', 'Andre Ohmen', 'Christian Schafmeister', 'Helene Le Gallo', 'Anna Riess', 'Rebecca Klein', 'Christoph Koelle', 'Gudrun Sprinz-Honner', 'Youness Ajouaou', 'Christian Haastert', 'Tobias Hartherz', 'Nejdet Oeztuerk', 'Ferdinand Rein', 'Mehmet Avci', 'Rainer Schroeder', 'Martin Herisch', 'Peter Stang', 'Ulrike Kolbinger', 'Steven Greenhill', 'Juergen Puscher', 'Bjoern Prinz', 'Michael Ehinger', 'Frank Voss', 'Nicolas Martin-Antequera', 'Christian Bauer', 'Patricia Jonientz', 'Mirko Ganz', 'Andreas Egelseder', 'Christian Ziegler', 'Rainer Schroeder', 'Martin Herisch', 'Juergen Puscher', 'Martin Herisch', 'Monika Schwebel', 'Karl-Heinz Fuchs', 'Harald Diel', 'Emanuel Stuebner', 'Holger Scholl', 'Mario Krapp', 'Marco Taufer', 'Juergen Puscher', 'Christian Ziegler', 'Klaus Brinkmann', 'Oliver Jost', 'Rolf-Eric Matthies', 'Oliver Prang', 'Ralf Laber', 'Andreas Egelseder', 'Rainer Schroeder', 'Andreas Greiner', 'Martin Herisch', 'Frank Launspach', 'Juergen Puscher', 'Paulo Mesquita', 'Martin Wickler', 'Kai Schneider', 'Martin Herisch', 'Andreas Willberger', 'Volker Kleespies', 'Christopher Steitz', 'Andreas Kopp', 'Martin Knoess', 'Markus Prokopp', 'Frank Gehron', 'Christian Bauer', 'Claudio Alfarano', 'Joerg Kohlbacher', 'Walter Mohr', 'Juergen Puscher', 'Paulo Mesquita', 'Michael Kraus', 'Martin Wickler', 'Kai Schneider', 'Manuel Hoffmann', 'Klaus Deeg', 'Ingo Aberer', 'Monika Schwebel', 'Simone Siegel', 'Katinka Hohmann', 'Susanne Filius', 'Markus Pachert', 'Sabrina Luft', 'Danny Kostorz', 'Maximilian Stork', 'Azubi Customer Service Center', 'Jennifer Bayraktaroglu', 'Erika Marschhaeuser', 'Kim Pau', 'Toni Schellenberger', 'Olaya Leon-Romero', 'Oliver Keil', 'Antje Abel', 'Karl-Heinz Riehl', 'Nicklas Mueller', 'Azubi Customer Service Center 2', 'Karolin Eysenbach', 'Edgar Minch', 'Juana Prieto-Lopez', 'Silke Reifschneider', 'Matthias Kern', 'Sebastian Knippel', 'Astrid Stanzl', 'Andre Kellmann', 'Vanessa Keil', 'Susanne Raab', 'Karin Kroll', 'Alexander Hunger', 'Sebastian Goldbach', 'Danijel Posavec', 'Desiree Altintas', 'Tanja Nowroth', 'Eric Kretschmann', 'Sebahat Arda-Helms', 'Tobias Fischer', 'Torsten Lamparter', 'DE-RPA-CSC', 'Klaus Brinkmann', 'Nejdet Oeztuerk', 'Ferdinand Rein', 'Mehmet Avci', 'Stefan Seufert', 'Thomas Labatzke', 'Florian Hammen', 'Gerd Ecker', 'Alex Rosental', 'David Herrmann', 'Hasan Karali', 'Tilman Wannemacher', 'Dieter Betke', 'Buesra Candir', 'Klaus Basmangin', 'Caroline Wolf', 'Axel Teichgraeber', 'Lothar Beylschmidt', 'Bernd Lede', 'Stephan Schweissing', 'Oliver Jost', 'Alexej Liebrecht', 'Monika Heimann', 'Thomas Lohmann', 'Thomas Dingeldein', 'Markus Heimann', 'Sebastian Zahn', 'Karl Nicolay', 'Ngoc-Minh Nguyen', 'Dominik Schaefer', 'Stefan Panten', 'Michael Reining', 'Ulrich Raueiser', 'Wolfgang Schulze', 'Igor Denneng', 'Axel Fischer', 'Susanne Karl', 'Sascha Dietzel', 'Denis Salesski', 'Oliver Boerner', 'Volker Kleespies', 'Mohammed El Hadrati', 'Florian Emich', 'Majid Rammah', 'Juergen Vinzenz', 'Yui Okada', 'Martina Hinkel', 'Mile Milovanovic', 'Dmitry Wied', 'Frank Sponer', 'Karlheinz Roehrs', 'Giuseppe Cucchiara', 'Lucas Krause', 'Nico Bernhardt', 'Alexej Kloos', 'Beate Fuchs', 'Andreas Sever', 'Thomas Strobel', 'Martin Bauer', 'Tobias Bachmeier', 'Bulut Karabulut', 'Melanie Firll', 'Alexander Ruhl', 'Rolf-Eric Matthies', 'Atsushi Okamoto', 'Ralph Benkenstein', 'Michael Ott', 'Thomas Peter', 'Birgit Germann', 'Joshua Pfeifer', 'Dirk Schoenau', 'Mazlum Akguel', 'Christoph Damm', 'Guido Schneider', 'Alexander Chipelik', 'Helmut Liese', 'Michael Soter', 'Christian Zickert', 'Florian Kindler', 'Kevin Allendorf', 'Mitsunobu Shinohara', 'Daniel Kornberger', 'Steffen Kron', 'Toshiyuki Mori', 'Andre Schreiber', 'Susanne Angele', 'Miosga Mario', 'Sebastian Bialas', 'Muhammad-Ahsan Qazi', 'Atsushi Fujiwara', 'Trapp Christian', 'Gross Stefan', 'Breidert Markus', 'Kristina Schatz', 'Mirja Brink', 'Claudia Baran', 'Marion Eusemann', 'Hamzah Ahmed', 'Mohamed Boudouhi', 'Peter Pachnik', 'Claus Nitsch', 'Andreas Gross', 'Abdelkarim Al-Kadi', 'Heiko Hasse', 'Viktor Wulfert', 'Arno Neumann', 'Joerg Honka', 'Vincenzo Addison', 'Thomas Walther', 'Marius Bueger', 'Bernd Walter', 'Samuel Groh', 'Michael Kretzschmar', 'Anna Graf', 'Monika Metz', 'Marco Gruber', 'Marius Diem', 'Claudia Wenchel', 'Markus Witte', 'Sabrina Kranz', 'Jan Hanse', 'Mirko Ganz', 'Nikolaj Krez', 'Irina Kistner', 'Marcel Ploesser', 'Jens Heppert', 'David Kerscher', 'Sara Klumpp', 'Haroun Kakar', 'Thorsten Winter', 'Volker Kleespies', 'Rolf-Eric Matthies', 'Richard Spengler', 'Harald Kuehne', 'Tobias Hartherz', 'Michael Becker', 'Olaf Hagelstein', 'Nejdet Oeztuerk', 'Michael Losert', 'Thomas Labatzke', 'Hasan Karali', 'Oliver Jost', 'Thomas Dingeldein', 'Markus Heimann', 'Sebastian Zahn', 'Michael Reining', 'Wolfgang Schulze', 'Sascha Dietzel', 'Denis Salesski', 'Mohammed El Hadrati', 'Florian Emich', 'Majid Rammah', 'Mile Milovanovic', 'Dmitry Wied', 'Karlheinz Roehrs', 'Andreas Sever', 'Tobias Bachmeier', 'Bulut Karabulut', 'Ralph Benkenstein', 'Michael Ott', 'Dirk Schoenau', 'Mazlum Akguel', 'Christoph Damm', 'Michael Soter', 'Christian Zickert', 'Kevin Allendorf', 'Daniel Kornberger', 'Steffen Kron', 'Kim Holy', 'Viola Jost', 'Burcu Cevik', 'Christine Seidel', 'Muhammad-Ahsan Qazi', 'Ulrich Lampen', 'Mohamed Boudouhi', 'Stephanie Kirchner', 'Irina Hermann', 'Lisa Meerheim', 'Andreas Gross', 'Abdelkarim Al-Kadi', 'Heiko Hasse', 'Tobias Hartherz', 'Ralf Wingen', 'Nico Rohm', 'Markus Kohler', 'Christine Seidel', 'Ulrich Lampen', 'Bettina Fink', 'Klopertanz Nadine', 'Melis Bora', 'Steven Greenhill', 'Angelika Frittmann', 'Nicolas-Eric Lamm', 'Marcel Geisen', 'Martin Knoess', 'Bjoern Mittenzwei', 'Jonas Hohmann', 'Hung Nguyen-Thanh', 'Jan Mennerich', 'Stephan Huebner', 'Timo Schlauch', 'Klaus Koop', 'Marcus Bock', 'Mario Spitz', 'Wiebke Roestel', 'Carsten Moeller', 'Joachim Klotz', 'Hartmut Schubert', 'Ute Bobber', 'Nicole Koop', 'Eugen Quast', 'Gerhard Haefner', 'Philipp Ameis', 'Dimitrios Pashalidis', 'Anne Schweder', 'Alexander Valentin', 'Andreas Bott', 'Thomas Neubieser', 'Markus Leich', 'Ralf Ginter', 'Ralph Lemmnitz', 'Frank Tschepke', 'Juergen Kallis', 'Ulrike Schlosser', 'Peter Pfaffenberger', 'Norman Glemser', 'Thomas Schwaninger', 'Erik Schneider', 'Ralf Wingen', 'Sebastian Riedel', 'Johann Leonhart', 'Frank Lieberwirth', 'Florian Auch', 'Norman Schulz', 'Nicole Kost', 'Andreas Reese', 'Thomas Boers', 'Roland Sieg', 'Seyfi Guenduez', 'Andre Stautz', 'Wassili Fink', 'Sven Remus', 'Peter Ellersiek', 'Klaus Deeg', 'Matthias Schnorrenberg', 'Christian Vollmer', 'Dirk Siemko', 'Regina Kueppers', 'Toni Schreier', 'Thomas Schwan', 'Matthias Klein', 'Markus Kruse', 'Thorsten Rasch', 'Steffen Wonsak', 'Andre Prosen', 'Martin Swonke', 'Jan-Christian Luttmann', 'Thomas Simon', 'Ingrid Kellermann', 'Christian Ackermann', 'Joerg Noll', 'Hilmi Sert', 'Manuel Reichart', 'Harald Haenssgen', 'Matthias Ronacher', 'Wolfgang Ebner', 'Helmut Gerdes', 'Silvia Czekala', 'Roland Kraemer', 'Thomas Hellmuthhaeuser', 'Markus Zaschka-Loebach', 'Manfred Strauss', 'Markus Blocher', 'Rene Henning', 'Harald Eisenhardt', 'Wolfgang Wein', 'Christian Schafmeister', 'Matthias Mahn', 'Ulf Suckow', 'Achim Knapp', 'Karsten Buehring', 'Thomas Zeissl', 'Guido Tiemann', 'Maik Lohmeyer', 'Stefan Atz', 'Zbigniew Langowski', 'Juergen Deinzer', 'Volker Stock', 'Mario Krapp', 'Markus Limper', 'Gerd Jopek', 'Christoph Theissing', 'Christoph Czomperlik', 'Christoph Nussbaum', 'Wilhelm Kuhlmann', 'Paul Stahmer', 'Christian Suchalla', 'Tobias Fritsche', 'Lejla Salievska', 'Johan Mitev', 'Kai Schilling', 'Thomas Heider', 'Marcel Voigt', 'Christian Rotter', 'Axel Schaefer', 'Vladimir Jungblut', 'Sven Heise', 'Steffen Skarus', 'Norbert Glas', 'Fabian Heidekorn', 'Reinhard Schade', 'Eckhard Cramer', 'Stefan Walter', 'Martin Schinkel', 'Andreas Fischer', 'Savas Oeztuerk', 'Rainer Schaefenacker', 'Josef Iglhaut', 'Detlef Hett', 'Frank Mueer', 'Patrick Blum', 'Eckard Stiehle', 'Andreas Micus', 'Werner Behmueller', 'Tim Graeser', 'Alexander Schur', 'Andreas Melzer', 'Ingo Aberer', 'Raimund Bauer', 'David Pajares', 'Juergen Beitzel', 'Guenter Timm', 'Andreas Koch', 'Klaus Romeiks', 'Patricia Jonientz', 'Herbert Linhardt', 'Hans-Joachim Seedorf', 'Helmut Probst', 'Nils Boy', 'Petra Decker', 'Bernd Symannek', 'Marco Taufer', 'Martin Klotz', 'Sven Eckhardt', 'Florian Wuttke', 'Markus Kohler', 'Edwin Kuenzel', 'Denny Ledrich', 'Stefan Huber', 'Bernd Kaiser', 'Andreas Egelseder', 'Pascal Borusiak', 'Ralf Laber', 'Kai Schneider', 'Karl-Heinz Fuchs', 'Katinka Hohmann', 'Danny Kostorz', 'Olaya Leon-Romero', 'Oliver Keil', 'Nicklas Mueller', 'Matthias Kern', 'Torsten Lamparter', 'David Blasek', 'Angelika Frittmann', 'Andreas Willberger', 'Ute Schroeder', 'Stephan Schweissing', 'Majid Rammah', 'Daniel Dittmann', 'Felice Scarpa', 'Yoko Igarashi', 'Markus Pachert', 'Jonas Baumann', 'Toni Schellenberger', 'Jasmin Perez', 'Christian Tome', 'Frank Gehron', 'Heiko Hestermann', 'Anette Sinemus', 'Torsten Lamparter', 'Bjoern Stoll', 'Florian Auth', 'Michael Schultz', 'Ralf Kohl', 'Werner Baumann', 'Axel Schaefer', 'Joerg Noll', 'Matthias Ronacher', 'Guido Tiemann', 'Gerd Jopek', 'Andreas Melzer', 'Ingo Aberer', 'Ralf Laber', 'Pierre Dalbritz', 'Klaus Deeg', 'Joerg Noll', 'Matthias Ronacher', 'Guido Tiemann', 'Gerd Jopek', 'Axel Schaefer', 'Andreas Melzer', 'Ingo Aberer', 'Rainer Schroeder', 'Martin Herisch', 'Bjoern Stoll', 'Steven Greenhill', 'Juergen Puscher', 'Paulo Mesquita', 'David Blasek', 'Peter Schaefer', 'Kristina Pasternak', 'Tobias Heller', 'Heiko Hestermann', 'Juergen Becker', 'Uwe-Andreas Masur', 'Igor Hornak', 'Norbert Hertel', 'Azubi Finance', 'Michael Dohm', 'Lorena Brekalo', 'Richard Spengler', 'Ralph Herbrich', 'Verena Hellfritsch', 'Sara Klumpp', 'Andreas Gross', 'Abdelkarim Al-Kadi', 'Darko Pokos', 'Lukas Roehn', 'Christian Knoerzer', 'Haroun Kakar', 'Peter Stang', 'Stefan Jaenicke', 'Helge Bunk', 'Andreas Bott', 'Claus Kapp', 'Thomas Meyer', 'Udo Hartmann', 'Emanuel Stuebner', 'Jan-Christian Luttmann', 'Michael Schultz', 'Matthias Ronacher', 'Ralf Kohl', 'Katja Seifert', 'Ina Kulessa', 'Werner Baumann', 'Axel Schaefer', 'Joerg Heitlindemann', 'Nils Boy', 'Matthias Menge', 'Eric Straib', 'Michael Below', 'Peter Stang', 'Stefan Jaenicke', 'Achim Goelter', 'Steffen Tewes', 'Tadashi Takeuchi', 'Markus Blocher', 'Steffen Skarus', 'Patricia Jonientz', 'Nico Rohm', 'Andreas Egelseder', 'Steven Greenhill', 'Anja Pistner', 'Lena-Alejandra Lauer-Toro', 'Bjoern Stoll', 'Melis Bora', 'Claus Kapp', 'Thomas Meyer', 'Udo Hartmann', 'Andreas Brandt', 'Christian Burghardt', 'Willi-Paul Dueren', 'Ralph Herbrich', 'Deniz Kilic', 'Alexej Steblau', 'Michael Schultz', 'Karsten Schaetzlein', 'Axel Daffner', 'Ralf Kohl', 'Marcus Leiste', 'Christine Hasselluhn', 'Thomas Thiel', 'Martin Mueller', 'Werner Baumann', 'Oliver Lengenfelder', 'Axel Schaefer', 'Andreas Schnell', 'Hans-Uwe Mertens', 'Joerg Heitlindemann', 'Patricia Jonientz', 'Bernd Kaufer', 'Martin Heckel', 'Andreas Egelseder', 'Sylvia Borchers', 'Martin Herisch', 'David Blasek', 'Michael Becker', 'Ulrike Kolbinger', 'Andre Schreiber', 'Susanne Angele', 'Karl-Heinz Fuchs', 'Katrin Thor', 'Vincenzo Addison', 'Roland Sieg', 'Oliver Keil', 'Jasmin Perez', 'Bettina Greifzu-Eberhardt', 'Joerg Noll', 'Ralf Kohl', 'Verena Hellfritsch', 'Matthias Kern', 'Christian Bauer', 'Axel Schaefer', 'Christian-Alexander Krebs', 'Patrick Blum', 'Burcu Cevik', 'Desiree Altintas', 'Felix Rossmann', 'Christian Haastert', 'Anne Heidrich', 'Michael Dohm', 'Marina Steenbergen', 'Chiara Bellomo', 'Berfu-Merve Aydinyer', 'Steven Greenhill', 'Brigitte Martinez-Mendez', 'Bettina Fink', 'Patricia Jonientz', 'Christine Seidel', 'Andreas Egelseder', 'Kadira Merdzic', 'Martin Knoess', 'Markus Prokopp', 'Juergen Becker', 'Grit Scharein', 'Christian Bauer', 'Mirko Ganz', 'Michael Dohm', 'David Basiewicz', 'Lukas Roehn', 'Christoph Damm', 'Klaus Koop', 'Hartmut Schubert', 'Eugen Quast', 'Gerhard Haefner', 'Philipp Ameis', 'Ralf Ginter', 'Ralph Lemmnitz', 'Frank Tschepke', 'Juergen Kallis', 'Thomas Schwaninger', 'Frank Lieberwirth', 'Florian Auch', 'Peter Ellersiek', 'Christian Vollmer', 'Dirk Siemko', 'Thorsten Rasch', 'Martin Swonke', 'Ingrid Kellermann', 'Roland Kraemer', 'Christian Schafmeister', 'Stefan Atz', 'Juergen Deinzer', 'Volker Stock', 'Mario Krapp', 'Christoph Theissing', 'Christoph Czomperlik', 'Tobias Fritsche', 'Johan Mitev', 'Thomas Heider', 'Christian Rotter', 'Vladimir Jungblut', 'Norbert Glas', 'Fabian Heidekorn', 'Rainer Schaefenacker', 'Tim Graeser', 'David Pajares', 'Herbert Linhardt', 'Hans-Joachim Seedorf', 'Helmut Probst', 'Marco Taufer', 'Sven Eckhardt', 'Felix Rossmann', 'Polina Rozova', 'Bjoern Stoll', 'Steven Greenhill', 'Martin Herisch', 'Frank Launspach', 'Juergen Puscher', 'Paulo Mesquita', 'Nicolas-Eric Lamm', 'Michael Below', 'Peter Stang', 'Steven Greenhill', 'Christian Ziegler', 'Karl-Heinz Fuchs', 'Thorsten Rasch', 'Joerg Noll', 'Ralf Laber', 'Frank Voss', 'Verena Hellfritsch', 'Patricia Jonientz', 'Andreas Egelseder', 'Sonja Viola Birkenhake', 'Elena Klee', 'Stephan Joellenbeck', 'Andre Ohmen', 'Mario Heitmann', 'Dirk Emmerich', 'Thorsten Hergenroether', 'Frank Wesemann', 'Sven Haindl', 'Ronald Ehrlich', 'Gen Uchimido', 'Andreas Willberger', 'Steven Greenhill', 'Paulo Mesquita', 'Juergen Puscher', 'Kai Schneider', 'Ralf Laber', 'Klaus Brinkmann', 'Ferdinand Rein', 'Oliver Jost', 'Mohammed El Hadrati', 'Rolf-Eric Matthies', 'Michael Ott', 'Susanne Angele', 'Thorsten Rasch', 'Ulrich Lampen', 'Kristina Schatz', 'Martin Herisch', 'Ulrike Kolbinger', 'Stefan Jaenicke', 'Kai Schneider', 'Chiara Bellomo', 'Berfu-Merve Aydinyer', 'Klaus Brinkmann', 'Philipp Ameis', 'Juergen Kallis', 'Florian Auch', 'Dirk Siemko', 'Thorsten Rasch', 'Christoph Czomperlik', 'Vladimir Jungblut', 'Katja Michels', 'Hans-Joachim Seedorf', 'Felix Rossmann', 'Polina Rozova', 'Kristina Schatz', 'Rebecca Ruehl', 'Silke Blitz', 'Akiko Sciacovelli', 'Lixia Liao', 'Lin Fan', 'Stephan Johann', 'Edgar Minch', 'Christian Haastert', 'Eitenmueller Jennifer', 'Blanka Lueder', 'Axel Teichgraeber', 'Bernd Lede', 'Rolf-Eric Matthies', 'Ralph Benkenstein', 'Juan Bueno', 'Stephan Johann', 'Christoph Gote', 'Martin Knoess', 'Markus Prokopp', 'Pascal Dupuy', 'Frank Gehron', 'Klaus Mank', 'Marius Diem', 'Tim Trellenberg', 'Matthias Kern', 'Alexander Ochs', 'Amir Salihefendic', 'Christian Bauer', 'Mirko Ganz', 'Haroun Kakar', 'Karsten Buehring', 'Kai Schilling', 'Martin Herisch', 'Ulrike Kolbinger', 'Frank Launspach', 'Monika Schwebel', 'Karl-Heinz Fuchs', 'Harald Diel', 'Emanuel Stuebner', 'Holger Scholl', 'Mario Krapp', 'Marco Taufer', 'Steven Greenhill', 'Juergen Puscher', 'Paulo Mesquita', 'Daniel Farani', 'Marina Steenbergen', 'Manuel Hoffmann', 'Chiara Bellomo', 'Berfu-Merve Aydinyer', 'Marcel Geisen', 'David Herrmann', 'Dieter Betke', 'Axel Teichgraeber', 'Lothar Beylschmidt', 'Bernd Lede', 'Stephan Schweissing', 'Alexej Liebrecht', 'Thomas Lohmann', 'Dominik Schaefer', 'Ulrich Raueiser', 'Oliver Boerner', 'Juergen Vinzenz', 'Frank Sponer', 'Giuseppe Cucchiara', 'Lucas Krause', 'Nico Bernhardt', 'Martin Bauer', 'Alexander Ruhl', 'Rolf-Eric Matthies', 'Ralph Benkenstein', 'Torsten Nagel', 'Juan Bueno', 'Sven Simon', 'Stephan Johann', 'Christoph Gote', 'Martin Knoess', 'Markus Prokopp', 'Khalid Boulkhair', 'Pascal Dupuy', 'Michael Drogi', 'Frank Gehron', 'Klaus Mank', 'Marius Diem', 'Matthias Kern', 'Alexander Ochs', 'Amir Salihefendic', 'Christian Bauer', 'Claudio Alfarano', 'Joerg Kohlbacher', 'Mirko Ganz', 'Walter Mohr', 'Felix Rossmann', 'Polina Rozova', 'Gross Stefan', 'Claudia Baran', 'Eric Schwarzer', 'Simeon Rongstock', 'Haroun Kakar', 'Juergen Puscher', 'Thomas Dingeldein', 'Mohammed El Hadrati', 'Dmitry Wied', 'Mitsunobu Shinohara', 'Muhammad-Ahsan Qazi', 'Abdelkarim Al-Kadi', 'Brigitte Martinez-Mendez', 'Stephanie Tschunt', 'Christine Seidel', 'Stephan Johann', 'Yoko Igarashi', 'Christian Haastert', 'Klaus Brinkmann', 'Stefan Jaenicke', 'Helge Bunk', 'Michael Below', 'Peter Stang', 'Matthias Kern', 'Klaus Brinkmann', 'Elena Klee', 'Ralf Laber', 'Mario Heitmann', 'Gen Uchimido', 'Andreas Egelseder', 'Karl-Heinz Fuchs', 'Rudi Meder', 'Jan Marczinski', 'Azubi Human Resources', 'David Basiewicz', 'Silke Frank', 'Thomas Dingeldein', 'Dmitry Wied', 'Tobias Bachmeier', 'Mitsunobu Shinohara', 'Kim Holy', 'Marco Taufer', 'Muhammad-Ahsan Qazi', 'Rainer Schroeder', 'Martin Herisch', 'Juergen Puscher', 'Matthias Menge', 'Ute Schroeder', 'Simone Baumann', 'Emanuel Stuebner', 'Ina Kulessa', 'Nathalie Daniel', 'Tim Trellenberg', 'Monika Schmuck', 'Eva-Maria Perez-Gonzalez', 'Azubi Pricing2', 'Azubi Pricing', 'Charleen Nikoles', 'Eric Straib', 'Misel Balic', 'Michael Below', 'Nejdet Oeztuerk', 'Ferdinand Rein', 'Mehmet Avci', 'Susanne Angele', 'Marius Diem', 'Mirko Ganz', 'Sebastian Bialas', 'Haroun Kakar', 'Steven Greenhill', 'Verena Hellfritsch', 'Pascal Borusiak', 'Susanne Angele', 'Karl-Heinz Fuchs', 'Ralf Laber', 'Steven Greenhill', 'Rainer Schroeder', 'Martin Herisch', 'Peter Stang', 'Bjoern Stoll', 'DE-SVC-O365-SharePoint', 'Rainer Schroeder', 'Stefan Jaenicke', 'Helge Bunk', 'Andreas Greiner', 'Martin Herisch', 'Frank Launspach', 'Michael Below', 'Peter Stang', 'Angelika Frittmann', 'Ulrike Kolbinger', 'Andreas Willberger', 'Bjoern Stoll', 'Steven Greenhill', 'Juergen Puscher', 'Paulo Mesquita', 'Nicolas-Eric Lamm', 'Daniel Farani', 'Sylvia Borchers', 'Gabriele Sonntag', 'Christian von der Hoya', 'Fabian Strodl', 'Carsten Noack', 'Ralf Roske', 'Achim Goelter', 'Klaus Deeg', 'Joerg Noll', 'Matthias Ronacher', 'Dominik Lewin', 'Frank Voss', 'Ralf Kohl', 'Guido Tiemann', 'Gerd Jopek', 'Axel Schaefer', 'Alexander Banzhaf', 'Andreas Melzer', 'Ingo Aberer', 'Alexander Pawera', 'Diana Zdanowicz', 'Andreas Egelseder', 'Nejdet Oeztuerk', 'Ferdinand Rein', 'Mehmet Avci', 'Sylvia Borchers', 'Peter Schaefer', 'Christian Ziegler', 'Pascal Borusiak', 'Klaus Brinkmann', 'Susanne Angele', 'Karl-Heinz Fuchs', 'Thorsten Rasch', 'Ralf Laber', 'Verena Hellfritsch', 'Mario Heitmann', 'Matthias Kern', 'Christian Bauer', 'Christian Haastert', 'Diana Zdanowicz', 'Juergen Puscher', 'Andreas Egelseder', 'Christian Ziegler', 'Stephanie Tschunt', 'Tobias Hartherz', 'Nejdet Oeztuerk', 'Ferdinand Rein', 'Mehmet Avci', 'Sven Barner', 'Ralf Roske', 'Wolfgang Riedel', 'Tom Bauer', 'Peter Huber', 'Alexander Banzhaf', 'Frank Wesemann', 'Marco Gastel', 'Peter Schaefer', 'Pascal Borusiak', 'Marcel Geisen', 'Martina Hinkel', 'Karl-Heinz Fuchs', 'Yoko Igarashi', 'Harald Diel', 'Martin Knoess', 'Daniella Wichary', 'Markus Prokopp', 'Ralf Laber', 'Holger Scholl', 'Juergen Becker', 'Bjoern Mittenzwei', 'Jonas Hohmann', 'Grit Scharein', 'Christian Bauer', 'Hung Nguyen-Thanh', 'Stefan Ries', 'Mirko Ganz', 'Christian Haastert', 'Juergen Puscher', 'Michael Dohm', 'Joerg Dahlhoff', 'Bjoern Prinz', 'Michael Ehinger', 'Christoph Lang', 'Frank Voss', 'Silvia Czekala', 'Sebastian Birzer', 'Torsten Klein', 'Marcel Voigt', 'Helge Bunk', 'Yoko Igarashi', 'Stefan Jaenicke', 'Klaus Brinkmann', 'Sebastian Zahn', 'Mohammed El Hadrati', 'Alexej Kloos', 'Miosga Mario', 'Atsushi Fujiwara', 'Trapp Christian', 'Christian Mertens', 'Ralf Wingen', 'Matthias Schnorrenberg', 'Matthias Klein', 'Markus Kruse', 'Harald Eisenhardt', 'Torsten Klein', 'Christian Ziegler', 'Stephanie Tschunt', 'Ulrich Lampen', 'Andreas Egelseder', 'Christian Ziegler', 'Jonas Baumann', 'Andreas Brandt', 'Deniz Kilic', 'Alexej Steblau', 'Karsten Schaetzlein', 'Axel Daffner', 'Marcus Leiste', 'Christine Hasselluhn', 'Thomas Thiel', 'Oliver Lengenfelder', 'Andreas Schnell', 'Burcu Cevik', 'Hans-Uwe Mertens', 'Bernd Kaufer', 'Matthias Menge', 'Christine Seidel', 'Martin Heckel', 'Martin Herisch', 'Frank Launspach', 'Juergen Puscher', 'Paulo Mesquita', 'Torsten Nagel', 'Brigitte Jaxt', 'Juan Bueno', 'Sven Simon', 'Christian Haastert', 'Azubi Production Control', 'Gen Uchimido', 'Ulrich Lampen', 'Steven Greenhill', 'Rainer Schroeder', 'Martin Herisch', 'Frank Launspach', 'Bjoern Stoll', 'Juergen Puscher', 'Paulo Mesquita', 'Martin Wickler', 'Kai Schneider', 'Daniel Farani', 'Manuel Hoffmann', 'Peter Schaefer', 'David Blasek', 'Armin Sogerer', 'Stefan Voigt', 'Harald Haenssgen', 'Carsten Schork', 'Klaus Semik', 'Marco Pape', 'Patricia Jonientz', 'Michael-Gerhard Czapp', 'Andreas Egelseder', 'Sylvia Borchers', 'Stefan Jaenicke', 'Christian Ziegler', 'Marc-Oliver Schroeder', 'Daniella Wichary', 'Roland Sieg', 'Achim Goelter', 'Joerg Noll', 'Ralf Laber', 'Frank Voss', 'Patrick Blum', 'Stefan Ries', 'Patricia Jonientz', 'Andreas Egelseder', 'Christian Haastert', 'Kadira Merdzic', 'Marcel Geisen', 'Karl-Heinz Fuchs', 'Frank Friedmann', 'Ana Karach', 'Christoph Gote', 'Dragan Dankic', 'Martin Knoess', 'Markus Prokopp', 'Michael Drogi', 'Dierck Kerber', 'Frank Gehron', 'Juergen Schoernig', 'Verena Hellfritsch', 'Christian Bauer', 'Alexander Kistner', 'Andreas Reder', 'Walter Mohr', 'Anja Pistner', 'David Basiewicz', 'Verena Hellfritsch', 'Anja Pistner', 'Klopertanz Nadine', 'Lena-Alejandra Lauer-Toro', 'Ana Steryova', 'Lorenz Kleemann', 'Maximilian Foerster', 'Alina Blaikner', 'Bjoern Spranger', 'Brigitte Martinez-Mendez', 'Susanne Weber', 'Kathrin Modler', 'Azubi Marketing', 'Viola Jost', 'Samuel Schwab', 'Valdet Gacaferi', 'Nassrat Paryani', 'Samuel Berhane', 'Stephanie Tschunt', 'Bettina Fink', 'Burcu Cevik', 'Markus Schroeder', 'Patricia Jonientz', 'Matthias Menge', 'Christine Seidel', 'Klopertanz Nadine', 'Melis Bora', 'Eva-Maria Kuechle', 'Anne Heidrich', 'Andreas Egelseder', 'Stephanie Kirchner', 'Ariane Weitsch', 'Florian Hammen', 'Alex Rosental', 'Tilman Wannemacher', 'Buesra Candir', 'Axel Teichgraeber', 'Stephan Schweissing', 'Monika Heimann', 'Rolf-Eric Matthies', 'Sebastian Bialas', 'Ralf Laber', 'Harald Kuehne', 'Martina Hinkel', 'Monika Schwebel', 'Peter Pfaffenberger', 'Harald Diel', 'Holger Scholl', 'Lukas Soukup', 'Reinhard Schade', 'Juergen Muth', 'Holger Fastabend', 'Oliver Geier', 'Thomas Lindhammer', 'Jamal Hamim', 'Jens Heinrichs', 'Patricia Jonientz', 'Alexander Pawera', 'Andreas Egelseder', 'Mario Heitmann', 'Thorsten Hergenroether', 'Gabriele Sonntag', 'Joachim Klotz', 'Thomas Schwan', 'Wolfgang Wein', 'Zbigniew Langowski', 'Gerd Jopek', 'Reinhard Schade', 'Eckhard Cramer', 'Stefan Walter', 'Martin Klotz', 'Rainer Schroeder', 'Martin Herisch', 'Juergen Puscher', 'Michael Kraus', 'Manuel Hoffmann', 'Helge Bunk', 'Sylvia Borchers', 'Lukasz Krol', 'Stefan Jaenicke', 'Kadira Merdzic', 'Juergen Puscher', 'Ralf Laber', 'Gen Uchimido', 'Ulrich Lampen', 'Irina Hermann', 'Michael Below', 'Daniel Dittmann', 'Martin Knoess', 'Markus Prokopp', 'Pascal Dupuy', 'Christian Bauer', 'Steven Greenhill', 'Rainer Schroeder', 'Frank Launspach', 'Christian Ziegler', 'Pascal Borusiak', 'Marcel Geisen', 'Thomas Lohmann', 'Nico Bernhardt', 'Steffen Kron', 'Juan Bueno', 'Daniel Dittmann', 'Richard Spengler', 'Yoko Igarashi', 'Christoph Gote', 'Nicole Kost', 'Emanuel Stuebner', 'Andre Prosen', 'Edgar Minch', 'Andre Ohmen', 'Lejla Salievska', 'Christian Rotter', 'Stephanie Tschunt', 'Christian-Alexander Krebs', 'Joerg Kohlbacher', 'Bettina Fink', 'Jennifer Moreno-Barrientos', 'Alexander Schur', 'Markus Schroeder', 'Stefan Ries', 'Walter Mohr', 'Anja Pistner', 'Bjoern Stoll', 'Juergen Puscher', 'Florian Auth', 'Paulo Mesquita', 'Michael Kraus', 'Kai Schneider', 'Daniel Farani', 'Steven Greenhill', 'R</t>
+  </si>
+  <si>
+    <t>['Victor Dahnovici', 'Nick Tiloi', 'Dana Bajanaru', 'Valeria Dima', 'Radita Goaga', 'Andreea Ivasca', 'Mihaela Adam', 'Laurentiu Veres', 'Nick Tiloi', 'Ana Maria Bizdoaca', 'Victor Dahnovici', 'Alexandru Diaconu', 'Cristina Vacaroiu', 'Nick Tiloi', 'Mirona Cristache', 'Mirela Bumbea', 'Razvan Radu', 'Daniel Cirstea', 'Nick Tiloi', 'Dana Bajanaru', 'Iudith Dobre', 'Andrei Szekely', 'Tiberiu Maris', 'Mihai Teodorescu', 'Nick Tiloi', 'Nick Tiloi', 'Elena Florea', 'Victor Dahnovici', 'Cristian Sirman', 'Dragos Gheorghe', 'Andrei Gorgan', 'Bogdan Popa', 'Costel Roscan', 'Mihaela Croitoru', 'Nick Tiloi', 'Dana Bajanaru', 'Laurentiu Veres', 'Nick Tiloi', 'Adriana Muresan', 'Dana Bajanaru', 'Nick Tiloi', 'Mirela Bumbea', 'Andreea Ivasca', 'Nick Tiloi', 'Arnold Sztratya', 'Adrian Musat', 'Andra Cristea', 'Adriana Muresan', 'Dan Mali', 'Dorin Flueras', 'Vasile Popa', 'Ana Maria Bizdoaca', 'Ovidiu Cristea', 'Gabriela Timbuli', 'Dana Bajanaru', 'Florin Simion', 'Cristina Moisa', 'Cristian Ciontescu', 'Laurentiu Veres', 'Iudith Dobre', 'Alexandru Murasan', 'Ramona Dan', 'Eugen Stan', 'Mirona Cristache', 'Alexandru Stoican', 'Alexandru Marinescu', 'Radu Lesan', 'Elena Florea', 'Anamaria-Cristina Zanciu', 'Alexandra Barbu-Gorea', 'BÃ©la SzÃ©kely', 'Cristian Sirman', 'Gabriel Gheorghiu', 'Lucia Tudorescu', 'Davide Basta', 'Ionut Badescu', 'Marius Marica', 'Mihai Marchis', 'Camelia Turturica', 'Andrei Szekely', 'Flavius Pardos', 'Victor Dahnovici', 'Dragos Gheorghe', 'Cristian Maria', 'Emanuel Bac', 'Maxim Savca', 'George Turculet', 'Cosmin Jipa', 'Bogdan Groza', 'Tiberiu Maris', 'Adrian Toghe', 'Valeria Dima', 'Carmen Ghebeles', 'Alexandru Gheorghe', 'George Marin', 'Adrian Mihalcea', 'Mirela Bumbea', 'Gabriel Mihaila', 'Robert Szucs', 'Alexandru Grigore', "Walter D'Alessandro", 'Radita Goaga', 'Ciprian Livint', 'Mihaela Croitoru', 'Camelia Greconici', 'Cristian Badea', 'Cristina Guga', 'Alexandru Maris', 'Dan Savulovici', 'Alexandru Diaconu', 'Damaris Muresan', 'Alexandru Mihalcea', 'Cristina Mantaluta', 'Adelina Constantinescu', 'Valeriu Banu', 'Mihai Dumitru', 'Gener Temerbec', 'Alexandru Bobilca', 'Daniel Zahorte', 'Mihai Teodorescu', 'Vlad Vascan', 'Gabriel Aenoaei', 'Andrei Gorgan', 'Andreea Ivasca', 'Cristina Vacaroiu', 'Adrian Soare', 'Bogdan Popa', 'Razvan Radu', 'Corina Sas', 'Mihaela Adam', 'Catalin Mazilu', 'Eduard Cucu', 'Gabriel Micu', 'Mircea Ardeiu', 'Costel Roscan', 'Andrei Gheoca', 'Daniel Cirstea', 'Horatiu Preda', 'Cristian David', 'Elena Florea', 'Dana Bajanaru', 'Adriana Muresan', 'Mirona Cristache', 'Damaris Muresan']</t>
+  </si>
+  <si>
+    <t>['Vratislav Stanek', 'Zdenek Velfl', 'Jiri Jasik', 'Martin Vicar', 'Ludmila Latalova', 'Martin Vicar', 'Jiri Tvrdy', 'Bronislav Blaha', 'Jiri Zavrel', 'ex_P.Taus@smc.cz', 'Jiri Kolar', 'Jan Kalvoda', 'Mario Jakubec', 'Klara Horackova', 'Katerina Heilerova', 'Michaela Koerberova', 'Martin Neuhauser', 'Andrea Kolackova', 'Petr Cecak', 'Jan Tomko', 'Marek Strojil', 'Ondrej Moldan', 'Jiri Tvrdy', 'Karel Soukup', 'Jiri Kolar', 'Jiri Jasik', 'Katerina Fialova', 'Petr Safarik', 'Jiri Vesely', 'Pavel Prochazka', 'Vlastimil Lakomy', 'Petr Belohradsky', 'Jiri Zavrel', 'Jiri Hudec', 'Petr Belohradsky', 'Jiri Neuhauser', 'Petr Hettner', 'Jiri Seps', 'Jan Smidek', 'Jiri Kolar', 'Vratislav Stanek', 'Jiri Tvrdy', 'Klara Horackova', 'Jiri Tvrdy', 'Karel Soukup', 'Bronislav Blaha', 'Jiri Zavrel', 'Jiri Hudec', 'Vlastimil Lakomy', 'Jan Sigut', 'Martin Skranc', 'Petr Belohradsky', 'Martin Janacek', 'Zdenek Varmuza', 'Karel Soukup', 'Vratislav Stanek', 'Pavel Sedlacek', 'Vratislav Stanek', 'Josef Racansky', 'Klara Horackova', 'Jozef Mikus', 'Katerina Heilerova', 'Marek Vidlak', 'Katarina Kurillova', 'Martin Pabiska', 'Tomas Pribilik', 'Tomas Mlcousek', 'Ondrej Zidlicky', 'Alena Petrickova', 'David Kutalek', 'Jiri Klima', 'Petr Kremz', 'Radim Fridrich', 'Petra Novotna', 'Daniel Zurek', 'Jiri Vesely', 'Klara Horackova', 'Katerina Heilerova', 'Jiri Tvrdy', 'Jiri Kolar', 'Jiri Tvrdy', 'Jiri Kolar', 'Jozef Mikus', 'Katerina Chaloupkova', 'Jiri Neuhauser', 'Petr Hettner', 'Jiri Seps', 'Jan Smidek', 'Klara Horackova', 'Karel Prochazka', 'Ondrej Moldan', 'Jiri Tvrdy', 'Jiri Kolar', 'Pavel Sedlacek', 'Jarmila Spacilova', 'Jan Kalvoda', 'Mario Jakubec', 'Vratislav Stanek', 'Klara Horackova', 'Jozef Mikus', 'Tomas Pelikan', 'Katerina Heilerova', 'Marketa Sedlakova', 'Alena Petrickova', 'Radim Fridrich', 'Zdenek Velfl', 'Jan Sigut', 'Pavel Sedlacek', 'Jiri Tvrdy', 'Jiri Kolar', 'Jan Kalvoda', 'Mario Jakubec', 'Vratislav Stanek', 'Ales Turecek', 'Klara Horackova', 'Jozef Mikus', 'Marketa Sedlakova', 'Monika Spicakova', 'Alena Petrickova', 'Radim Fridrich', 'Martin Vicar', 'Maria Rolkova', 'Hana Wichova', 'Jiri Zavrel', 'Martin Skranc', 'Jiri Zavrel', 'Vratislav Stanek']</t>
+  </si>
+  <si>
+    <t>['Robert Angel', 'Christian Platz', 'Thomas Handlinger', 'Markus Fasching', 'Christoph Krydl', 'Maximilian Svatek', 'Miroslav Gawron', 'Bernhard Schwalm', 'Clemens Doppler', 'Sabrina Jatschka', 'Martina Hoeller', 'Ursula Hartweger-Vogl', 'Stefan Bischof', 'Simone Gruber', 'Ernst Schneider', 'Christine Jatschka', 'Manjit Arora', 'warehouse 3.', 'Monika Schrenk', 'Stefan Janotta', 'Christoph Krydl', 'Dominic Petri', 'Anna Haibl', 'Bernhard Fenz', 'Andreas Zussner', 'Ulrike Stanzer', 'ex_b.karner@smc.at', 'Marcus Kohlbeck', 'Ernst Schneider', 'Christine Jatschka', 'warehouse 3.', 'Matthias Reimitz', 'Christiane Serobanyane', 'ex_J.Lang@smc.at', 'Sabrina Jatschka', 'Daniel Bauer', 'Angelika Eichinger', 'Bernhard Heigl', 'Nathalie Mader', 'Simone Gruber', 'Tamara Judex', 'Rainer Sendlinger', 'Christoph Krydl', 'Ursula Hartweger-Vogl', 'Bernhard Umgeher', 'Alexander Elsinger', 'Sabrina Chrpa', 'Angelika Eichinger', 'Daniela Sefzig', 'Florian Gruber', 'Stefan Leis', 'Stefan Herzig', 'Nick NE. Ehrenstrasser', 'Miroslav Gawron', 'ex_A.Czezatke@smc.at', 'Clemens Doppler', 'Alexander Elsinger', 'Claudia Hoedl', 'Markus Platz', 'Elisabeth Wenzl', 'Rainer Lehner', 'Andreas Hanifl', 'Tomas Ruzicka', 'Miroslav Gawron', 'Raul Lucescu', 'Stephan Maurer', 'Katharina Yassemipour', 'Martin Winklmueller', 'Mathilde Spacek', 'Johannes Schwarz', 'Maximilian Svatek', 'Ulrich Reisenbauer', 'Christoph Krydl', 'Michael Miller', 'Ursula Hartweger-Vogl', 'Stefan Bischof', 'Claudia Litschauer', 'Bettina Fauster', 'Andreas Zussner', 'Istvan Barat', 'David Postl', 'Lars Unterberger', 'Michael Sala', 'Grygorii Gaidukevych', 'ex_g.strem@smc.at', 'Ernst Schneider', 'Markus Schulz', 'Gerald Rammel', 'ex_Ch.Litschauer@smc.at', 'Barbara Eggenhofer', 'Vesna Klicic', 'Marcus Kohlbeck', 'Gernot Hombrecher', 'Norbert Schneider', 'Anna Haibl', 'Sabrina Jatschka', 'Raul Lucescu', 'Andreas Konstanda', 'Bettina Fauster', 'Alfred Trappl', 'Daniel Bauer', 'Claudia Hoedl', 'Dietmar Lanzersdorfer', 'Tanja Scheiner', 'Andreas Schratzberger', 'Richard Schoelzhorn', 'Josef Rieder', 'Marcus Kohlbeck', 'Clemens Doppler', 'Bettina Fauster', 'Peter Ladler', 'Markus Platz', 'Marcus Kohlbeck', 'Clemens Doppler', 'Alexander Hofbauer', 'Alexander Elsinger', 'Istvan Barat', 'Stephan Maurer', 'Marcus Kohlbeck', 'Clemens Doppler', 'ex_A.Czezatke@smc.at', 'Clemens Doppler', 'Alexander Elsinger', 'Maximilian Svatek', 'Daniela Sefzig', 'Florian Gruber', 'Stefan Leis', 'Stefan Herzig', 'ex_p.wotawa@smc.at', 'Guenther Paller', 'Matthias Zeman', 'Michal Marienka', 'ex_E.Marek@smc.at', 'Gerald Rammel', 'Benedikt Halwidl', 'ex_c.dittrich@smc.at', 'Miroslav Gawron', 'Bernhard Schwalm', 'Manfred Bauer', 'Ramy Mikhael', 'ex_Ch.Litschauer@smc.at', 'Vesna Klicic', 'Damir Sikiric', 'Gerhard Boehm', 'Stefan Langgartner', 'Dominic Petri', 'Marcus Kohlbeck', 'Norbert Schneider', 'Clemens Doppler', 'Alexander Hofbauer', 'Anna Haibl', 'Sabrina Jatschka', 'Raul Lucescu', 'Manfred Anfang', 'Alexander Elsinger', 'Bettina Fauster', 'Thomas Wyt', 'Martina Hoeller', 'Nick NE. Ehrenstrasser', 'Clemens Doppler', 'Alexander Hofbauer', 'Raul Lucescu', 'Katharina Yassemipour', 'Sabrina Jatschka', 'Christian Platz', 'Ernst Schneider', 'Ursula Hartweger-Vogl', 'Stefan Bischof', 'Claudia Litschauer', 'Clement Pucher', 'Bernhard Schwalm', 'Marcus Kohlbeck', 'Alexander Elsinger', 'Martin Winklmueller', 'Mathilde Spacek', 'Martin Schuh', 'Robert Angel', 'Christian Platz', 'Martin Schuh', 'Gernot Galler', 'Lars Unterberger', 'Michael Sala', 'Clement Pucher', 'Marcus Kohlbeck', 'Manfred Anfang', 'Bettina Fauster', 'Christoph Krydl', 'Robert Angel', 'Markus Schulz', 'Maximilian Svatek', 'Monika Schrenk', 'Ursula Hartweger-Vogl', 'Claudia Litschauer', 'Robert Angel', 'Istvan Barat', 'Tomas Ruzicka', 'Tom TRtst. Ruzicka', 'Peter Strubl', 'Andreas Hanifl', 'Marcus Ott', 'Istvan Barat', 'Tomas Ruzicka', 'Rainer Lehner', 'Rainer Lehner', 'Robert Angel', 'Stephan Maurer', 'Markus Schulz', 'Christian Paulhart', 'Peter Pichler', 'Katharina Yassemipour', 'Johannes Schwarz', 'Rainer Sendlinger', 'Maximilian Svatek', 'Monika Schrenk', 'Gabriele Kohlbeck', 'Christoph Krydl', 'Ursula Hartweger-Vogl', 'Daniel Bauer', 'Istvan Barat', 'Istvan Barat', 'Maximilian Svatek', 'Christine Jatschka', 'Clement Pucher', 'Florian Papai', 'ex_c.kraft@smc.at', 'Rainer Sendlinger', 'Gerhard Boehm', 'Monika Schrenk', 'Petra Pichler-Gruenbeck', 'Bernhard Heigl', 'Andreas Zussner', 'Istvan Barat', 'Daniel Bauer', 'Christoph Rapf', 'Georg Egelwolf', 'Juergen Hrabak', 'Patrick Holzer', 'Petra Pichler-Gruenbeck', 'Matthias Reimitz', 'Alexander Elsinger', 'Matthias Reimitz', 'Claudia Litschauer', 'Ernst Schneider', 'Christine Jatschka', 'Manjit Arora', 'warehouse 3.', 'Monika Schrenk', 'Gerald Friczmann', 'Birgit Liebhart-Stojic', 'ex_J.Lang@smc.at', 'Daniel Bauer', 'Jozsef Icsei', 'ex_b.karner@smc.at', 'Roman Schoen', 'Istvan Barat', 'Sabrina Jatschka', 'ex_p.wotawa@smc.at', 'Benedikt Halwidl', 'Clement Pucher', 'Marcus Kohlbeck', 'Clemens Doppler', 'Bettina Fauster', 'ex_p.wotawa@smc.at', 'Benedikt Halwidl', 'Clement Pucher', 'ex_c.sperling@smc.at', 'Ramy Mikhael', 'Marcus Kohlbeck', 'Petra Pichler-Gruenbeck', 'Alexander Hofbauer', 'Bernhard Heigl', 'Evelin Puck', 'Simone Gruber', 'Petra Thienel', 'Evelyn Brait', 'Martha Lehner', 'Dagmar Billek', 'Karin Gassner', 'Robert Angel', 'Ernst Schneider', 'Christine Jatschka', 'Stefan Bischof', 'ex_J.Lang@smc.at', 'Miroslav Gawron', 'ex_A.Czezatke@smc.at', 'Stefan Bischof', 'Christoph Rapf', 'Daniel Bauer', 'Werner Ripplinger', 'Martina Hoeller', 'Rainer Sendlinger', 'Robert Rudolph', 'Claudia Litschauer', 'Petra Pichler-Gruenbeck', 'Manfred Anfang', 'ex_L.Pfeiffer@smc.at', 'Michael Grinninger', 'Martina Auer', 'Pamela Pistracher', 'Matthias Reimitz', 'Bernhard Umgeher', 'Elisabeth Heinrich', 'Karl Eisner', 'Stefan Janotta', 'Verena Eigl', 'Sonja Esberger', 'Manuela Penner', 'Johanna Neulinger']</t>
+  </si>
+  <si>
+    <t>['Stig Grani', 'Stig Grani', 'Mir Karim', 'Mir Karim', 'Stig Grani', 'Anita FrÃ¸yset', 'Stig Grani', 'Olav Andre Ã˜ren Karlsen', 'Stig Grani', 'Stig Grani', 'Anton Tjernlund', 'Anis Sadiq', 'Fredrik Roaldstveit', 'Mikis Michael', 'Mir Karim', 'Jan Ã…ge BrattÃ¥s', 'Anita FrÃ¸yset', 'Olav Andre Ã˜ren Karlsen', 'Fredrik Ryslett', 'Marcus Kolberg', 'Trond L. Gulliksen', 'Stig Grani', 'Stig Grani', 'Stig Grani', 'Trond L. Gulliksen', 'Anita FrÃ¸yset']</t>
+  </si>
+  <si>
+    <t>['Filip Koziol', 'Marek Jarzebowski', 'Rafal Szulc', 'Antoni Szczechura', 'Antoni Szczechura', 'Katarzyna Pawlowska', 'Maciej Roczkalski', 'ex_K.Sitek@smc.pl', 'Martyna Bucikiewicz', 'Krzysztof Szczesny', 'Piotr Guzy', 'Piotr Kruk', 'Radoslaw Mendon', 'Pawel Kaminski', 'Norbert Pieniak', 'Arkadiusz Szelag', 'Pawel Broda', 'Radoslaw Mendon', 'Pawel Borowiec', 'Mateusz Kedzierski', 'Pawel Nowak', 'Rafal Szulc', 'Katarzyna Pawlowska', 'Damian Kedziorek']</t>
+  </si>
+  <si>
+    <t>['Kristian Filyovski', 'Petar Mlekarov', 'Elena Grigorova', 'ex_S.Marinkev@smc.bg', 'Petar Mlekarov', 'Asen Georgiev', 'Plamen Turkedjiev', 'Veselin Bozov', 'Nedko Petrov', 'Elena Grigorova', 'Hristo Krastev']</t>
+  </si>
+  <si>
+    <t>['Tomas Somjak', 'Alena Brezianska', 'Tomas Somjak', 'Alena Brezianska', 'Martin Holonka', 'Matej Ottava', 'Roman Gawron', 'Kristian Kavuliak', 'Kristian Oros', 'Pavel Kovac', 'Jozef Rusnak', 'Roman Gawron', 'Matej Ottava', 'Marian Palenik', 'Filip Soska', 'Kristian Oros', 'Zuzana Palatkova', 'Miroslav Holonka', 'Roman Gawron', 'Tomas Somjak', 'Tomas Somjak', 'Ivana Strauchova']</t>
+  </si>
+  <si>
+    <t>['Marjan Matoh', 'Bostjan Zitnik', 'Bostjan Zitnik', 'Martina Jevsevar', 'Otmar Fafulic', 'Zvone Matoh', 'Viljem Bozic', 'Ales Matko', 'Jan Matko', 'Brigita Lokar', 'Ales Matko']</t>
+  </si>
+  <si>
+    <t>['Ivan Herceg', 'Marjan Vlahovic', 'Ivan Herceg']</t>
+  </si>
+  <si>
+    <t>['Andras Liskany', 'Peter Csete', 'Peter Csete', 'Zsuzsanna Gergete', 'Sandor Kajari', 'Botond Biro', 'Beata Molnar', 'Ildiko Vargane Voller', 'Tibor Taksonyi', 'Richard Bajzak', 'Tamas Kiss', 'Tibor Fil', 'Andras Liskany', 'Emese Ipolyi', 'Peter Csete', 'Zsigmond Nagy']</t>
+  </si>
+  <si>
+    <t>['Branislav Lackovic']</t>
+  </si>
+  <si>
+    <t>['Anastasija Bartkevica', 'Janis Hohbergs', 'Guntis Karklins', 'Guntis Karklins', 'Guntis Karklins', 'Maris Kjakste', 'Egils Lieknins', 'Guntis Karklins', 'Janis Hohbergs', 'Guntis Karklins', 'Egils Lieknins', 'Guntis Karklins', 'Alvis Dubovs', 'Rihards Tarvids', 'Maris Lukasevics', 'Janis Hohbergs', 'Ainars Tucins', 'Anastasija Bartkevica', 'Haralds Pauls', 'Kristofors Elbers-Karklins', 'Serafima Kiselyova', 'Maris Kjakste', 'Kristaps Logins', 'Roberts SkadiÅ†Å¡', 'Svetlana Jedzijeva', 'Kristaps Pidiks', 'Natalja Kirjakova', 'BSC', 'Oskars PurinÅ¡', 'Iveta Plaude', 'Reinis Kutris', 'Egils Lieknins', 'Serafima Kiselyova']</t>
+  </si>
+  <si>
+    <t>['Unai GarcÃ\xada de VicuÃ±a (Admin)', 'Unai GarcÃ\xada de VicuÃ±a (Admin)', 'Unai GarcÃ\xada de VicuÃ±a (Admin)', 'Unai GarcÃ\xada de VicuÃ±a (Admin)', 'Unai GarcÃ\xada de VicuÃ±a (Admin)', 'Unai GarcÃ\xada de VicuÃ±a (Admin)', 'Unai GarcÃ\xada de VicuÃ±a (Admin)']</t>
+  </si>
+  <si>
+    <t>['Eleazar Marbach Test DE1']</t>
+  </si>
+  <si>
+    <t>['Marius Lipnickas', 'Marius Lipnickas', 'Evaldas Å½vejys', 'DovilÄ— MaÄ\x8diulienÄ—', 'DovilÄ— MaÄ\x8diulienÄ—', 'Giedrius Senovaitis', 'Marius Lipnickas', 'Paulius Urbonas', 'Antanas Zaliks', 'Tomas Nutautas', 'Vladimir Noskov', 'Evaldas Å½vejys', 'Marius Lipnickas', 'Vladimir Noskov', 'Evaldas Å½vejys', 'Vladimir Noskov']</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +237,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,92 +561,204 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="n">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>SharePoint Backups 1SMCEMEA.onmicrosoft.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SharePoint Backups 1SMCEMEA.onmicrosoft.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SharePoint Backups 1SMCEMEA.onmicrosoft.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SharePoint Backups 1SMCEMEA.onmicrosoft.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SharePoint Backups 1SMCEMEA.onmicrosoft.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SharePoint Backups 1SMCEMEA.onmicrosoft.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SharePoint Backups 1SMCEMEA.onmicrosoft.com</t>
-        </is>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final version with .exe
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kizan-my.sharepoint.com/personal/julian_heidt_kizan_com/Documents/Documents/Code/Scott's shit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_172D6CC783422E32471B2911595ED87656C70E5E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{813EE455-DD96-4FCB-98BE-4342AB27E556}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_172D6CC783E22972BFF82D11595ED87656C70E5E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{248E2400-C1D0-4283-BBCA-70A4DAC66FBC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7747,7 +7747,7 @@
   <dimension ref="A1:ZH31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
error on line 88, comment above it.
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D241"/>
+  <dimension ref="A1:C241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,9 +440,6 @@
       <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -457,12 +454,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EMC-Safety</t>
         </is>
       </c>
     </row>
@@ -479,12 +471,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Operations</t>
         </is>
       </c>
     </row>
@@ -501,12 +488,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EMC-Safety</t>
         </is>
       </c>
     </row>
@@ -523,12 +505,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU6+2</t>
         </is>
       </c>
     </row>
@@ -545,12 +522,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EMC-Safety</t>
         </is>
       </c>
     </row>
@@ -567,12 +539,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-IT-Firewall Refresh Project (GB &amp; IE)</t>
         </is>
       </c>
     </row>
@@ -589,12 +556,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-IT-Firewall Refresh Project (GB &amp; IE)</t>
         </is>
       </c>
     </row>
@@ -611,12 +573,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-Marel-All</t>
         </is>
       </c>
     </row>
@@ -633,12 +590,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Accounts</t>
         </is>
       </c>
     </row>
@@ -655,12 +607,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Accounts</t>
         </is>
       </c>
     </row>
@@ -677,12 +624,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Accounts</t>
         </is>
       </c>
     </row>
@@ -699,12 +641,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB Sales Managers' Comms</t>
         </is>
       </c>
     </row>
@@ -721,12 +658,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-OcadoWinTeam</t>
         </is>
       </c>
     </row>
@@ -743,12 +675,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Logistics</t>
         </is>
       </c>
     </row>
@@ -765,12 +692,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>IE-FileTransfer</t>
         </is>
       </c>
     </row>
@@ -787,12 +709,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-Sales-AA40</t>
         </is>
       </c>
     </row>
@@ -809,12 +726,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA20</t>
         </is>
       </c>
     </row>
@@ -831,12 +743,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA20</t>
         </is>
       </c>
     </row>
@@ -853,12 +760,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA20</t>
         </is>
       </c>
     </row>
@@ -875,12 +777,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EMC-Proof-Reading</t>
         </is>
       </c>
     </row>
@@ -897,12 +794,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-IT-Firewall Refresh Project (GB &amp; IE)</t>
         </is>
       </c>
     </row>
@@ -919,12 +811,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EC1T - Mechatronic &amp; Network</t>
         </is>
       </c>
     </row>
@@ -941,12 +828,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EC1T - Mechatronic &amp; Network</t>
         </is>
       </c>
     </row>
@@ -963,12 +845,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-IT-JapanADServer</t>
         </is>
       </c>
     </row>
@@ -985,12 +862,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EIT-RPA Project</t>
         </is>
       </c>
     </row>
@@ -1007,12 +879,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-IT</t>
         </is>
       </c>
     </row>
@@ -1029,12 +896,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-ASM-Labels</t>
         </is>
       </c>
     </row>
@@ -1051,12 +913,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-Sales-AC10</t>
         </is>
       </c>
     </row>
@@ -1073,12 +930,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EMC-EU6 Product Management team</t>
         </is>
       </c>
     </row>
@@ -1095,12 +947,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>IE-FileTransfer</t>
         </is>
       </c>
     </row>
@@ -1117,12 +964,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU6+2</t>
         </is>
       </c>
     </row>
@@ -1139,12 +981,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Operations</t>
         </is>
       </c>
     </row>
@@ -1161,12 +998,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>EU-ERP Support</t>
         </is>
       </c>
     </row>
@@ -1183,12 +1015,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-Manufacturing-Team</t>
         </is>
       </c>
     </row>
@@ -1205,12 +1032,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EIT-Internal Control</t>
         </is>
       </c>
     </row>
@@ -1227,12 +1049,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -1249,12 +1066,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-Manufacturing-Team</t>
         </is>
       </c>
     </row>
@@ -1271,12 +1083,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ERP Support</t>
         </is>
       </c>
     </row>
@@ -1293,12 +1100,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-Sales-EDGFocusGroup</t>
         </is>
       </c>
     </row>
@@ -1315,12 +1117,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF50</t>
         </is>
       </c>
     </row>
@@ -1337,12 +1134,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF40</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1151,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF50</t>
         </is>
       </c>
     </row>
@@ -1381,12 +1168,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB40</t>
         </is>
       </c>
     </row>
@@ -1403,12 +1185,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF40</t>
         </is>
       </c>
     </row>
@@ -1425,12 +1202,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB40</t>
         </is>
       </c>
     </row>
@@ -1447,12 +1219,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF40</t>
         </is>
       </c>
     </row>
@@ -1469,12 +1236,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EIT-Reporting</t>
         </is>
       </c>
     </row>
@@ -1491,12 +1253,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ASM-Labels</t>
         </is>
       </c>
     </row>
@@ -1513,12 +1270,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-Sales-AB50</t>
         </is>
       </c>
     </row>
@@ -1535,12 +1287,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsManagement</t>
         </is>
       </c>
     </row>
@@ -1557,12 +1304,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsDesign</t>
         </is>
       </c>
     </row>
@@ -1579,12 +1321,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsDesign</t>
         </is>
       </c>
     </row>
@@ -1601,12 +1338,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsEngineering</t>
         </is>
       </c>
     </row>
@@ -1623,12 +1355,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsDesign</t>
         </is>
       </c>
     </row>
@@ -1645,12 +1372,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsDesign</t>
         </is>
       </c>
     </row>
@@ -1667,12 +1389,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsDesign</t>
         </is>
       </c>
     </row>
@@ -1689,12 +1406,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsDesign</t>
         </is>
       </c>
     </row>
@@ -1711,12 +1423,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsDesign</t>
         </is>
       </c>
     </row>
@@ -1733,12 +1440,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsDesign</t>
         </is>
       </c>
     </row>
@@ -1755,12 +1457,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsEngineering</t>
         </is>
       </c>
     </row>
@@ -1777,12 +1474,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegionalSalesPR</t>
         </is>
       </c>
     </row>
@@ -1799,12 +1491,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-Instrumentation-FluidControl</t>
         </is>
       </c>
     </row>
@@ -1821,12 +1508,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>IE-FileTransfer</t>
         </is>
       </c>
     </row>
@@ -1843,12 +1525,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-Accounts</t>
         </is>
       </c>
     </row>
@@ -1865,12 +1542,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Accounts</t>
         </is>
       </c>
     </row>
@@ -1887,12 +1559,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>CH-IT-MarbachTest</t>
         </is>
       </c>
     </row>
@@ -1909,12 +1576,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EC1T - Mechatronic &amp; Network</t>
         </is>
       </c>
     </row>
@@ -1931,12 +1593,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-GTAP-Team</t>
         </is>
       </c>
     </row>
@@ -1953,12 +1610,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsEngineering</t>
         </is>
       </c>
     </row>
@@ -1975,12 +1627,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>EU-ETC-ActuatorsManagement</t>
         </is>
       </c>
     </row>
@@ -1997,12 +1644,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EIT-RPA Project</t>
         </is>
       </c>
     </row>
@@ -2019,12 +1661,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsEngineering</t>
         </is>
       </c>
     </row>
@@ -2041,12 +1678,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-GTAP-Team</t>
         </is>
       </c>
     </row>
@@ -2063,12 +1695,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EIT-RPA Project</t>
         </is>
       </c>
     </row>
@@ -2085,12 +1712,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EC1T - Mechatronic &amp; Network</t>
         </is>
       </c>
     </row>
@@ -2107,12 +1729,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Operations</t>
         </is>
       </c>
     </row>
@@ -2129,12 +1746,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EIT-eWorkplace</t>
         </is>
       </c>
     </row>
@@ -2151,12 +1763,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EIT-RPA Project</t>
         </is>
       </c>
     </row>
@@ -2173,12 +1780,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA40</t>
         </is>
       </c>
     </row>
@@ -2195,12 +1797,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsEngineering</t>
         </is>
       </c>
     </row>
@@ -2217,12 +1814,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EIT-RPA Project</t>
         </is>
       </c>
     </row>
@@ -2239,12 +1831,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-Manufacturing-Team</t>
         </is>
       </c>
     </row>
@@ -2261,12 +1848,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Logistics</t>
         </is>
       </c>
     </row>
@@ -2283,12 +1865,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -2305,12 +1882,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -2327,12 +1899,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Zendesk-GB-IE-ZA</t>
         </is>
       </c>
     </row>
@@ -2349,12 +1916,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-SalesEngineering</t>
         </is>
       </c>
     </row>
@@ -2371,12 +1933,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-CovidTeam</t>
         </is>
       </c>
     </row>
@@ -2393,12 +1950,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Operations</t>
         </is>
       </c>
     </row>
@@ -2415,12 +1967,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Quality</t>
         </is>
       </c>
     </row>
@@ -2437,12 +1984,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-KeyAccountsPR</t>
         </is>
       </c>
     </row>
@@ -2459,12 +2001,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-MentorPilot</t>
         </is>
       </c>
     </row>
@@ -2481,12 +2018,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EMC-DT Project</t>
         </is>
       </c>
     </row>
@@ -2503,12 +2035,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>EU-ETC-ActuatorsEngineering</t>
         </is>
       </c>
     </row>
@@ -2525,12 +2052,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>EU-ETC-ActuatorsEngineering</t>
         </is>
       </c>
     </row>
@@ -2547,12 +2069,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-Manufacturing-Team</t>
         </is>
       </c>
     </row>
@@ -2569,12 +2086,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionEngineering</t>
         </is>
       </c>
     </row>
@@ -2591,12 +2103,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionEngineering</t>
         </is>
       </c>
     </row>
@@ -2613,12 +2120,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionEngineering</t>
         </is>
       </c>
     </row>
@@ -2635,12 +2137,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionEngineering</t>
         </is>
       </c>
     </row>
@@ -2657,12 +2154,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionEngineering</t>
         </is>
       </c>
     </row>
@@ -2679,12 +2171,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionEngineering</t>
         </is>
       </c>
     </row>
@@ -2701,12 +2188,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionEngineering</t>
         </is>
       </c>
     </row>
@@ -2723,12 +2205,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionEngineering</t>
         </is>
       </c>
     </row>
@@ -2745,12 +2222,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-GTAP-Team</t>
         </is>
       </c>
     </row>
@@ -2767,12 +2239,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-Marel-All</t>
         </is>
       </c>
     </row>
@@ -2789,12 +2256,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AC20</t>
         </is>
       </c>
     </row>
@@ -2811,12 +2273,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AC20</t>
         </is>
       </c>
     </row>
@@ -2833,12 +2290,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ECG-European-Chiller-Group</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2307,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-SalesEngineering</t>
         </is>
       </c>
     </row>
@@ -2877,12 +2324,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-SalesEngineering</t>
         </is>
       </c>
     </row>
@@ -2899,12 +2341,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-SalesEngineering</t>
         </is>
       </c>
     </row>
@@ -2921,12 +2358,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-SalesEngineering</t>
         </is>
       </c>
     </row>
@@ -2943,12 +2375,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-PM-WorkingGroup-Vaccum</t>
         </is>
       </c>
     </row>
@@ -2965,12 +2392,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-SalesEngineering</t>
         </is>
       </c>
     </row>
@@ -2987,12 +2409,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ECG-European-Chiller-Group</t>
         </is>
       </c>
     </row>
@@ -3009,12 +2426,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-SalesEngineering</t>
         </is>
       </c>
     </row>
@@ -3031,12 +2443,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-SalesEngineering</t>
         </is>
       </c>
     </row>
@@ -3053,12 +2460,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ECG-European-Chiller-Group</t>
         </is>
       </c>
     </row>
@@ -3075,12 +2477,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA40</t>
         </is>
       </c>
     </row>
@@ -3097,12 +2494,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-Sales-AC40</t>
         </is>
       </c>
     </row>
@@ -3119,12 +2511,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AC40</t>
         </is>
       </c>
     </row>
@@ -3141,12 +2528,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AC40</t>
         </is>
       </c>
     </row>
@@ -3163,12 +2545,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>IE-FileTransfer</t>
         </is>
       </c>
     </row>
@@ -3185,12 +2562,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-IT-Test</t>
         </is>
       </c>
     </row>
@@ -3207,12 +2579,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-KeyAccountsPR</t>
         </is>
       </c>
     </row>
@@ -3229,12 +2596,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>SE-UK-Mycronic</t>
         </is>
       </c>
     </row>
@@ -3251,12 +2613,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-IT-MobilePhoneContract</t>
         </is>
       </c>
     </row>
@@ -3273,12 +2630,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-Manufacturing-Team</t>
         </is>
       </c>
     </row>
@@ -3295,12 +2647,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsEngineering</t>
         </is>
       </c>
     </row>
@@ -3317,12 +2664,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-ActuatorsEngineering</t>
         </is>
       </c>
     </row>
@@ -3339,12 +2681,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB30</t>
         </is>
       </c>
     </row>
@@ -3361,12 +2698,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB30</t>
         </is>
       </c>
     </row>
@@ -3383,12 +2715,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionControl</t>
         </is>
       </c>
     </row>
@@ -3405,12 +2732,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionControl</t>
         </is>
       </c>
     </row>
@@ -3427,12 +2749,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionControl</t>
         </is>
       </c>
     </row>
@@ -3449,12 +2766,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionControl</t>
         </is>
       </c>
     </row>
@@ -3471,12 +2783,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-ProductionControl</t>
         </is>
       </c>
     </row>
@@ -3493,12 +2800,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-IT-Test</t>
         </is>
       </c>
     </row>
@@ -3515,12 +2817,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EIT-Reporting</t>
         </is>
       </c>
     </row>
@@ -3537,12 +2834,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3559,12 +2851,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>EU-ETC-AdminGroup</t>
         </is>
       </c>
     </row>
@@ -3581,12 +2868,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>EU-ETC-AdminGroup</t>
         </is>
       </c>
     </row>
@@ -3603,12 +2885,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AdminGroup</t>
         </is>
       </c>
     </row>
@@ -3625,12 +2902,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AdminGroup</t>
         </is>
       </c>
     </row>
@@ -3647,12 +2919,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AdminGroup</t>
         </is>
       </c>
     </row>
@@ -3669,12 +2936,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AdminGroup</t>
         </is>
       </c>
     </row>
@@ -3691,12 +2953,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-IT-MobilePhoneContract</t>
         </is>
       </c>
     </row>
@@ -3713,12 +2970,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Operations</t>
         </is>
       </c>
     </row>
@@ -3735,12 +2987,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3757,12 +3004,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3779,12 +3021,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3801,12 +3038,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3823,12 +3055,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3845,12 +3072,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D156" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3867,12 +3089,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3889,12 +3106,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D158" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3911,12 +3123,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3933,12 +3140,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D160" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3955,12 +3157,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D161" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3977,12 +3174,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GBâ€“DesignEngineering</t>
         </is>
       </c>
     </row>
@@ -3999,12 +3191,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF20</t>
         </is>
       </c>
     </row>
@@ -4021,12 +3208,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF30</t>
         </is>
       </c>
     </row>
@@ -4043,12 +3225,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Facilities</t>
         </is>
       </c>
     </row>
@@ -4065,12 +3242,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D166" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-GDPR-Workgroup</t>
         </is>
       </c>
     </row>
@@ -4087,12 +3259,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB20</t>
         </is>
       </c>
     </row>
@@ -4109,12 +3276,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB20</t>
         </is>
       </c>
     </row>
@@ -4131,12 +3293,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB50</t>
         </is>
       </c>
     </row>
@@ -4153,12 +3310,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D170" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF50</t>
         </is>
       </c>
     </row>
@@ -4175,12 +3327,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D171" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-Sales-MettlerToledo</t>
         </is>
       </c>
     </row>
@@ -4197,12 +3344,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D172" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-Sales-OcadoWinTeam</t>
         </is>
       </c>
     </row>
@@ -4219,12 +3361,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA30</t>
         </is>
       </c>
     </row>
@@ -4241,12 +3378,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D174" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>IE-FileTransfer</t>
         </is>
       </c>
     </row>
@@ -4263,12 +3395,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegionAE</t>
         </is>
       </c>
     </row>
@@ -4285,12 +3412,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF30</t>
         </is>
       </c>
     </row>
@@ -4307,12 +3429,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-MettlerToledo</t>
         </is>
       </c>
     </row>
@@ -4329,12 +3446,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D178" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AirEquipSection</t>
         </is>
       </c>
     </row>
@@ -4351,12 +3463,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D179" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-PM-WorkingGroup-Vaccum</t>
         </is>
       </c>
     </row>
@@ -4373,12 +3480,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D180" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AirEquipSection</t>
         </is>
       </c>
     </row>
@@ -4395,12 +3497,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D181" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -4417,12 +3514,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D182" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -4439,12 +3531,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D183" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -4461,12 +3548,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D184" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegionAE</t>
         </is>
       </c>
     </row>
@@ -4483,12 +3565,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D185" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegionAE</t>
         </is>
       </c>
     </row>
@@ -4505,12 +3582,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D186" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegionAE</t>
         </is>
       </c>
     </row>
@@ -4527,12 +3599,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D187" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegionAE</t>
         </is>
       </c>
     </row>
@@ -4549,12 +3616,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D188" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegionAE</t>
         </is>
       </c>
     </row>
@@ -4571,12 +3633,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D189" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Operations</t>
         </is>
       </c>
     </row>
@@ -4593,12 +3650,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D190" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ECG-European-Chiller-Group</t>
         </is>
       </c>
     </row>
@@ -4615,12 +3667,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D191" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AirEquipSection</t>
         </is>
       </c>
     </row>
@@ -4637,12 +3684,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D192" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB40</t>
         </is>
       </c>
     </row>
@@ -4659,12 +3701,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D193" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-EMC-Safety</t>
         </is>
       </c>
     </row>
@@ -4681,12 +3718,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D194" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA30</t>
         </is>
       </c>
     </row>
@@ -4703,12 +3735,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D195" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF30</t>
         </is>
       </c>
     </row>
@@ -4725,12 +3752,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D196" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB10</t>
         </is>
       </c>
     </row>
@@ -4747,12 +3769,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D197" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB10</t>
         </is>
       </c>
     </row>
@@ -4769,12 +3786,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D198" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AB10</t>
         </is>
       </c>
     </row>
@@ -4791,12 +3803,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D199" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA10</t>
         </is>
       </c>
     </row>
@@ -4813,12 +3820,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D200" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA10</t>
         </is>
       </c>
     </row>
@@ -4835,12 +3837,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D201" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA10</t>
         </is>
       </c>
     </row>
@@ -4857,12 +3854,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D202" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF30</t>
         </is>
       </c>
     </row>
@@ -4879,12 +3871,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D203" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF30</t>
         </is>
       </c>
     </row>
@@ -4901,12 +3888,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D204" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF20</t>
         </is>
       </c>
     </row>
@@ -4923,12 +3905,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D205" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF20</t>
         </is>
       </c>
     </row>
@@ -4945,12 +3922,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D206" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF20</t>
         </is>
       </c>
     </row>
@@ -4967,12 +3939,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D207" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF20</t>
         </is>
       </c>
     </row>
@@ -4989,12 +3956,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D208" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-AF20</t>
         </is>
       </c>
     </row>
@@ -5011,12 +3973,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D209" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Logistics</t>
         </is>
       </c>
     </row>
@@ -5033,12 +3990,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D210" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Logistics</t>
         </is>
       </c>
     </row>
@@ -5055,12 +4007,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D211" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Logistics</t>
         </is>
       </c>
     </row>
@@ -5077,12 +4024,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D212" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Logistics</t>
         </is>
       </c>
     </row>
@@ -5099,12 +4041,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D213" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Logistics</t>
         </is>
       </c>
     </row>
@@ -5121,12 +4058,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D214" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-PM-WorkingGroup-Vaccum</t>
         </is>
       </c>
     </row>
@@ -5143,12 +4075,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D215" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AirEquipSection</t>
         </is>
       </c>
     </row>
@@ -5165,12 +4092,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D216" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AirEquipSection</t>
         </is>
       </c>
     </row>
@@ -5187,12 +4109,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D217" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AirEquipSection</t>
         </is>
       </c>
     </row>
@@ -5209,12 +4126,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D218" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AirEquipSection</t>
         </is>
       </c>
     </row>
@@ -5231,12 +4143,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D219" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AirEquipSection</t>
         </is>
       </c>
     </row>
@@ -5253,12 +4160,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D220" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>EU-ETC-AirEquipSection</t>
         </is>
       </c>
     </row>
@@ -5275,12 +4177,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D221" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA40</t>
         </is>
       </c>
     </row>
@@ -5297,12 +4194,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D222" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-AA40</t>
         </is>
       </c>
     </row>
@@ -5319,12 +4211,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D223" t="inlineStr">
-        <is>
-          <t>owner</t>
+          <t>GB-Facilities</t>
         </is>
       </c>
     </row>
@@ -5341,12 +4228,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D224" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Facilities</t>
         </is>
       </c>
     </row>
@@ -5363,12 +4245,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D225" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Facilities</t>
         </is>
       </c>
     </row>
@@ -5385,12 +4262,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D226" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Quality</t>
         </is>
       </c>
     </row>
@@ -5407,12 +4279,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D227" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>IE-FileTransfer</t>
         </is>
       </c>
     </row>
@@ -5429,12 +4296,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D228" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>IE-FileTransfer</t>
         </is>
       </c>
     </row>
@@ -5451,12 +4313,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D229" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-Indirect</t>
         </is>
       </c>
     </row>
@@ -5473,12 +4330,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D230" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-Sales-RegAF-Indirect</t>
         </is>
       </c>
     </row>
@@ -5495,12 +4347,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D231" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5517,12 +4364,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D232" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5539,12 +4381,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D233" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5561,12 +4398,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D234" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5583,12 +4415,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D235" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5605,12 +4432,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D236" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5627,12 +4449,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D237" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5649,12 +4466,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D238" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5671,12 +4483,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D239" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5693,12 +4500,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D240" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>
@@ -5715,12 +4517,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>member</t>
-        </is>
-      </c>
-      <c r="D241" t="inlineStr">
-        <is>
-          <t>member</t>
+          <t>GB-InsideSales</t>
         </is>
       </c>
     </row>

</xml_diff>